<commit_message>
Update chart, report, finaldoc documents
</commit_message>
<xml_diff>
--- a/Project/Gantt chart.xlsx
+++ b/Project/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stupc\Documents\GitHub\trip-clothing-planner\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40EEB70-A7E7-456B-BB29-CADBE73D3D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1D0CF0-ED12-4EA2-8464-2B02AECBBC72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="69">
   <si>
     <t>GANTT CHART SD2 - CHATBOT</t>
   </si>
@@ -197,9 +197,6 @@
     <t>Github Repository</t>
   </si>
   <si>
-    <t>Research</t>
-  </si>
-  <si>
     <t>Karen</t>
   </si>
   <si>
@@ -227,9 +224,6 @@
     <t>Entity mapping</t>
   </si>
   <si>
-    <t>Onboarding</t>
-  </si>
-  <si>
     <t>Group</t>
   </si>
   <si>
@@ -242,10 +236,58 @@
     <t>Project Performance / Monitoring</t>
   </si>
   <si>
-    <t>Project Final Documentation</t>
-  </si>
-  <si>
     <t xml:space="preserve">Prototype </t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report </t>
+  </si>
+  <si>
+    <t>Project Documentation</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>1.7</t>
+  </si>
+  <si>
+    <t>1.8</t>
+  </si>
+  <si>
+    <t>1.9</t>
+  </si>
+  <si>
+    <t>1.11</t>
+  </si>
+  <si>
+    <t>1.12</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>First research</t>
   </si>
 </sst>
 </file>
@@ -695,7 +737,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -871,15 +913,6 @@
     <xf numFmtId="9" fontId="24" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="24" fillId="17" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="24" fillId="17" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -890,14 +923,15 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -907,12 +941,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="15" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -933,16 +961,21 @@
     <xf numFmtId="0" fontId="16" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1261,10 +1294,10 @@
     <tabColor rgb="FF3D85C6"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BG51"/>
+  <dimension ref="A1:BG50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1283,38 +1316,38 @@
   <sheetData>
     <row r="1" spans="1:59" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="88" t="s">
+      <c r="B1" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="88"/>
-      <c r="O1" s="88"/>
-      <c r="P1" s="88"/>
-      <c r="Q1" s="88"/>
-      <c r="R1" s="88"/>
-      <c r="S1" s="88"/>
-      <c r="T1" s="88"/>
-      <c r="U1" s="88"/>
-      <c r="V1" s="88"/>
-      <c r="W1" s="88"/>
-      <c r="X1" s="88"/>
-      <c r="Y1" s="88"/>
-      <c r="Z1" s="88"/>
-      <c r="AA1" s="88"/>
-      <c r="AB1" s="88"/>
-      <c r="AC1" s="88"/>
-      <c r="AD1" s="88"/>
-      <c r="AE1" s="88"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="86"/>
+      <c r="O1" s="86"/>
+      <c r="P1" s="86"/>
+      <c r="Q1" s="86"/>
+      <c r="R1" s="86"/>
+      <c r="S1" s="86"/>
+      <c r="T1" s="86"/>
+      <c r="U1" s="86"/>
+      <c r="V1" s="86"/>
+      <c r="W1" s="86"/>
+      <c r="X1" s="86"/>
+      <c r="Y1" s="86"/>
+      <c r="Z1" s="86"/>
+      <c r="AA1" s="86"/>
+      <c r="AB1" s="86"/>
+      <c r="AC1" s="86"/>
+      <c r="AD1" s="86"/>
+      <c r="AE1" s="86"/>
       <c r="AF1" s="2"/>
       <c r="AG1" s="2"/>
       <c r="AH1" s="2"/>
@@ -1346,36 +1379,36 @@
     </row>
     <row r="2" spans="1:59" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="70"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="70"/>
-      <c r="V2" s="70"/>
-      <c r="W2" s="70"/>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="70"/>
-      <c r="Z2" s="70"/>
-      <c r="AA2" s="70"/>
-      <c r="AB2" s="70"/>
-      <c r="AC2" s="70"/>
-      <c r="AD2" s="70"/>
-      <c r="AE2" s="70"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="87"/>
+      <c r="M2" s="87"/>
+      <c r="N2" s="87"/>
+      <c r="O2" s="87"/>
+      <c r="P2" s="87"/>
+      <c r="Q2" s="87"/>
+      <c r="R2" s="87"/>
+      <c r="S2" s="87"/>
+      <c r="T2" s="87"/>
+      <c r="U2" s="87"/>
+      <c r="V2" s="87"/>
+      <c r="W2" s="87"/>
+      <c r="X2" s="87"/>
+      <c r="Y2" s="87"/>
+      <c r="Z2" s="87"/>
+      <c r="AA2" s="87"/>
+      <c r="AB2" s="87"/>
+      <c r="AC2" s="87"/>
+      <c r="AD2" s="87"/>
+      <c r="AE2" s="87"/>
       <c r="AF2" s="3"/>
       <c r="AG2" s="3"/>
       <c r="AH2" s="3"/>
@@ -1468,39 +1501,39 @@
     </row>
     <row r="4" spans="1:59" ht="21" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A4" s="1"/>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="73" t="s">
+      <c r="C4" s="70"/>
+      <c r="D4" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
       <c r="H4" s="9"/>
-      <c r="I4" s="89" t="s">
+      <c r="I4" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="90"/>
-      <c r="O4" s="90"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
+      <c r="L4" s="67"/>
+      <c r="M4" s="67"/>
+      <c r="N4" s="67"/>
+      <c r="O4" s="67"/>
       <c r="P4" s="11"/>
-      <c r="Q4" s="90"/>
-      <c r="R4" s="90"/>
-      <c r="S4" s="90"/>
-      <c r="T4" s="90"/>
-      <c r="U4" s="90"/>
-      <c r="V4" s="90"/>
-      <c r="W4" s="90"/>
-      <c r="X4" s="90"/>
-      <c r="Y4" s="90"/>
-      <c r="Z4" s="90"/>
-      <c r="AA4" s="90"/>
-      <c r="AB4" s="90"/>
+      <c r="Q4" s="67"/>
+      <c r="R4" s="67"/>
+      <c r="S4" s="67"/>
+      <c r="T4" s="67"/>
+      <c r="U4" s="67"/>
+      <c r="V4" s="67"/>
+      <c r="W4" s="67"/>
+      <c r="X4" s="67"/>
+      <c r="Y4" s="67"/>
+      <c r="Z4" s="67"/>
+      <c r="AA4" s="67"/>
+      <c r="AB4" s="67"/>
       <c r="AC4" s="10"/>
       <c r="AD4" s="2"/>
       <c r="AE4" s="2"/>
@@ -1535,38 +1568,38 @@
     </row>
     <row r="5" spans="1:59" ht="21" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A5" s="1"/>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="72"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
       <c r="H5" s="12"/>
-      <c r="I5" s="71" t="s">
+      <c r="I5" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
-      <c r="P5" s="74" t="s">
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
+      <c r="M5" s="70"/>
+      <c r="N5" s="70"/>
+      <c r="O5" s="70"/>
+      <c r="P5" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="Q5" s="72"/>
-      <c r="R5" s="72"/>
-      <c r="S5" s="72"/>
-      <c r="T5" s="72"/>
-      <c r="U5" s="72"/>
-      <c r="V5" s="72"/>
-      <c r="W5" s="72"/>
-      <c r="X5" s="72"/>
-      <c r="Y5" s="72"/>
-      <c r="Z5" s="72"/>
-      <c r="AA5" s="72"/>
+      <c r="Q5" s="70"/>
+      <c r="R5" s="70"/>
+      <c r="S5" s="70"/>
+      <c r="T5" s="70"/>
+      <c r="U5" s="70"/>
+      <c r="V5" s="70"/>
+      <c r="W5" s="70"/>
+      <c r="X5" s="70"/>
+      <c r="Y5" s="70"/>
+      <c r="Z5" s="70"/>
+      <c r="AA5" s="70"/>
       <c r="AB5" s="13"/>
       <c r="AC5" s="10"/>
       <c r="AD5" s="1"/>
@@ -1602,14 +1635,14 @@
     </row>
     <row r="6" spans="1:59" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
-      <c r="B6" s="87" t="s">
+      <c r="B6" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
       <c r="H6" s="15"/>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
@@ -1726,169 +1759,169 @@
     </row>
     <row r="8" spans="1:59" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="75" t="s">
+      <c r="C8" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="75" t="s">
+      <c r="D8" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="77" t="s">
+      <c r="E8" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="77" t="s">
+      <c r="F8" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="75" t="s">
+      <c r="G8" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="78" t="s">
+      <c r="I8" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="76"/>
-      <c r="K8" s="76"/>
-      <c r="L8" s="76"/>
-      <c r="M8" s="76"/>
-      <c r="N8" s="76"/>
-      <c r="O8" s="76"/>
-      <c r="P8" s="76"/>
-      <c r="Q8" s="76"/>
-      <c r="R8" s="76"/>
-      <c r="S8" s="76"/>
-      <c r="T8" s="76"/>
-      <c r="U8" s="76"/>
-      <c r="V8" s="76"/>
-      <c r="W8" s="76"/>
-      <c r="X8" s="79" t="s">
+      <c r="J8" s="74"/>
+      <c r="K8" s="74"/>
+      <c r="L8" s="74"/>
+      <c r="M8" s="74"/>
+      <c r="N8" s="74"/>
+      <c r="O8" s="74"/>
+      <c r="P8" s="74"/>
+      <c r="Q8" s="74"/>
+      <c r="R8" s="74"/>
+      <c r="S8" s="74"/>
+      <c r="T8" s="74"/>
+      <c r="U8" s="74"/>
+      <c r="V8" s="74"/>
+      <c r="W8" s="74"/>
+      <c r="X8" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="Y8" s="76"/>
-      <c r="Z8" s="76"/>
-      <c r="AA8" s="76"/>
-      <c r="AB8" s="76"/>
-      <c r="AC8" s="76"/>
-      <c r="AD8" s="76"/>
-      <c r="AE8" s="76"/>
-      <c r="AF8" s="76"/>
-      <c r="AG8" s="76"/>
-      <c r="AH8" s="76"/>
-      <c r="AI8" s="76"/>
-      <c r="AJ8" s="76"/>
-      <c r="AK8" s="76"/>
-      <c r="AL8" s="80" t="s">
+      <c r="Y8" s="74"/>
+      <c r="Z8" s="74"/>
+      <c r="AA8" s="74"/>
+      <c r="AB8" s="74"/>
+      <c r="AC8" s="74"/>
+      <c r="AD8" s="74"/>
+      <c r="AE8" s="74"/>
+      <c r="AF8" s="74"/>
+      <c r="AG8" s="74"/>
+      <c r="AH8" s="74"/>
+      <c r="AI8" s="74"/>
+      <c r="AJ8" s="74"/>
+      <c r="AK8" s="74"/>
+      <c r="AL8" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="AM8" s="76"/>
-      <c r="AN8" s="76"/>
-      <c r="AO8" s="76"/>
-      <c r="AP8" s="76"/>
-      <c r="AQ8" s="76"/>
-      <c r="AR8" s="76"/>
-      <c r="AS8" s="76"/>
-      <c r="AT8" s="76"/>
-      <c r="AU8" s="76"/>
-      <c r="AV8" s="76"/>
-      <c r="AW8" s="76"/>
-      <c r="AX8" s="76"/>
-      <c r="AY8" s="76"/>
-      <c r="AZ8" s="76"/>
-      <c r="BA8" s="76"/>
-      <c r="BB8" s="76"/>
-      <c r="BC8" s="76"/>
-      <c r="BD8" s="76"/>
-      <c r="BE8" s="76"/>
-      <c r="BF8" s="76"/>
+      <c r="AM8" s="74"/>
+      <c r="AN8" s="74"/>
+      <c r="AO8" s="74"/>
+      <c r="AP8" s="74"/>
+      <c r="AQ8" s="74"/>
+      <c r="AR8" s="74"/>
+      <c r="AS8" s="74"/>
+      <c r="AT8" s="74"/>
+      <c r="AU8" s="74"/>
+      <c r="AV8" s="74"/>
+      <c r="AW8" s="74"/>
+      <c r="AX8" s="74"/>
+      <c r="AY8" s="74"/>
+      <c r="AZ8" s="74"/>
+      <c r="BA8" s="74"/>
+      <c r="BB8" s="74"/>
+      <c r="BC8" s="74"/>
+      <c r="BD8" s="74"/>
+      <c r="BE8" s="74"/>
+      <c r="BF8" s="74"/>
       <c r="BG8" s="14"/>
     </row>
     <row r="9" spans="1:59" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
-      <c r="B9" s="76"/>
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="76"/>
-      <c r="F9" s="76"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="76"/>
-      <c r="I9" s="81" t="s">
+      <c r="B9" s="74"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="82"/>
-      <c r="K9" s="82"/>
-      <c r="L9" s="82"/>
-      <c r="M9" s="82"/>
-      <c r="N9" s="82"/>
-      <c r="O9" s="82"/>
-      <c r="P9" s="82"/>
-      <c r="Q9" s="81" t="s">
+      <c r="J9" s="78"/>
+      <c r="K9" s="78"/>
+      <c r="L9" s="78"/>
+      <c r="M9" s="78"/>
+      <c r="N9" s="78"/>
+      <c r="O9" s="78"/>
+      <c r="P9" s="78"/>
+      <c r="Q9" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="R9" s="82"/>
-      <c r="S9" s="82"/>
-      <c r="T9" s="82"/>
-      <c r="U9" s="82"/>
-      <c r="V9" s="82"/>
-      <c r="W9" s="83"/>
-      <c r="X9" s="84" t="s">
+      <c r="R9" s="78"/>
+      <c r="S9" s="78"/>
+      <c r="T9" s="78"/>
+      <c r="U9" s="78"/>
+      <c r="V9" s="78"/>
+      <c r="W9" s="79"/>
+      <c r="X9" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="Y9" s="82"/>
-      <c r="Z9" s="82"/>
-      <c r="AA9" s="82"/>
-      <c r="AB9" s="82"/>
-      <c r="AC9" s="82"/>
-      <c r="AD9" s="83"/>
-      <c r="AE9" s="85" t="s">
+      <c r="Y9" s="78"/>
+      <c r="Z9" s="78"/>
+      <c r="AA9" s="78"/>
+      <c r="AB9" s="78"/>
+      <c r="AC9" s="78"/>
+      <c r="AD9" s="79"/>
+      <c r="AE9" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="AF9" s="82"/>
-      <c r="AG9" s="82"/>
-      <c r="AH9" s="82"/>
-      <c r="AI9" s="82"/>
-      <c r="AJ9" s="82"/>
-      <c r="AK9" s="83"/>
-      <c r="AL9" s="86" t="s">
+      <c r="AF9" s="78"/>
+      <c r="AG9" s="78"/>
+      <c r="AH9" s="78"/>
+      <c r="AI9" s="78"/>
+      <c r="AJ9" s="78"/>
+      <c r="AK9" s="79"/>
+      <c r="AL9" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="AM9" s="82"/>
-      <c r="AN9" s="82"/>
-      <c r="AO9" s="82"/>
-      <c r="AP9" s="82"/>
-      <c r="AQ9" s="82"/>
-      <c r="AR9" s="83"/>
-      <c r="AS9" s="86" t="s">
+      <c r="AM9" s="78"/>
+      <c r="AN9" s="78"/>
+      <c r="AO9" s="78"/>
+      <c r="AP9" s="78"/>
+      <c r="AQ9" s="78"/>
+      <c r="AR9" s="79"/>
+      <c r="AS9" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="AT9" s="82"/>
-      <c r="AU9" s="82"/>
-      <c r="AV9" s="82"/>
-      <c r="AW9" s="82"/>
-      <c r="AX9" s="82"/>
-      <c r="AY9" s="82"/>
-      <c r="AZ9" s="86" t="s">
+      <c r="AT9" s="78"/>
+      <c r="AU9" s="78"/>
+      <c r="AV9" s="78"/>
+      <c r="AW9" s="78"/>
+      <c r="AX9" s="78"/>
+      <c r="AY9" s="78"/>
+      <c r="AZ9" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="BA9" s="82"/>
-      <c r="BB9" s="82"/>
-      <c r="BC9" s="82"/>
-      <c r="BD9" s="82"/>
-      <c r="BE9" s="82"/>
-      <c r="BF9" s="83"/>
+      <c r="BA9" s="78"/>
+      <c r="BB9" s="78"/>
+      <c r="BC9" s="78"/>
+      <c r="BD9" s="78"/>
+      <c r="BE9" s="78"/>
+      <c r="BF9" s="79"/>
       <c r="BG9" s="19"/>
     </row>
     <row r="10" spans="1:59" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
-      <c r="B10" s="76"/>
-      <c r="C10" s="76"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="76"/>
-      <c r="G10" s="76"/>
-      <c r="H10" s="76"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
       <c r="I10" s="21" t="s">
         <v>25</v>
       </c>
@@ -2043,13 +2076,13 @@
     </row>
     <row r="11" spans="1:59" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
-      <c r="B11" s="76"/>
-      <c r="C11" s="76"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="76"/>
-      <c r="H11" s="76"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="74"/>
       <c r="I11" s="21">
         <v>9</v>
       </c>
@@ -2269,8 +2302,8 @@
     </row>
     <row r="13" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="35"/>
-      <c r="B13" s="36">
-        <v>1.1000000000000001</v>
+      <c r="B13" s="36" t="s">
+        <v>67</v>
       </c>
       <c r="C13" s="37" t="s">
         <v>31</v>
@@ -2344,8 +2377,8 @@
     </row>
     <row r="14" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="35"/>
-      <c r="B14" s="36">
-        <v>1.2</v>
+      <c r="B14" s="36" t="s">
+        <v>55</v>
       </c>
       <c r="C14" s="37" t="s">
         <v>33</v>
@@ -2419,8 +2452,8 @@
     </row>
     <row r="15" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35"/>
-      <c r="B15" s="36">
-        <v>1.3</v>
+      <c r="B15" s="36" t="s">
+        <v>56</v>
       </c>
       <c r="C15" s="37" t="s">
         <v>34</v>
@@ -2494,8 +2527,8 @@
     </row>
     <row r="16" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="35"/>
-      <c r="B16" s="36">
-        <v>1.4</v>
+      <c r="B16" s="36" t="s">
+        <v>57</v>
       </c>
       <c r="C16" s="37" t="s">
         <v>35</v>
@@ -2569,8 +2602,8 @@
     </row>
     <row r="17" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="35"/>
-      <c r="B17" s="36">
-        <v>1.5</v>
+      <c r="B17" s="36" t="s">
+        <v>58</v>
       </c>
       <c r="C17" s="37" t="s">
         <v>37</v>
@@ -2644,14 +2677,14 @@
     </row>
     <row r="18" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="35"/>
-      <c r="B18" s="36">
-        <v>1.6</v>
+      <c r="B18" s="36" t="s">
+        <v>59</v>
       </c>
       <c r="C18" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="37" t="s">
         <v>38</v>
-      </c>
-      <c r="D18" s="37" t="s">
-        <v>39</v>
       </c>
       <c r="E18" s="38">
         <v>45719</v>
@@ -2663,11 +2696,11 @@
         <v>3</v>
       </c>
       <c r="H18" s="40">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I18" s="41"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="42"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="41"/>
       <c r="L18" s="46"/>
       <c r="M18" s="46"/>
       <c r="N18" s="46"/>
@@ -2719,14 +2752,14 @@
     </row>
     <row r="19" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="35"/>
-      <c r="B19" s="36">
-        <v>1.7</v>
+      <c r="B19" s="36" t="s">
+        <v>60</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E19" s="38">
         <v>45719</v>
@@ -2738,7 +2771,7 @@
         <v>3</v>
       </c>
       <c r="H19" s="40">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="I19" s="41"/>
       <c r="J19" s="46"/>
@@ -2749,8 +2782,8 @@
       <c r="O19" s="46"/>
       <c r="P19" s="46"/>
       <c r="Q19" s="46"/>
-      <c r="R19" s="42"/>
-      <c r="S19" s="42"/>
+      <c r="R19" s="41"/>
+      <c r="S19" s="41"/>
       <c r="T19" s="46"/>
       <c r="U19" s="46"/>
       <c r="V19" s="46"/>
@@ -2794,11 +2827,11 @@
     </row>
     <row r="20" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" s="35"/>
-      <c r="B20" s="36">
-        <v>1.8</v>
+      <c r="B20" s="36" t="s">
+        <v>61</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D20" s="37" t="s">
         <v>36</v>
@@ -2870,10 +2903,10 @@
     <row r="21" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="35"/>
       <c r="B21" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="37" t="s">
         <v>41</v>
-      </c>
-      <c r="C21" s="37" t="s">
-        <v>42</v>
       </c>
       <c r="D21" s="37" t="s">
         <v>32</v>
@@ -2945,13 +2978,13 @@
     <row r="22" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" s="35"/>
       <c r="B22" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="37" t="s">
-        <v>42</v>
-      </c>
       <c r="D22" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E22" s="38">
         <v>45726</v>
@@ -2963,7 +2996,7 @@
         <v>3</v>
       </c>
       <c r="H22" s="40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="50"/>
       <c r="J22" s="51"/>
@@ -2973,9 +3006,9 @@
       <c r="N22" s="51"/>
       <c r="O22" s="51"/>
       <c r="P22" s="51"/>
-      <c r="Q22" s="42"/>
-      <c r="R22" s="42"/>
-      <c r="S22" s="42"/>
+      <c r="Q22" s="41"/>
+      <c r="R22" s="41"/>
+      <c r="S22" s="41"/>
       <c r="T22" s="51"/>
       <c r="U22" s="51"/>
       <c r="V22" s="51"/>
@@ -3020,10 +3053,10 @@
     <row r="23" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="35"/>
       <c r="B23" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="37" t="s">
         <v>41</v>
-      </c>
-      <c r="C23" s="37" t="s">
-        <v>42</v>
       </c>
       <c r="D23" s="37" t="s">
         <v>36</v>
@@ -3038,7 +3071,7 @@
         <v>3</v>
       </c>
       <c r="H23" s="40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" s="50"/>
       <c r="J23" s="51"/>
@@ -3048,9 +3081,9 @@
       <c r="N23" s="51"/>
       <c r="O23" s="51"/>
       <c r="P23" s="51"/>
-      <c r="Q23" s="42"/>
-      <c r="R23" s="42"/>
-      <c r="S23" s="42"/>
+      <c r="Q23" s="41"/>
+      <c r="R23" s="41"/>
+      <c r="S23" s="41"/>
       <c r="T23" s="51"/>
       <c r="U23" s="51"/>
       <c r="V23" s="51"/>
@@ -3095,27 +3128,27 @@
     <row r="24" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="35"/>
       <c r="B24" s="36" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="C24" s="37" t="s">
         <v>43</v>
       </c>
       <c r="D24" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="F24" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="G24" s="39" t="s">
-        <v>43</v>
+        <v>32</v>
+      </c>
+      <c r="E24" s="38">
+        <v>45732</v>
+      </c>
+      <c r="F24" s="38">
+        <v>45739</v>
+      </c>
+      <c r="G24" s="39">
+        <v>1</v>
       </c>
       <c r="H24" s="40">
-        <v>0</v>
-      </c>
-      <c r="I24" s="50"/>
+        <v>1</v>
+      </c>
+      <c r="I24" s="41"/>
       <c r="J24" s="51"/>
       <c r="K24" s="51"/>
       <c r="L24" s="51"/>
@@ -3169,14 +3202,14 @@
     </row>
     <row r="25" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="35"/>
-      <c r="B25" s="36">
-        <v>1.9</v>
+      <c r="B25" s="36" t="s">
+        <v>63</v>
       </c>
       <c r="C25" s="37" t="s">
         <v>44</v>
       </c>
       <c r="D25" s="37" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E25" s="38">
         <v>45732</v>
@@ -3185,14 +3218,14 @@
         <v>45739</v>
       </c>
       <c r="G25" s="39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H25" s="40">
-        <v>1</v>
-      </c>
-      <c r="I25" s="41"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="51"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="50"/>
+      <c r="J25" s="41"/>
+      <c r="K25" s="41"/>
       <c r="L25" s="51"/>
       <c r="M25" s="51"/>
       <c r="N25" s="51"/>
@@ -3244,14 +3277,14 @@
     </row>
     <row r="26" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="35"/>
-      <c r="B26" s="36">
-        <v>1.1100000000000001</v>
+      <c r="B26" s="36" t="s">
+        <v>63</v>
       </c>
       <c r="C26" s="37" t="s">
         <v>45</v>
       </c>
       <c r="D26" s="37" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E26" s="38">
         <v>45732</v>
@@ -3260,13 +3293,13 @@
         <v>45739</v>
       </c>
       <c r="G26" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H26" s="40">
         <v>0</v>
       </c>
       <c r="I26" s="50"/>
-      <c r="J26" s="42"/>
+      <c r="J26" s="51"/>
       <c r="K26" s="42"/>
       <c r="L26" s="51"/>
       <c r="M26" s="51"/>
@@ -3319,8 +3352,8 @@
     </row>
     <row r="27" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="35"/>
-      <c r="B27" s="36">
-        <v>1.1100000000000001</v>
+      <c r="B27" s="36" t="s">
+        <v>64</v>
       </c>
       <c r="C27" s="37" t="s">
         <v>46</v>
@@ -3394,14 +3427,14 @@
     </row>
     <row r="28" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="35"/>
-      <c r="B28" s="36">
-        <v>1.1200000000000001</v>
+      <c r="B28" s="36" t="s">
+        <v>64</v>
       </c>
       <c r="C28" s="37" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D28" s="37" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E28" s="38">
         <v>45732</v>
@@ -3410,26 +3443,26 @@
         <v>45739</v>
       </c>
       <c r="G28" s="39">
+        <v>8</v>
+      </c>
+      <c r="H28" s="40">
         <v>1</v>
-      </c>
-      <c r="H28" s="40">
-        <v>0</v>
       </c>
       <c r="I28" s="50"/>
       <c r="J28" s="51"/>
-      <c r="K28" s="42"/>
+      <c r="K28" s="51"/>
       <c r="L28" s="51"/>
       <c r="M28" s="51"/>
       <c r="N28" s="51"/>
       <c r="O28" s="51"/>
-      <c r="P28" s="51"/>
-      <c r="Q28" s="51"/>
-      <c r="R28" s="51"/>
-      <c r="S28" s="51"/>
-      <c r="T28" s="51"/>
-      <c r="U28" s="51"/>
-      <c r="V28" s="51"/>
-      <c r="W28" s="51"/>
+      <c r="P28" s="41"/>
+      <c r="Q28" s="41"/>
+      <c r="R28" s="41"/>
+      <c r="S28" s="41"/>
+      <c r="T28" s="41"/>
+      <c r="U28" s="41"/>
+      <c r="V28" s="41"/>
+      <c r="W28" s="41"/>
       <c r="X28" s="51"/>
       <c r="Y28" s="51"/>
       <c r="Z28" s="51"/>
@@ -3469,14 +3502,14 @@
     </row>
     <row r="29" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="35"/>
-      <c r="B29" s="36">
-        <v>1.1200000000000001</v>
+      <c r="B29" s="36" t="s">
+        <v>42</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D29" s="37" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="E29" s="38">
         <v>45732</v>
@@ -3485,26 +3518,26 @@
         <v>45739</v>
       </c>
       <c r="G29" s="39">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H29" s="40">
         <v>0</v>
       </c>
       <c r="I29" s="50"/>
       <c r="J29" s="51"/>
-      <c r="K29" s="42"/>
+      <c r="K29" s="51"/>
       <c r="L29" s="51"/>
       <c r="M29" s="51"/>
       <c r="N29" s="51"/>
       <c r="O29" s="51"/>
-      <c r="P29" s="51"/>
-      <c r="Q29" s="51"/>
-      <c r="R29" s="51"/>
-      <c r="S29" s="51"/>
-      <c r="T29" s="51"/>
-      <c r="U29" s="51"/>
-      <c r="V29" s="51"/>
-      <c r="W29" s="51"/>
+      <c r="P29" s="42"/>
+      <c r="Q29" s="42"/>
+      <c r="R29" s="42"/>
+      <c r="S29" s="42"/>
+      <c r="T29" s="42"/>
+      <c r="U29" s="42"/>
+      <c r="V29" s="42"/>
+      <c r="W29" s="42"/>
       <c r="X29" s="51"/>
       <c r="Y29" s="51"/>
       <c r="Z29" s="51"/>
@@ -3544,29 +3577,29 @@
     </row>
     <row r="30" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="35"/>
-      <c r="B30" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="E30" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="F30" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="G30" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="H30" s="40">
+      <c r="B30" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="F30" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="G30" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="H30" s="56">
         <v>0</v>
       </c>
-      <c r="I30" s="50"/>
-      <c r="J30" s="51"/>
+      <c r="I30" s="57"/>
+      <c r="J30" s="58"/>
       <c r="K30" s="51"/>
       <c r="L30" s="51"/>
       <c r="M30" s="51"/>
@@ -3617,174 +3650,168 @@
       <c r="BF30" s="52"/>
       <c r="BG30" s="35"/>
     </row>
-    <row r="31" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="35"/>
-      <c r="B31" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="D31" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="E31" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="F31" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="G31" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="H31" s="56">
+    <row r="31" spans="1:59" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="B31" s="28">
+        <v>2</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="30"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="34"/>
+      <c r="L31" s="34"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="32"/>
+      <c r="O31" s="32"/>
+      <c r="P31" s="32"/>
+      <c r="Q31" s="32"/>
+      <c r="R31" s="32"/>
+      <c r="S31" s="32"/>
+      <c r="T31" s="32"/>
+      <c r="U31" s="32"/>
+      <c r="V31" s="32"/>
+      <c r="W31" s="32"/>
+      <c r="X31" s="32"/>
+      <c r="Y31" s="32"/>
+      <c r="Z31" s="32"/>
+      <c r="AA31" s="32"/>
+      <c r="AB31" s="32"/>
+      <c r="AC31" s="32"/>
+      <c r="AD31" s="32"/>
+      <c r="AE31" s="32"/>
+      <c r="AF31" s="32"/>
+      <c r="AG31" s="32"/>
+      <c r="AH31" s="32"/>
+      <c r="AI31" s="32"/>
+      <c r="AJ31" s="32"/>
+      <c r="AK31" s="32"/>
+      <c r="AL31" s="32"/>
+      <c r="AM31" s="32"/>
+      <c r="AN31" s="32"/>
+      <c r="AO31" s="32"/>
+      <c r="AP31" s="32"/>
+      <c r="AQ31" s="32"/>
+      <c r="AR31" s="32"/>
+      <c r="AS31" s="32"/>
+      <c r="AT31" s="32"/>
+      <c r="AU31" s="32"/>
+      <c r="AV31" s="32"/>
+      <c r="AW31" s="32"/>
+      <c r="AX31" s="32"/>
+      <c r="AY31" s="32"/>
+      <c r="AZ31" s="32"/>
+      <c r="BA31" s="32"/>
+      <c r="BB31" s="32"/>
+      <c r="BC31" s="32"/>
+      <c r="BD31" s="32"/>
+      <c r="BE31" s="32"/>
+      <c r="BF31" s="32"/>
+      <c r="BG31" s="14"/>
+    </row>
+    <row r="32" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="35"/>
+      <c r="B32" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="F32" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="G32" s="39">
         <v>0</v>
       </c>
-      <c r="I31" s="57"/>
-      <c r="J31" s="58"/>
-      <c r="K31" s="51"/>
-      <c r="L31" s="51"/>
-      <c r="M31" s="51"/>
-      <c r="N31" s="51"/>
-      <c r="O31" s="51"/>
-      <c r="P31" s="51"/>
-      <c r="Q31" s="51"/>
-      <c r="R31" s="51"/>
-      <c r="S31" s="51"/>
-      <c r="T31" s="51"/>
-      <c r="U31" s="51"/>
-      <c r="V31" s="51"/>
-      <c r="W31" s="51"/>
-      <c r="X31" s="51"/>
-      <c r="Y31" s="51"/>
-      <c r="Z31" s="51"/>
-      <c r="AA31" s="51"/>
-      <c r="AB31" s="51"/>
-      <c r="AC31" s="52"/>
-      <c r="AD31" s="52"/>
-      <c r="AE31" s="52"/>
-      <c r="AF31" s="52"/>
-      <c r="AG31" s="52"/>
-      <c r="AH31" s="52"/>
-      <c r="AI31" s="52"/>
-      <c r="AJ31" s="52"/>
-      <c r="AK31" s="52"/>
-      <c r="AL31" s="51"/>
-      <c r="AM31" s="51"/>
-      <c r="AN31" s="51"/>
-      <c r="AO31" s="51"/>
-      <c r="AP31" s="51"/>
-      <c r="AQ31" s="51"/>
-      <c r="AR31" s="51"/>
-      <c r="AS31" s="51"/>
-      <c r="AT31" s="51"/>
-      <c r="AU31" s="51"/>
-      <c r="AV31" s="51"/>
-      <c r="AW31" s="51"/>
-      <c r="AX31" s="51"/>
-      <c r="AY31" s="51"/>
-      <c r="AZ31" s="51"/>
-      <c r="BA31" s="52"/>
-      <c r="BB31" s="52"/>
-      <c r="BC31" s="52"/>
-      <c r="BD31" s="52"/>
-      <c r="BE31" s="52"/>
-      <c r="BF31" s="52"/>
-      <c r="BG31" s="35"/>
-    </row>
-    <row r="32" spans="1:59" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
-      <c r="B32" s="28">
-        <v>2</v>
-      </c>
-      <c r="C32" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32" s="30"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="32"/>
-      <c r="J32" s="33"/>
-      <c r="K32" s="34"/>
-      <c r="L32" s="34"/>
-      <c r="M32" s="32"/>
-      <c r="N32" s="32"/>
-      <c r="O32" s="32"/>
-      <c r="P32" s="32"/>
-      <c r="Q32" s="32"/>
-      <c r="R32" s="32"/>
-      <c r="S32" s="32"/>
-      <c r="T32" s="32"/>
-      <c r="U32" s="32"/>
-      <c r="V32" s="32"/>
-      <c r="W32" s="32"/>
-      <c r="X32" s="32"/>
-      <c r="Y32" s="32"/>
-      <c r="Z32" s="32"/>
-      <c r="AA32" s="32"/>
-      <c r="AB32" s="32"/>
-      <c r="AC32" s="32"/>
-      <c r="AD32" s="32"/>
-      <c r="AE32" s="32"/>
-      <c r="AF32" s="32"/>
-      <c r="AG32" s="32"/>
-      <c r="AH32" s="32"/>
-      <c r="AI32" s="32"/>
-      <c r="AJ32" s="32"/>
-      <c r="AK32" s="32"/>
-      <c r="AL32" s="32"/>
-      <c r="AM32" s="32"/>
-      <c r="AN32" s="32"/>
-      <c r="AO32" s="32"/>
-      <c r="AP32" s="32"/>
-      <c r="AQ32" s="32"/>
-      <c r="AR32" s="32"/>
-      <c r="AS32" s="32"/>
-      <c r="AT32" s="32"/>
-      <c r="AU32" s="32"/>
-      <c r="AV32" s="32"/>
-      <c r="AW32" s="32"/>
-      <c r="AX32" s="32"/>
-      <c r="AY32" s="32"/>
-      <c r="AZ32" s="32"/>
-      <c r="BA32" s="32"/>
-      <c r="BB32" s="32"/>
-      <c r="BC32" s="32"/>
-      <c r="BD32" s="32"/>
-      <c r="BE32" s="32"/>
-      <c r="BF32" s="32"/>
-      <c r="BG32" s="14"/>
+      <c r="H32" s="40">
+        <v>0</v>
+      </c>
+      <c r="I32" s="50"/>
+      <c r="J32" s="59"/>
+      <c r="K32" s="43"/>
+      <c r="L32" s="43"/>
+      <c r="M32" s="43"/>
+      <c r="N32" s="46"/>
+      <c r="O32" s="46"/>
+      <c r="P32" s="46"/>
+      <c r="Q32" s="46"/>
+      <c r="R32" s="46"/>
+      <c r="S32" s="46"/>
+      <c r="T32" s="46"/>
+      <c r="U32" s="46"/>
+      <c r="V32" s="46"/>
+      <c r="W32" s="46"/>
+      <c r="X32" s="60"/>
+      <c r="Y32" s="60"/>
+      <c r="Z32" s="60"/>
+      <c r="AA32" s="60"/>
+      <c r="AB32" s="60"/>
+      <c r="AC32" s="61"/>
+      <c r="AD32" s="61"/>
+      <c r="AE32" s="47"/>
+      <c r="AF32" s="47"/>
+      <c r="AG32" s="47"/>
+      <c r="AH32" s="47"/>
+      <c r="AI32" s="47"/>
+      <c r="AJ32" s="47"/>
+      <c r="AK32" s="47"/>
+      <c r="AL32" s="46"/>
+      <c r="AM32" s="46"/>
+      <c r="AN32" s="46"/>
+      <c r="AO32" s="46"/>
+      <c r="AP32" s="46"/>
+      <c r="AQ32" s="46"/>
+      <c r="AR32" s="46"/>
+      <c r="AS32" s="46"/>
+      <c r="AT32" s="46"/>
+      <c r="AU32" s="46"/>
+      <c r="AV32" s="46"/>
+      <c r="AW32" s="46"/>
+      <c r="AX32" s="46"/>
+      <c r="AY32" s="46"/>
+      <c r="AZ32" s="46"/>
+      <c r="BA32" s="47"/>
+      <c r="BB32" s="47"/>
+      <c r="BC32" s="47"/>
+      <c r="BD32" s="47"/>
+      <c r="BE32" s="47"/>
+      <c r="BF32" s="47"/>
+      <c r="BG32" s="35"/>
     </row>
     <row r="33" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="35"/>
-      <c r="B33" s="36">
-        <v>2.1</v>
-      </c>
+      <c r="B33" s="36"/>
       <c r="C33" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D33" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="E33" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="F33" s="38" t="s">
-        <v>43</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
       <c r="G33" s="39">
         <v>0</v>
       </c>
       <c r="H33" s="40">
         <v>0</v>
       </c>
-      <c r="I33" s="50"/>
-      <c r="J33" s="59"/>
-      <c r="K33" s="43"/>
-      <c r="L33" s="43"/>
-      <c r="M33" s="43"/>
+      <c r="I33" s="62"/>
+      <c r="J33" s="45"/>
+      <c r="K33" s="46"/>
+      <c r="L33" s="46"/>
+      <c r="M33" s="46"/>
       <c r="N33" s="46"/>
       <c r="O33" s="46"/>
       <c r="P33" s="46"/>
@@ -3795,13 +3822,13 @@
       <c r="U33" s="46"/>
       <c r="V33" s="46"/>
       <c r="W33" s="46"/>
-      <c r="X33" s="60"/>
-      <c r="Y33" s="60"/>
-      <c r="Z33" s="60"/>
-      <c r="AA33" s="60"/>
-      <c r="AB33" s="60"/>
-      <c r="AC33" s="61"/>
-      <c r="AD33" s="61"/>
+      <c r="X33" s="46"/>
+      <c r="Y33" s="46"/>
+      <c r="Z33" s="46"/>
+      <c r="AA33" s="46"/>
+      <c r="AB33" s="46"/>
+      <c r="AC33" s="47"/>
+      <c r="AD33" s="47"/>
       <c r="AE33" s="47"/>
       <c r="AF33" s="47"/>
       <c r="AG33" s="47"/>
@@ -3836,10 +3863,10 @@
       <c r="A34" s="35"/>
       <c r="B34" s="36"/>
       <c r="C34" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D34" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E34" s="38"/>
       <c r="F34" s="38"/>
@@ -3905,17 +3932,17 @@
       <c r="A35" s="35"/>
       <c r="B35" s="36"/>
       <c r="C35" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D35" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E35" s="38"/>
       <c r="F35" s="38"/>
       <c r="G35" s="39">
         <v>0</v>
       </c>
-      <c r="H35" s="40">
+      <c r="H35" s="49">
         <v>0</v>
       </c>
       <c r="I35" s="62"/>
@@ -3970,148 +3997,148 @@
       <c r="BF35" s="47"/>
       <c r="BG35" s="35"/>
     </row>
-    <row r="36" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="35"/>
-      <c r="B36" s="36"/>
-      <c r="C36" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="D36" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="E36" s="38"/>
-      <c r="F36" s="38"/>
-      <c r="G36" s="39">
+    <row r="36" spans="1:59" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="28">
+        <v>3</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" s="30"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="32"/>
+      <c r="J36" s="33"/>
+      <c r="K36" s="34"/>
+      <c r="L36" s="34"/>
+      <c r="M36" s="32"/>
+      <c r="N36" s="32"/>
+      <c r="O36" s="32"/>
+      <c r="P36" s="32"/>
+      <c r="Q36" s="32"/>
+      <c r="R36" s="32"/>
+      <c r="S36" s="32"/>
+      <c r="T36" s="32"/>
+      <c r="U36" s="32"/>
+      <c r="V36" s="32"/>
+      <c r="W36" s="32"/>
+      <c r="X36" s="32"/>
+      <c r="Y36" s="32"/>
+      <c r="Z36" s="32"/>
+      <c r="AA36" s="32"/>
+      <c r="AB36" s="32"/>
+      <c r="AC36" s="32"/>
+      <c r="AD36" s="32"/>
+      <c r="AE36" s="32"/>
+      <c r="AF36" s="32"/>
+      <c r="AG36" s="32"/>
+      <c r="AH36" s="32"/>
+      <c r="AI36" s="32"/>
+      <c r="AJ36" s="32"/>
+      <c r="AK36" s="32"/>
+      <c r="AL36" s="32"/>
+      <c r="AM36" s="32"/>
+      <c r="AN36" s="32"/>
+      <c r="AO36" s="32"/>
+      <c r="AP36" s="32"/>
+      <c r="AQ36" s="32"/>
+      <c r="AR36" s="32"/>
+      <c r="AS36" s="32"/>
+      <c r="AT36" s="32"/>
+      <c r="AU36" s="32"/>
+      <c r="AV36" s="32"/>
+      <c r="AW36" s="32"/>
+      <c r="AX36" s="32"/>
+      <c r="AY36" s="32"/>
+      <c r="AZ36" s="32"/>
+      <c r="BA36" s="32"/>
+      <c r="BB36" s="32"/>
+      <c r="BC36" s="32"/>
+      <c r="BD36" s="32"/>
+      <c r="BE36" s="32"/>
+      <c r="BF36" s="32"/>
+      <c r="BG36" s="14"/>
+    </row>
+    <row r="37" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="35"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="39">
         <v>0</v>
       </c>
-      <c r="H36" s="49">
+      <c r="H37" s="40">
         <v>0</v>
       </c>
-      <c r="I36" s="62"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="46"/>
-      <c r="L36" s="46"/>
-      <c r="M36" s="46"/>
-      <c r="N36" s="46"/>
-      <c r="O36" s="46"/>
-      <c r="P36" s="46"/>
-      <c r="Q36" s="46"/>
-      <c r="R36" s="46"/>
-      <c r="S36" s="46"/>
-      <c r="T36" s="46"/>
-      <c r="U36" s="46"/>
-      <c r="V36" s="46"/>
-      <c r="W36" s="46"/>
-      <c r="X36" s="46"/>
-      <c r="Y36" s="46"/>
-      <c r="Z36" s="46"/>
-      <c r="AA36" s="46"/>
-      <c r="AB36" s="46"/>
-      <c r="AC36" s="47"/>
-      <c r="AD36" s="47"/>
-      <c r="AE36" s="47"/>
-      <c r="AF36" s="47"/>
-      <c r="AG36" s="47"/>
-      <c r="AH36" s="47"/>
-      <c r="AI36" s="47"/>
-      <c r="AJ36" s="47"/>
-      <c r="AK36" s="47"/>
-      <c r="AL36" s="46"/>
-      <c r="AM36" s="46"/>
-      <c r="AN36" s="46"/>
-      <c r="AO36" s="46"/>
-      <c r="AP36" s="46"/>
-      <c r="AQ36" s="46"/>
-      <c r="AR36" s="46"/>
-      <c r="AS36" s="46"/>
-      <c r="AT36" s="46"/>
-      <c r="AU36" s="46"/>
-      <c r="AV36" s="46"/>
-      <c r="AW36" s="46"/>
-      <c r="AX36" s="46"/>
-      <c r="AY36" s="46"/>
-      <c r="AZ36" s="46"/>
-      <c r="BA36" s="47"/>
-      <c r="BB36" s="47"/>
-      <c r="BC36" s="47"/>
-      <c r="BD36" s="47"/>
-      <c r="BE36" s="47"/>
-      <c r="BF36" s="47"/>
-      <c r="BG36" s="35"/>
-    </row>
-    <row r="37" spans="1:59" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="28">
-        <v>3</v>
-      </c>
-      <c r="C37" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="D37" s="30"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="33"/>
-      <c r="K37" s="34"/>
-      <c r="L37" s="34"/>
-      <c r="M37" s="32"/>
-      <c r="N37" s="32"/>
-      <c r="O37" s="32"/>
-      <c r="P37" s="32"/>
-      <c r="Q37" s="32"/>
-      <c r="R37" s="32"/>
-      <c r="S37" s="32"/>
-      <c r="T37" s="32"/>
-      <c r="U37" s="32"/>
-      <c r="V37" s="32"/>
-      <c r="W37" s="32"/>
-      <c r="X37" s="32"/>
-      <c r="Y37" s="32"/>
-      <c r="Z37" s="32"/>
-      <c r="AA37" s="32"/>
-      <c r="AB37" s="32"/>
-      <c r="AC37" s="32"/>
-      <c r="AD37" s="32"/>
-      <c r="AE37" s="32"/>
-      <c r="AF37" s="32"/>
-      <c r="AG37" s="32"/>
-      <c r="AH37" s="32"/>
-      <c r="AI37" s="32"/>
-      <c r="AJ37" s="32"/>
-      <c r="AK37" s="32"/>
-      <c r="AL37" s="32"/>
-      <c r="AM37" s="32"/>
-      <c r="AN37" s="32"/>
-      <c r="AO37" s="32"/>
-      <c r="AP37" s="32"/>
-      <c r="AQ37" s="32"/>
-      <c r="AR37" s="32"/>
-      <c r="AS37" s="32"/>
-      <c r="AT37" s="32"/>
-      <c r="AU37" s="32"/>
-      <c r="AV37" s="32"/>
-      <c r="AW37" s="32"/>
-      <c r="AX37" s="32"/>
-      <c r="AY37" s="32"/>
-      <c r="AZ37" s="32"/>
-      <c r="BA37" s="32"/>
-      <c r="BB37" s="32"/>
-      <c r="BC37" s="32"/>
-      <c r="BD37" s="32"/>
-      <c r="BE37" s="32"/>
-      <c r="BF37" s="32"/>
-      <c r="BG37" s="14"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="59"/>
+      <c r="K37" s="43"/>
+      <c r="L37" s="43"/>
+      <c r="M37" s="43"/>
+      <c r="N37" s="46"/>
+      <c r="O37" s="46"/>
+      <c r="P37" s="46"/>
+      <c r="Q37" s="46"/>
+      <c r="R37" s="46"/>
+      <c r="S37" s="46"/>
+      <c r="T37" s="46"/>
+      <c r="U37" s="46"/>
+      <c r="V37" s="46"/>
+      <c r="W37" s="46"/>
+      <c r="X37" s="46"/>
+      <c r="Y37" s="46"/>
+      <c r="Z37" s="46"/>
+      <c r="AA37" s="46"/>
+      <c r="AB37" s="46"/>
+      <c r="AC37" s="47"/>
+      <c r="AD37" s="47"/>
+      <c r="AE37" s="47"/>
+      <c r="AF37" s="47"/>
+      <c r="AG37" s="47"/>
+      <c r="AH37" s="47"/>
+      <c r="AI37" s="47"/>
+      <c r="AJ37" s="47"/>
+      <c r="AK37" s="47"/>
+      <c r="AL37" s="46"/>
+      <c r="AM37" s="46"/>
+      <c r="AN37" s="46"/>
+      <c r="AO37" s="46"/>
+      <c r="AP37" s="46"/>
+      <c r="AQ37" s="46"/>
+      <c r="AR37" s="46"/>
+      <c r="AS37" s="46"/>
+      <c r="AT37" s="46"/>
+      <c r="AU37" s="46"/>
+      <c r="AV37" s="46"/>
+      <c r="AW37" s="46"/>
+      <c r="AX37" s="46"/>
+      <c r="AY37" s="46"/>
+      <c r="AZ37" s="46"/>
+      <c r="BA37" s="47"/>
+      <c r="BB37" s="47"/>
+      <c r="BC37" s="47"/>
+      <c r="BD37" s="47"/>
+      <c r="BE37" s="47"/>
+      <c r="BF37" s="47"/>
+      <c r="BG37" s="35"/>
     </row>
     <row r="38" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" s="35"/>
       <c r="B38" s="36"/>
       <c r="C38" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D38" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E38" s="38"/>
       <c r="F38" s="38"/>
@@ -4121,11 +4148,11 @@
       <c r="H38" s="40">
         <v>0</v>
       </c>
-      <c r="I38" s="50"/>
-      <c r="J38" s="59"/>
-      <c r="K38" s="43"/>
-      <c r="L38" s="43"/>
-      <c r="M38" s="43"/>
+      <c r="I38" s="62"/>
+      <c r="J38" s="45"/>
+      <c r="K38" s="46"/>
+      <c r="L38" s="46"/>
+      <c r="M38" s="46"/>
       <c r="N38" s="46"/>
       <c r="O38" s="46"/>
       <c r="P38" s="46"/>
@@ -4177,10 +4204,10 @@
       <c r="A39" s="35"/>
       <c r="B39" s="36"/>
       <c r="C39" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D39" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E39" s="38"/>
       <c r="F39" s="38"/>
@@ -4246,17 +4273,17 @@
       <c r="A40" s="35"/>
       <c r="B40" s="36"/>
       <c r="C40" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D40" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E40" s="38"/>
       <c r="F40" s="38"/>
       <c r="G40" s="39">
         <v>0</v>
       </c>
-      <c r="H40" s="40">
+      <c r="H40" s="49">
         <v>0</v>
       </c>
       <c r="I40" s="62"/>
@@ -4315,17 +4342,17 @@
       <c r="A41" s="35"/>
       <c r="B41" s="36"/>
       <c r="C41" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D41" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E41" s="38"/>
       <c r="F41" s="38"/>
       <c r="G41" s="39">
         <v>0</v>
       </c>
-      <c r="H41" s="49">
+      <c r="H41" s="40">
         <v>0</v>
       </c>
       <c r="I41" s="62"/>
@@ -4384,10 +4411,10 @@
       <c r="A42" s="35"/>
       <c r="B42" s="36"/>
       <c r="C42" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D42" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E42" s="38"/>
       <c r="F42" s="38"/>
@@ -4449,223 +4476,223 @@
       <c r="BF42" s="47"/>
       <c r="BG42" s="35"/>
     </row>
-    <row r="43" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="35"/>
-      <c r="B43" s="36"/>
-      <c r="C43" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="E43" s="38"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="39">
+    <row r="43" spans="1:59" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="14"/>
+      <c r="B43" s="28">
+        <v>4</v>
+      </c>
+      <c r="C43" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D43" s="30"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="30"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="32"/>
+      <c r="J43" s="33"/>
+      <c r="K43" s="34"/>
+      <c r="L43" s="34"/>
+      <c r="M43" s="32"/>
+      <c r="N43" s="32"/>
+      <c r="O43" s="32"/>
+      <c r="P43" s="32"/>
+      <c r="Q43" s="32"/>
+      <c r="R43" s="32"/>
+      <c r="S43" s="32"/>
+      <c r="T43" s="32"/>
+      <c r="U43" s="32"/>
+      <c r="V43" s="32"/>
+      <c r="W43" s="32"/>
+      <c r="X43" s="32"/>
+      <c r="Y43" s="32"/>
+      <c r="Z43" s="32"/>
+      <c r="AA43" s="32"/>
+      <c r="AB43" s="32"/>
+      <c r="AC43" s="32"/>
+      <c r="AD43" s="32"/>
+      <c r="AE43" s="32"/>
+      <c r="AF43" s="32"/>
+      <c r="AG43" s="32"/>
+      <c r="AH43" s="32"/>
+      <c r="AI43" s="32"/>
+      <c r="AJ43" s="32"/>
+      <c r="AK43" s="32"/>
+      <c r="AL43" s="32"/>
+      <c r="AM43" s="32"/>
+      <c r="AN43" s="32"/>
+      <c r="AO43" s="32"/>
+      <c r="AP43" s="32"/>
+      <c r="AQ43" s="32"/>
+      <c r="AR43" s="32"/>
+      <c r="AS43" s="32"/>
+      <c r="AT43" s="32"/>
+      <c r="AU43" s="32"/>
+      <c r="AV43" s="32"/>
+      <c r="AW43" s="32"/>
+      <c r="AX43" s="32"/>
+      <c r="AY43" s="32"/>
+      <c r="AZ43" s="32"/>
+      <c r="BA43" s="32"/>
+      <c r="BB43" s="32"/>
+      <c r="BC43" s="32"/>
+      <c r="BD43" s="32"/>
+      <c r="BE43" s="32"/>
+      <c r="BF43" s="32"/>
+      <c r="BG43" s="14"/>
+    </row>
+    <row r="44" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="35"/>
+      <c r="B44" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="D44" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="E44" s="38">
+        <v>45726</v>
+      </c>
+      <c r="F44" s="38">
+        <v>45774</v>
+      </c>
+      <c r="G44" s="39">
+        <v>50</v>
+      </c>
+      <c r="H44" s="40">
         <v>0</v>
       </c>
-      <c r="H43" s="40">
-        <v>0</v>
-      </c>
-      <c r="I43" s="62"/>
-      <c r="J43" s="45"/>
-      <c r="K43" s="46"/>
-      <c r="L43" s="46"/>
-      <c r="M43" s="46"/>
-      <c r="N43" s="46"/>
-      <c r="O43" s="46"/>
-      <c r="P43" s="46"/>
-      <c r="Q43" s="46"/>
-      <c r="R43" s="46"/>
-      <c r="S43" s="46"/>
-      <c r="T43" s="46"/>
-      <c r="U43" s="46"/>
-      <c r="V43" s="46"/>
-      <c r="W43" s="46"/>
-      <c r="X43" s="46"/>
-      <c r="Y43" s="46"/>
-      <c r="Z43" s="46"/>
-      <c r="AA43" s="46"/>
-      <c r="AB43" s="46"/>
-      <c r="AC43" s="47"/>
-      <c r="AD43" s="47"/>
-      <c r="AE43" s="47"/>
-      <c r="AF43" s="47"/>
-      <c r="AG43" s="47"/>
-      <c r="AH43" s="47"/>
-      <c r="AI43" s="47"/>
-      <c r="AJ43" s="47"/>
-      <c r="AK43" s="47"/>
-      <c r="AL43" s="46"/>
-      <c r="AM43" s="46"/>
-      <c r="AN43" s="46"/>
-      <c r="AO43" s="46"/>
-      <c r="AP43" s="46"/>
-      <c r="AQ43" s="46"/>
-      <c r="AR43" s="46"/>
-      <c r="AS43" s="46"/>
-      <c r="AT43" s="46"/>
-      <c r="AU43" s="46"/>
-      <c r="AV43" s="46"/>
-      <c r="AW43" s="46"/>
-      <c r="AX43" s="46"/>
-      <c r="AY43" s="46"/>
-      <c r="AZ43" s="46"/>
-      <c r="BA43" s="47"/>
-      <c r="BB43" s="47"/>
-      <c r="BC43" s="47"/>
-      <c r="BD43" s="47"/>
-      <c r="BE43" s="47"/>
-      <c r="BF43" s="47"/>
-      <c r="BG43" s="35"/>
-    </row>
-    <row r="44" spans="1:59" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
-      <c r="B44" s="28">
-        <v>4</v>
-      </c>
-      <c r="C44" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="D44" s="30"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="30"/>
-      <c r="H44" s="30"/>
-      <c r="I44" s="32"/>
-      <c r="J44" s="33"/>
-      <c r="K44" s="34"/>
-      <c r="L44" s="34"/>
-      <c r="M44" s="32"/>
-      <c r="N44" s="32"/>
-      <c r="O44" s="32"/>
-      <c r="P44" s="32"/>
-      <c r="Q44" s="32"/>
-      <c r="R44" s="32"/>
-      <c r="S44" s="32"/>
-      <c r="T44" s="32"/>
-      <c r="U44" s="32"/>
-      <c r="V44" s="32"/>
-      <c r="W44" s="32"/>
-      <c r="X44" s="32"/>
-      <c r="Y44" s="32"/>
-      <c r="Z44" s="32"/>
-      <c r="AA44" s="32"/>
-      <c r="AB44" s="32"/>
-      <c r="AC44" s="32"/>
-      <c r="AD44" s="32"/>
-      <c r="AE44" s="32"/>
-      <c r="AF44" s="32"/>
-      <c r="AG44" s="32"/>
-      <c r="AH44" s="32"/>
-      <c r="AI44" s="32"/>
-      <c r="AJ44" s="32"/>
-      <c r="AK44" s="32"/>
-      <c r="AL44" s="32"/>
-      <c r="AM44" s="32"/>
-      <c r="AN44" s="32"/>
-      <c r="AO44" s="32"/>
-      <c r="AP44" s="32"/>
-      <c r="AQ44" s="32"/>
-      <c r="AR44" s="32"/>
-      <c r="AS44" s="32"/>
-      <c r="AT44" s="32"/>
-      <c r="AU44" s="32"/>
-      <c r="AV44" s="32"/>
-      <c r="AW44" s="32"/>
-      <c r="AX44" s="32"/>
-      <c r="AY44" s="32"/>
-      <c r="AZ44" s="32"/>
-      <c r="BA44" s="32"/>
-      <c r="BB44" s="32"/>
-      <c r="BC44" s="32"/>
-      <c r="BD44" s="32"/>
-      <c r="BE44" s="32"/>
-      <c r="BF44" s="32"/>
-      <c r="BG44" s="14"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
+      <c r="K44" s="41"/>
+      <c r="L44" s="41"/>
+      <c r="M44" s="41"/>
+      <c r="N44" s="41"/>
+      <c r="O44" s="41"/>
+      <c r="P44" s="41"/>
+      <c r="Q44" s="41"/>
+      <c r="R44" s="41"/>
+      <c r="S44" s="41"/>
+      <c r="T44" s="41"/>
+      <c r="U44" s="41"/>
+      <c r="V44" s="41"/>
+      <c r="W44" s="41"/>
+      <c r="X44" s="63"/>
+      <c r="Y44" s="63"/>
+      <c r="Z44" s="63"/>
+      <c r="AA44" s="63"/>
+      <c r="AB44" s="63"/>
+      <c r="AC44" s="64"/>
+      <c r="AD44" s="64"/>
+      <c r="AE44" s="64"/>
+      <c r="AF44" s="64"/>
+      <c r="AG44" s="64"/>
+      <c r="AH44" s="64"/>
+      <c r="AI44" s="64"/>
+      <c r="AJ44" s="64"/>
+      <c r="AK44" s="64"/>
+      <c r="AL44" s="63"/>
+      <c r="AM44" s="63"/>
+      <c r="AN44" s="63"/>
+      <c r="AO44" s="63"/>
+      <c r="AP44" s="63"/>
+      <c r="AQ44" s="63"/>
+      <c r="AR44" s="63"/>
+      <c r="AS44" s="63"/>
+      <c r="AT44" s="63"/>
+      <c r="AU44" s="63"/>
+      <c r="AV44" s="63"/>
+      <c r="AW44" s="63"/>
+      <c r="AX44" s="63"/>
+      <c r="AY44" s="63"/>
+      <c r="AZ44" s="63"/>
+      <c r="BA44" s="64"/>
+      <c r="BB44" s="64"/>
+      <c r="BC44" s="64"/>
+      <c r="BD44" s="64"/>
+      <c r="BE44" s="64"/>
+      <c r="BF44" s="64"/>
+      <c r="BG44" s="35"/>
     </row>
     <row r="45" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A45" s="35"/>
-      <c r="B45" s="36">
-        <v>4.0999999999999996</v>
-      </c>
+      <c r="B45" s="36"/>
       <c r="C45" s="37" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="D45" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="E45" s="38">
-        <v>45726</v>
-      </c>
-      <c r="F45" s="38">
-        <v>45774</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="E45" s="38"/>
+      <c r="F45" s="38"/>
       <c r="G45" s="39">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="H45" s="40">
         <v>0</v>
       </c>
-      <c r="I45" s="63"/>
-      <c r="J45" s="64"/>
-      <c r="K45" s="65"/>
-      <c r="L45" s="65"/>
-      <c r="M45" s="65"/>
-      <c r="N45" s="66"/>
-      <c r="O45" s="66"/>
-      <c r="P45" s="66"/>
-      <c r="Q45" s="66"/>
-      <c r="R45" s="66"/>
-      <c r="S45" s="66"/>
-      <c r="T45" s="66"/>
-      <c r="U45" s="66"/>
-      <c r="V45" s="66"/>
-      <c r="W45" s="66"/>
-      <c r="X45" s="66"/>
-      <c r="Y45" s="66"/>
-      <c r="Z45" s="66"/>
-      <c r="AA45" s="66"/>
-      <c r="AB45" s="66"/>
-      <c r="AC45" s="67"/>
-      <c r="AD45" s="67"/>
-      <c r="AE45" s="67"/>
-      <c r="AF45" s="67"/>
-      <c r="AG45" s="67"/>
-      <c r="AH45" s="67"/>
-      <c r="AI45" s="67"/>
-      <c r="AJ45" s="67"/>
-      <c r="AK45" s="67"/>
-      <c r="AL45" s="66"/>
-      <c r="AM45" s="66"/>
-      <c r="AN45" s="66"/>
-      <c r="AO45" s="66"/>
-      <c r="AP45" s="66"/>
-      <c r="AQ45" s="66"/>
-      <c r="AR45" s="66"/>
-      <c r="AS45" s="66"/>
-      <c r="AT45" s="66"/>
-      <c r="AU45" s="66"/>
-      <c r="AV45" s="66"/>
-      <c r="AW45" s="66"/>
-      <c r="AX45" s="66"/>
-      <c r="AY45" s="66"/>
-      <c r="AZ45" s="66"/>
-      <c r="BA45" s="67"/>
-      <c r="BB45" s="67"/>
-      <c r="BC45" s="67"/>
-      <c r="BD45" s="67"/>
-      <c r="BE45" s="67"/>
-      <c r="BF45" s="67"/>
+      <c r="I45" s="62"/>
+      <c r="J45" s="45"/>
+      <c r="K45" s="46"/>
+      <c r="L45" s="46"/>
+      <c r="M45" s="46"/>
+      <c r="N45" s="46"/>
+      <c r="O45" s="46"/>
+      <c r="P45" s="46"/>
+      <c r="Q45" s="46"/>
+      <c r="R45" s="46"/>
+      <c r="S45" s="46"/>
+      <c r="T45" s="46"/>
+      <c r="U45" s="46"/>
+      <c r="V45" s="46"/>
+      <c r="W45" s="46"/>
+      <c r="X45" s="46"/>
+      <c r="Y45" s="46"/>
+      <c r="Z45" s="46"/>
+      <c r="AA45" s="46"/>
+      <c r="AB45" s="46"/>
+      <c r="AC45" s="47"/>
+      <c r="AD45" s="47"/>
+      <c r="AE45" s="47"/>
+      <c r="AF45" s="47"/>
+      <c r="AG45" s="47"/>
+      <c r="AH45" s="47"/>
+      <c r="AI45" s="47"/>
+      <c r="AJ45" s="47"/>
+      <c r="AK45" s="47"/>
+      <c r="AL45" s="46"/>
+      <c r="AM45" s="46"/>
+      <c r="AN45" s="46"/>
+      <c r="AO45" s="46"/>
+      <c r="AP45" s="46"/>
+      <c r="AQ45" s="46"/>
+      <c r="AR45" s="46"/>
+      <c r="AS45" s="46"/>
+      <c r="AT45" s="46"/>
+      <c r="AU45" s="46"/>
+      <c r="AV45" s="46"/>
+      <c r="AW45" s="46"/>
+      <c r="AX45" s="46"/>
+      <c r="AY45" s="46"/>
+      <c r="AZ45" s="46"/>
+      <c r="BA45" s="47"/>
+      <c r="BB45" s="47"/>
+      <c r="BC45" s="47"/>
+      <c r="BD45" s="47"/>
+      <c r="BE45" s="47"/>
+      <c r="BF45" s="47"/>
       <c r="BG45" s="35"/>
     </row>
     <row r="46" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A46" s="35"/>
       <c r="B46" s="36"/>
       <c r="C46" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D46" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E46" s="38"/>
       <c r="F46" s="38"/>
@@ -4731,17 +4758,17 @@
       <c r="A47" s="35"/>
       <c r="B47" s="36"/>
       <c r="C47" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D47" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E47" s="38"/>
       <c r="F47" s="38"/>
       <c r="G47" s="39">
         <v>0</v>
       </c>
-      <c r="H47" s="40">
+      <c r="H47" s="49">
         <v>0</v>
       </c>
       <c r="I47" s="62"/>
@@ -4796,84 +4823,76 @@
       <c r="BF47" s="47"/>
       <c r="BG47" s="35"/>
     </row>
-    <row r="48" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="35"/>
-      <c r="B48" s="36"/>
-      <c r="C48" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="D48" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="E48" s="38"/>
-      <c r="F48" s="38"/>
-      <c r="G48" s="39">
-        <v>0</v>
-      </c>
-      <c r="H48" s="49">
-        <v>0</v>
-      </c>
-      <c r="I48" s="62"/>
-      <c r="J48" s="45"/>
-      <c r="K48" s="46"/>
-      <c r="L48" s="46"/>
-      <c r="M48" s="46"/>
-      <c r="N48" s="46"/>
-      <c r="O48" s="46"/>
-      <c r="P48" s="46"/>
-      <c r="Q48" s="46"/>
-      <c r="R48" s="46"/>
-      <c r="S48" s="46"/>
-      <c r="T48" s="46"/>
-      <c r="U48" s="46"/>
-      <c r="V48" s="46"/>
-      <c r="W48" s="46"/>
-      <c r="X48" s="46"/>
-      <c r="Y48" s="46"/>
-      <c r="Z48" s="46"/>
-      <c r="AA48" s="46"/>
-      <c r="AB48" s="46"/>
-      <c r="AC48" s="47"/>
-      <c r="AD48" s="47"/>
-      <c r="AE48" s="47"/>
-      <c r="AF48" s="47"/>
-      <c r="AG48" s="47"/>
-      <c r="AH48" s="47"/>
-      <c r="AI48" s="47"/>
-      <c r="AJ48" s="47"/>
-      <c r="AK48" s="47"/>
-      <c r="AL48" s="46"/>
-      <c r="AM48" s="46"/>
-      <c r="AN48" s="46"/>
-      <c r="AO48" s="46"/>
-      <c r="AP48" s="46"/>
-      <c r="AQ48" s="46"/>
-      <c r="AR48" s="46"/>
-      <c r="AS48" s="46"/>
-      <c r="AT48" s="46"/>
-      <c r="AU48" s="46"/>
-      <c r="AV48" s="46"/>
-      <c r="AW48" s="46"/>
-      <c r="AX48" s="46"/>
-      <c r="AY48" s="46"/>
-      <c r="AZ48" s="46"/>
-      <c r="BA48" s="47"/>
-      <c r="BB48" s="47"/>
-      <c r="BC48" s="47"/>
-      <c r="BD48" s="47"/>
-      <c r="BE48" s="47"/>
-      <c r="BF48" s="47"/>
-      <c r="BG48" s="35"/>
+    <row r="48" spans="1:59" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="14"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="65"/>
+      <c r="F48" s="65"/>
+      <c r="G48" s="66"/>
+      <c r="H48" s="66"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="14"/>
+      <c r="K48" s="14"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="14"/>
+      <c r="N48" s="14"/>
+      <c r="O48" s="14"/>
+      <c r="P48" s="14"/>
+      <c r="Q48" s="14"/>
+      <c r="R48" s="14"/>
+      <c r="S48" s="14"/>
+      <c r="T48" s="14"/>
+      <c r="U48" s="14"/>
+      <c r="V48" s="14"/>
+      <c r="W48" s="14"/>
+      <c r="X48" s="14"/>
+      <c r="Y48" s="14"/>
+      <c r="Z48" s="14"/>
+      <c r="AA48" s="14"/>
+      <c r="AB48" s="14"/>
+      <c r="AC48" s="14"/>
+      <c r="AD48" s="14"/>
+      <c r="AE48" s="14"/>
+      <c r="AF48" s="14"/>
+      <c r="AG48" s="14"/>
+      <c r="AH48" s="14"/>
+      <c r="AI48" s="14"/>
+      <c r="AJ48" s="14"/>
+      <c r="AK48" s="14"/>
+      <c r="AL48" s="14"/>
+      <c r="AM48" s="14"/>
+      <c r="AN48" s="14"/>
+      <c r="AO48" s="14"/>
+      <c r="AP48" s="14"/>
+      <c r="AQ48" s="14"/>
+      <c r="AR48" s="14"/>
+      <c r="AS48" s="14"/>
+      <c r="AT48" s="14"/>
+      <c r="AU48" s="14"/>
+      <c r="AV48" s="14"/>
+      <c r="AW48" s="14"/>
+      <c r="AX48" s="14"/>
+      <c r="AY48" s="14"/>
+      <c r="AZ48" s="14"/>
+      <c r="BA48" s="14"/>
+      <c r="BB48" s="14"/>
+      <c r="BC48" s="14"/>
+      <c r="BD48" s="14"/>
+      <c r="BE48" s="14"/>
+      <c r="BF48" s="14"/>
+      <c r="BG48" s="14"/>
     </row>
     <row r="49" spans="1:59" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14"/>
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
       <c r="D49" s="14"/>
-      <c r="E49" s="68"/>
-      <c r="F49" s="68"/>
-      <c r="G49" s="69"/>
-      <c r="H49" s="69"/>
+      <c r="E49" s="65"/>
+      <c r="F49" s="65"/>
+      <c r="G49" s="66"/>
+      <c r="H49" s="66"/>
       <c r="I49" s="14"/>
       <c r="J49" s="14"/>
       <c r="K49" s="14"/>
@@ -4931,10 +4950,10 @@
       <c r="B50" s="14"/>
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
-      <c r="E50" s="68"/>
-      <c r="F50" s="68"/>
-      <c r="G50" s="69"/>
-      <c r="H50" s="69"/>
+      <c r="E50" s="65"/>
+      <c r="F50" s="65"/>
+      <c r="G50" s="66"/>
+      <c r="H50" s="66"/>
       <c r="I50" s="14"/>
       <c r="J50" s="14"/>
       <c r="K50" s="14"/>
@@ -4987,69 +5006,20 @@
       <c r="BF50" s="14"/>
       <c r="BG50" s="14"/>
     </row>
-    <row r="51" spans="1:59" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="68"/>
-      <c r="F51" s="68"/>
-      <c r="G51" s="69"/>
-      <c r="H51" s="69"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14"/>
-      <c r="L51" s="14"/>
-      <c r="M51" s="14"/>
-      <c r="N51" s="14"/>
-      <c r="O51" s="14"/>
-      <c r="P51" s="14"/>
-      <c r="Q51" s="14"/>
-      <c r="R51" s="14"/>
-      <c r="S51" s="14"/>
-      <c r="T51" s="14"/>
-      <c r="U51" s="14"/>
-      <c r="V51" s="14"/>
-      <c r="W51" s="14"/>
-      <c r="X51" s="14"/>
-      <c r="Y51" s="14"/>
-      <c r="Z51" s="14"/>
-      <c r="AA51" s="14"/>
-      <c r="AB51" s="14"/>
-      <c r="AC51" s="14"/>
-      <c r="AD51" s="14"/>
-      <c r="AE51" s="14"/>
-      <c r="AF51" s="14"/>
-      <c r="AG51" s="14"/>
-      <c r="AH51" s="14"/>
-      <c r="AI51" s="14"/>
-      <c r="AJ51" s="14"/>
-      <c r="AK51" s="14"/>
-      <c r="AL51" s="14"/>
-      <c r="AM51" s="14"/>
-      <c r="AN51" s="14"/>
-      <c r="AO51" s="14"/>
-      <c r="AP51" s="14"/>
-      <c r="AQ51" s="14"/>
-      <c r="AR51" s="14"/>
-      <c r="AS51" s="14"/>
-      <c r="AT51" s="14"/>
-      <c r="AU51" s="14"/>
-      <c r="AV51" s="14"/>
-      <c r="AW51" s="14"/>
-      <c r="AX51" s="14"/>
-      <c r="AY51" s="14"/>
-      <c r="AZ51" s="14"/>
-      <c r="BA51" s="14"/>
-      <c r="BB51" s="14"/>
-      <c r="BC51" s="14"/>
-      <c r="BD51" s="14"/>
-      <c r="BE51" s="14"/>
-      <c r="BF51" s="14"/>
-      <c r="BG51" s="14"/>
-    </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B1:AE2"/>
+    <mergeCell ref="AL8:BF8"/>
+    <mergeCell ref="I9:P9"/>
+    <mergeCell ref="Q9:W9"/>
+    <mergeCell ref="X9:AD9"/>
+    <mergeCell ref="AE9:AK9"/>
+    <mergeCell ref="AL9:AR9"/>
+    <mergeCell ref="AS9:AY9"/>
+    <mergeCell ref="AZ9:BF9"/>
+    <mergeCell ref="I8:W8"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:G5"/>
     <mergeCell ref="P5:AA5"/>
@@ -5058,25 +5028,13 @@
     <mergeCell ref="C8:C11"/>
     <mergeCell ref="H8:H11"/>
     <mergeCell ref="X8:AK8"/>
-    <mergeCell ref="AL8:BF8"/>
-    <mergeCell ref="I9:P9"/>
-    <mergeCell ref="Q9:W9"/>
-    <mergeCell ref="X9:AD9"/>
-    <mergeCell ref="AE9:AK9"/>
-    <mergeCell ref="AL9:AR9"/>
-    <mergeCell ref="AS9:AY9"/>
-    <mergeCell ref="AZ9:BF9"/>
     <mergeCell ref="D8:D11"/>
     <mergeCell ref="E8:E11"/>
     <mergeCell ref="F8:F11"/>
     <mergeCell ref="G8:G11"/>
     <mergeCell ref="I5:O5"/>
-    <mergeCell ref="I8:W8"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="B1:AE2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H33:H48 H13:H31">
+  <conditionalFormatting sqref="H32:H47 H13:H30">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Updates doc for delivery milestone01
</commit_message>
<xml_diff>
--- a/Project/Gantt chart.xlsx
+++ b/Project/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stupc\Documents\GitHub\trip-clothing-planner\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1D0CF0-ED12-4EA2-8464-2B02AECBBC72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A2C9C8-2FE5-4E8A-B00E-953CA0BC7163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="72">
   <si>
     <t>GANTT CHART SD2 - CHATBOT</t>
   </si>
@@ -239,9 +239,6 @@
     <t xml:space="preserve">Prototype </t>
   </si>
   <si>
-    <t>Report</t>
-  </si>
-  <si>
     <t xml:space="preserve">Report </t>
   </si>
   <si>
@@ -288,6 +285,18 @@
   </si>
   <si>
     <t>First research</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>1.13</t>
+  </si>
+  <si>
+    <t>1.14</t>
+  </si>
+  <si>
+    <t>Fill project doc</t>
   </si>
 </sst>
 </file>
@@ -431,7 +440,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -514,12 +523,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
         <bgColor rgb="FFCCCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA4C2F4"/>
-        <bgColor rgb="FFA4C2F4"/>
       </patternFill>
     </fill>
     <fill>
@@ -737,7 +740,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -858,9 +861,6 @@
     <xf numFmtId="9" fontId="24" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="24" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -875,7 +875,7 @@
     <xf numFmtId="165" fontId="24" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="23" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="23" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="24" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -913,10 +913,10 @@
     <xf numFmtId="9" fontId="24" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -931,22 +931,19 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -961,20 +958,23 @@
     <xf numFmtId="0" fontId="16" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="15" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1296,8 +1296,8 @@
   </sheetPr>
   <dimension ref="A1:BG50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1316,38 +1316,38 @@
   <sheetData>
     <row r="1" spans="1:59" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="86"/>
-      <c r="O1" s="86"/>
-      <c r="P1" s="86"/>
-      <c r="Q1" s="86"/>
-      <c r="R1" s="86"/>
-      <c r="S1" s="86"/>
-      <c r="T1" s="86"/>
-      <c r="U1" s="86"/>
-      <c r="V1" s="86"/>
-      <c r="W1" s="86"/>
-      <c r="X1" s="86"/>
-      <c r="Y1" s="86"/>
-      <c r="Z1" s="86"/>
-      <c r="AA1" s="86"/>
-      <c r="AB1" s="86"/>
-      <c r="AC1" s="86"/>
-      <c r="AD1" s="86"/>
-      <c r="AE1" s="86"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="71"/>
+      <c r="R1" s="71"/>
+      <c r="S1" s="71"/>
+      <c r="T1" s="71"/>
+      <c r="U1" s="71"/>
+      <c r="V1" s="71"/>
+      <c r="W1" s="71"/>
+      <c r="X1" s="71"/>
+      <c r="Y1" s="71"/>
+      <c r="Z1" s="71"/>
+      <c r="AA1" s="71"/>
+      <c r="AB1" s="71"/>
+      <c r="AC1" s="71"/>
+      <c r="AD1" s="71"/>
+      <c r="AE1" s="71"/>
       <c r="AF1" s="2"/>
       <c r="AG1" s="2"/>
       <c r="AH1" s="2"/>
@@ -1379,36 +1379,36 @@
     </row>
     <row r="2" spans="1:59" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="87"/>
-      <c r="M2" s="87"/>
-      <c r="N2" s="87"/>
-      <c r="O2" s="87"/>
-      <c r="P2" s="87"/>
-      <c r="Q2" s="87"/>
-      <c r="R2" s="87"/>
-      <c r="S2" s="87"/>
-      <c r="T2" s="87"/>
-      <c r="U2" s="87"/>
-      <c r="V2" s="87"/>
-      <c r="W2" s="87"/>
-      <c r="X2" s="87"/>
-      <c r="Y2" s="87"/>
-      <c r="Z2" s="87"/>
-      <c r="AA2" s="87"/>
-      <c r="AB2" s="87"/>
-      <c r="AC2" s="87"/>
-      <c r="AD2" s="87"/>
-      <c r="AE2" s="87"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="72"/>
+      <c r="P2" s="72"/>
+      <c r="Q2" s="72"/>
+      <c r="R2" s="72"/>
+      <c r="S2" s="72"/>
+      <c r="T2" s="72"/>
+      <c r="U2" s="72"/>
+      <c r="V2" s="72"/>
+      <c r="W2" s="72"/>
+      <c r="X2" s="72"/>
+      <c r="Y2" s="72"/>
+      <c r="Z2" s="72"/>
+      <c r="AA2" s="72"/>
+      <c r="AB2" s="72"/>
+      <c r="AC2" s="72"/>
+      <c r="AD2" s="72"/>
+      <c r="AE2" s="72"/>
       <c r="AF2" s="3"/>
       <c r="AG2" s="3"/>
       <c r="AH2" s="3"/>
@@ -1501,39 +1501,39 @@
     </row>
     <row r="4" spans="1:59" ht="21" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A4" s="1"/>
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="70"/>
-      <c r="D4" s="85" t="s">
+      <c r="C4" s="69"/>
+      <c r="D4" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
       <c r="H4" s="9"/>
-      <c r="I4" s="68" t="s">
+      <c r="I4" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
-      <c r="M4" s="67"/>
-      <c r="N4" s="67"/>
-      <c r="O4" s="67"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="66"/>
+      <c r="O4" s="66"/>
       <c r="P4" s="11"/>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67"/>
-      <c r="T4" s="67"/>
-      <c r="U4" s="67"/>
-      <c r="V4" s="67"/>
-      <c r="W4" s="67"/>
-      <c r="X4" s="67"/>
-      <c r="Y4" s="67"/>
-      <c r="Z4" s="67"/>
-      <c r="AA4" s="67"/>
-      <c r="AB4" s="67"/>
+      <c r="Q4" s="66"/>
+      <c r="R4" s="66"/>
+      <c r="S4" s="66"/>
+      <c r="T4" s="66"/>
+      <c r="U4" s="66"/>
+      <c r="V4" s="66"/>
+      <c r="W4" s="66"/>
+      <c r="X4" s="66"/>
+      <c r="Y4" s="66"/>
+      <c r="Z4" s="66"/>
+      <c r="AA4" s="66"/>
+      <c r="AB4" s="66"/>
       <c r="AC4" s="10"/>
       <c r="AD4" s="2"/>
       <c r="AE4" s="2"/>
@@ -1568,38 +1568,38 @@
     </row>
     <row r="5" spans="1:59" ht="21" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A5" s="1"/>
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
       <c r="H5" s="12"/>
-      <c r="I5" s="69" t="s">
+      <c r="I5" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="70"/>
-      <c r="K5" s="70"/>
-      <c r="L5" s="70"/>
-      <c r="M5" s="70"/>
-      <c r="N5" s="70"/>
-      <c r="O5" s="70"/>
-      <c r="P5" s="72" t="s">
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="Q5" s="70"/>
-      <c r="R5" s="70"/>
-      <c r="S5" s="70"/>
-      <c r="T5" s="70"/>
-      <c r="U5" s="70"/>
-      <c r="V5" s="70"/>
-      <c r="W5" s="70"/>
-      <c r="X5" s="70"/>
-      <c r="Y5" s="70"/>
-      <c r="Z5" s="70"/>
-      <c r="AA5" s="70"/>
+      <c r="Q5" s="69"/>
+      <c r="R5" s="69"/>
+      <c r="S5" s="69"/>
+      <c r="T5" s="69"/>
+      <c r="U5" s="69"/>
+      <c r="V5" s="69"/>
+      <c r="W5" s="69"/>
+      <c r="X5" s="69"/>
+      <c r="Y5" s="69"/>
+      <c r="Z5" s="69"/>
+      <c r="AA5" s="69"/>
       <c r="AB5" s="13"/>
       <c r="AC5" s="10"/>
       <c r="AD5" s="1"/>
@@ -1635,14 +1635,14 @@
     </row>
     <row r="6" spans="1:59" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="69"/>
       <c r="H6" s="15"/>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
@@ -1759,28 +1759,28 @@
     </row>
     <row r="8" spans="1:59" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="73" t="s">
+      <c r="C8" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="73" t="s">
+      <c r="D8" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="83" t="s">
+      <c r="E8" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="83" t="s">
+      <c r="F8" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="73" t="s">
+      <c r="G8" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="73" t="s">
+      <c r="H8" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="84" t="s">
+      <c r="I8" s="81" t="s">
         <v>15</v>
       </c>
       <c r="J8" s="74"/>
@@ -1797,7 +1797,7 @@
       <c r="U8" s="74"/>
       <c r="V8" s="74"/>
       <c r="W8" s="74"/>
-      <c r="X8" s="75" t="s">
+      <c r="X8" s="85" t="s">
         <v>16</v>
       </c>
       <c r="Y8" s="74"/>
@@ -1813,7 +1813,7 @@
       <c r="AI8" s="74"/>
       <c r="AJ8" s="74"/>
       <c r="AK8" s="74"/>
-      <c r="AL8" s="76" t="s">
+      <c r="AL8" s="73" t="s">
         <v>17</v>
       </c>
       <c r="AM8" s="74"/>
@@ -1847,70 +1847,70 @@
       <c r="F9" s="74"/>
       <c r="G9" s="74"/>
       <c r="H9" s="74"/>
-      <c r="I9" s="77" t="s">
+      <c r="I9" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="78"/>
-      <c r="K9" s="78"/>
-      <c r="L9" s="78"/>
-      <c r="M9" s="78"/>
-      <c r="N9" s="78"/>
-      <c r="O9" s="78"/>
-      <c r="P9" s="78"/>
-      <c r="Q9" s="77" t="s">
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
+      <c r="O9" s="76"/>
+      <c r="P9" s="76"/>
+      <c r="Q9" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="R9" s="78"/>
-      <c r="S9" s="78"/>
-      <c r="T9" s="78"/>
-      <c r="U9" s="78"/>
-      <c r="V9" s="78"/>
-      <c r="W9" s="79"/>
-      <c r="X9" s="80" t="s">
+      <c r="R9" s="76"/>
+      <c r="S9" s="76"/>
+      <c r="T9" s="76"/>
+      <c r="U9" s="76"/>
+      <c r="V9" s="76"/>
+      <c r="W9" s="77"/>
+      <c r="X9" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="Y9" s="78"/>
-      <c r="Z9" s="78"/>
-      <c r="AA9" s="78"/>
-      <c r="AB9" s="78"/>
-      <c r="AC9" s="78"/>
-      <c r="AD9" s="79"/>
-      <c r="AE9" s="81" t="s">
+      <c r="Y9" s="76"/>
+      <c r="Z9" s="76"/>
+      <c r="AA9" s="76"/>
+      <c r="AB9" s="76"/>
+      <c r="AC9" s="76"/>
+      <c r="AD9" s="77"/>
+      <c r="AE9" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="AF9" s="78"/>
-      <c r="AG9" s="78"/>
-      <c r="AH9" s="78"/>
-      <c r="AI9" s="78"/>
-      <c r="AJ9" s="78"/>
-      <c r="AK9" s="79"/>
-      <c r="AL9" s="82" t="s">
+      <c r="AF9" s="76"/>
+      <c r="AG9" s="76"/>
+      <c r="AH9" s="76"/>
+      <c r="AI9" s="76"/>
+      <c r="AJ9" s="76"/>
+      <c r="AK9" s="77"/>
+      <c r="AL9" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="AM9" s="78"/>
-      <c r="AN9" s="78"/>
-      <c r="AO9" s="78"/>
-      <c r="AP9" s="78"/>
-      <c r="AQ9" s="78"/>
-      <c r="AR9" s="79"/>
-      <c r="AS9" s="82" t="s">
+      <c r="AM9" s="76"/>
+      <c r="AN9" s="76"/>
+      <c r="AO9" s="76"/>
+      <c r="AP9" s="76"/>
+      <c r="AQ9" s="76"/>
+      <c r="AR9" s="77"/>
+      <c r="AS9" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="AT9" s="78"/>
-      <c r="AU9" s="78"/>
-      <c r="AV9" s="78"/>
-      <c r="AW9" s="78"/>
-      <c r="AX9" s="78"/>
-      <c r="AY9" s="78"/>
-      <c r="AZ9" s="82" t="s">
+      <c r="AT9" s="76"/>
+      <c r="AU9" s="76"/>
+      <c r="AV9" s="76"/>
+      <c r="AW9" s="76"/>
+      <c r="AX9" s="76"/>
+      <c r="AY9" s="76"/>
+      <c r="AZ9" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="BA9" s="78"/>
-      <c r="BB9" s="78"/>
-      <c r="BC9" s="78"/>
-      <c r="BD9" s="78"/>
-      <c r="BE9" s="78"/>
-      <c r="BF9" s="79"/>
+      <c r="BA9" s="76"/>
+      <c r="BB9" s="76"/>
+      <c r="BC9" s="76"/>
+      <c r="BD9" s="76"/>
+      <c r="BE9" s="76"/>
+      <c r="BF9" s="77"/>
       <c r="BG9" s="19"/>
     </row>
     <row r="10" spans="1:59" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2303,7 +2303,7 @@
     <row r="13" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="35"/>
       <c r="B13" s="36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C13" s="37" t="s">
         <v>31</v>
@@ -2326,59 +2326,59 @@
       <c r="I13" s="41"/>
       <c r="J13" s="41"/>
       <c r="K13" s="41"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="43"/>
-      <c r="O13" s="43"/>
-      <c r="P13" s="43"/>
-      <c r="Q13" s="43"/>
-      <c r="R13" s="43"/>
-      <c r="S13" s="43"/>
-      <c r="T13" s="43"/>
-      <c r="U13" s="43"/>
-      <c r="V13" s="43"/>
-      <c r="W13" s="43"/>
-      <c r="X13" s="43"/>
-      <c r="Y13" s="43"/>
-      <c r="Z13" s="43"/>
-      <c r="AA13" s="43"/>
-      <c r="AB13" s="43"/>
-      <c r="AC13" s="44"/>
-      <c r="AD13" s="44"/>
-      <c r="AE13" s="44"/>
-      <c r="AF13" s="44"/>
-      <c r="AG13" s="44"/>
-      <c r="AH13" s="44"/>
-      <c r="AI13" s="44"/>
-      <c r="AJ13" s="44"/>
-      <c r="AK13" s="44"/>
-      <c r="AL13" s="43"/>
-      <c r="AM13" s="43"/>
-      <c r="AN13" s="43"/>
-      <c r="AO13" s="43"/>
-      <c r="AP13" s="43"/>
-      <c r="AQ13" s="43"/>
-      <c r="AR13" s="43"/>
-      <c r="AS13" s="43"/>
-      <c r="AT13" s="43"/>
-      <c r="AU13" s="43"/>
-      <c r="AV13" s="43"/>
-      <c r="AW13" s="43"/>
-      <c r="AX13" s="43"/>
-      <c r="AY13" s="43"/>
-      <c r="AZ13" s="43"/>
-      <c r="BA13" s="44"/>
-      <c r="BB13" s="44"/>
-      <c r="BC13" s="44"/>
-      <c r="BD13" s="44"/>
-      <c r="BE13" s="44"/>
-      <c r="BF13" s="44"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="42"/>
+      <c r="N13" s="42"/>
+      <c r="O13" s="42"/>
+      <c r="P13" s="42"/>
+      <c r="Q13" s="42"/>
+      <c r="R13" s="42"/>
+      <c r="S13" s="42"/>
+      <c r="T13" s="42"/>
+      <c r="U13" s="42"/>
+      <c r="V13" s="42"/>
+      <c r="W13" s="42"/>
+      <c r="X13" s="42"/>
+      <c r="Y13" s="42"/>
+      <c r="Z13" s="42"/>
+      <c r="AA13" s="42"/>
+      <c r="AB13" s="42"/>
+      <c r="AC13" s="43"/>
+      <c r="AD13" s="43"/>
+      <c r="AE13" s="43"/>
+      <c r="AF13" s="43"/>
+      <c r="AG13" s="43"/>
+      <c r="AH13" s="43"/>
+      <c r="AI13" s="43"/>
+      <c r="AJ13" s="43"/>
+      <c r="AK13" s="43"/>
+      <c r="AL13" s="42"/>
+      <c r="AM13" s="42"/>
+      <c r="AN13" s="42"/>
+      <c r="AO13" s="42"/>
+      <c r="AP13" s="42"/>
+      <c r="AQ13" s="42"/>
+      <c r="AR13" s="42"/>
+      <c r="AS13" s="42"/>
+      <c r="AT13" s="42"/>
+      <c r="AU13" s="42"/>
+      <c r="AV13" s="42"/>
+      <c r="AW13" s="42"/>
+      <c r="AX13" s="42"/>
+      <c r="AY13" s="42"/>
+      <c r="AZ13" s="42"/>
+      <c r="BA13" s="43"/>
+      <c r="BB13" s="43"/>
+      <c r="BC13" s="43"/>
+      <c r="BD13" s="43"/>
+      <c r="BE13" s="43"/>
+      <c r="BF13" s="43"/>
       <c r="BG13" s="35"/>
     </row>
     <row r="14" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="35"/>
       <c r="B14" s="36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="37" t="s">
         <v>33</v>
@@ -2399,61 +2399,61 @@
         <v>1</v>
       </c>
       <c r="I14" s="41"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="46"/>
-      <c r="L14" s="46"/>
-      <c r="M14" s="46"/>
-      <c r="N14" s="46"/>
-      <c r="O14" s="46"/>
-      <c r="P14" s="46"/>
-      <c r="Q14" s="46"/>
-      <c r="R14" s="46"/>
-      <c r="S14" s="46"/>
-      <c r="T14" s="46"/>
-      <c r="U14" s="46"/>
-      <c r="V14" s="46"/>
-      <c r="W14" s="46"/>
-      <c r="X14" s="46"/>
-      <c r="Y14" s="46"/>
-      <c r="Z14" s="46"/>
-      <c r="AA14" s="46"/>
-      <c r="AB14" s="46"/>
-      <c r="AC14" s="47"/>
-      <c r="AD14" s="47"/>
-      <c r="AE14" s="47"/>
-      <c r="AF14" s="47"/>
-      <c r="AG14" s="47"/>
-      <c r="AH14" s="47"/>
-      <c r="AI14" s="47"/>
-      <c r="AJ14" s="47"/>
-      <c r="AK14" s="47"/>
-      <c r="AL14" s="46"/>
-      <c r="AM14" s="46"/>
-      <c r="AN14" s="46"/>
-      <c r="AO14" s="46"/>
-      <c r="AP14" s="46"/>
-      <c r="AQ14" s="46"/>
-      <c r="AR14" s="46"/>
-      <c r="AS14" s="46"/>
-      <c r="AT14" s="46"/>
-      <c r="AU14" s="46"/>
-      <c r="AV14" s="46"/>
-      <c r="AW14" s="46"/>
-      <c r="AX14" s="46"/>
-      <c r="AY14" s="46"/>
-      <c r="AZ14" s="46"/>
-      <c r="BA14" s="47"/>
-      <c r="BB14" s="47"/>
-      <c r="BC14" s="47"/>
-      <c r="BD14" s="47"/>
-      <c r="BE14" s="47"/>
-      <c r="BF14" s="47"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="45"/>
+      <c r="M14" s="45"/>
+      <c r="N14" s="45"/>
+      <c r="O14" s="45"/>
+      <c r="P14" s="45"/>
+      <c r="Q14" s="45"/>
+      <c r="R14" s="45"/>
+      <c r="S14" s="45"/>
+      <c r="T14" s="45"/>
+      <c r="U14" s="45"/>
+      <c r="V14" s="45"/>
+      <c r="W14" s="45"/>
+      <c r="X14" s="45"/>
+      <c r="Y14" s="45"/>
+      <c r="Z14" s="45"/>
+      <c r="AA14" s="45"/>
+      <c r="AB14" s="45"/>
+      <c r="AC14" s="46"/>
+      <c r="AD14" s="46"/>
+      <c r="AE14" s="46"/>
+      <c r="AF14" s="46"/>
+      <c r="AG14" s="46"/>
+      <c r="AH14" s="46"/>
+      <c r="AI14" s="46"/>
+      <c r="AJ14" s="46"/>
+      <c r="AK14" s="46"/>
+      <c r="AL14" s="45"/>
+      <c r="AM14" s="45"/>
+      <c r="AN14" s="45"/>
+      <c r="AO14" s="45"/>
+      <c r="AP14" s="45"/>
+      <c r="AQ14" s="45"/>
+      <c r="AR14" s="45"/>
+      <c r="AS14" s="45"/>
+      <c r="AT14" s="45"/>
+      <c r="AU14" s="45"/>
+      <c r="AV14" s="45"/>
+      <c r="AW14" s="45"/>
+      <c r="AX14" s="45"/>
+      <c r="AY14" s="45"/>
+      <c r="AZ14" s="45"/>
+      <c r="BA14" s="46"/>
+      <c r="BB14" s="46"/>
+      <c r="BC14" s="46"/>
+      <c r="BD14" s="46"/>
+      <c r="BE14" s="46"/>
+      <c r="BF14" s="46"/>
       <c r="BG14" s="35"/>
     </row>
     <row r="15" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35"/>
       <c r="B15" s="36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="37" t="s">
         <v>34</v>
@@ -2474,61 +2474,61 @@
         <v>1</v>
       </c>
       <c r="I15" s="41"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="46"/>
-      <c r="L15" s="46"/>
-      <c r="M15" s="46"/>
-      <c r="N15" s="46"/>
-      <c r="O15" s="46"/>
-      <c r="P15" s="46"/>
-      <c r="Q15" s="46"/>
-      <c r="R15" s="46"/>
-      <c r="S15" s="46"/>
-      <c r="T15" s="46"/>
-      <c r="U15" s="46"/>
-      <c r="V15" s="46"/>
-      <c r="W15" s="46"/>
-      <c r="X15" s="46"/>
-      <c r="Y15" s="46"/>
-      <c r="Z15" s="46"/>
-      <c r="AA15" s="46"/>
-      <c r="AB15" s="46"/>
-      <c r="AC15" s="47"/>
-      <c r="AD15" s="47"/>
-      <c r="AE15" s="47"/>
-      <c r="AF15" s="47"/>
-      <c r="AG15" s="47"/>
-      <c r="AH15" s="47"/>
-      <c r="AI15" s="47"/>
-      <c r="AJ15" s="47"/>
-      <c r="AK15" s="47"/>
-      <c r="AL15" s="46"/>
-      <c r="AM15" s="46"/>
-      <c r="AN15" s="46"/>
-      <c r="AO15" s="46"/>
-      <c r="AP15" s="46"/>
-      <c r="AQ15" s="46"/>
-      <c r="AR15" s="46"/>
-      <c r="AS15" s="46"/>
-      <c r="AT15" s="46"/>
-      <c r="AU15" s="46"/>
-      <c r="AV15" s="46"/>
-      <c r="AW15" s="46"/>
-      <c r="AX15" s="46"/>
-      <c r="AY15" s="46"/>
-      <c r="AZ15" s="46"/>
-      <c r="BA15" s="47"/>
-      <c r="BB15" s="47"/>
-      <c r="BC15" s="47"/>
-      <c r="BD15" s="47"/>
-      <c r="BE15" s="47"/>
-      <c r="BF15" s="47"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="45"/>
+      <c r="M15" s="45"/>
+      <c r="N15" s="45"/>
+      <c r="O15" s="45"/>
+      <c r="P15" s="45"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="45"/>
+      <c r="S15" s="45"/>
+      <c r="T15" s="45"/>
+      <c r="U15" s="45"/>
+      <c r="V15" s="45"/>
+      <c r="W15" s="45"/>
+      <c r="X15" s="45"/>
+      <c r="Y15" s="45"/>
+      <c r="Z15" s="45"/>
+      <c r="AA15" s="45"/>
+      <c r="AB15" s="45"/>
+      <c r="AC15" s="46"/>
+      <c r="AD15" s="46"/>
+      <c r="AE15" s="46"/>
+      <c r="AF15" s="46"/>
+      <c r="AG15" s="46"/>
+      <c r="AH15" s="46"/>
+      <c r="AI15" s="46"/>
+      <c r="AJ15" s="46"/>
+      <c r="AK15" s="46"/>
+      <c r="AL15" s="45"/>
+      <c r="AM15" s="45"/>
+      <c r="AN15" s="45"/>
+      <c r="AO15" s="45"/>
+      <c r="AP15" s="45"/>
+      <c r="AQ15" s="45"/>
+      <c r="AR15" s="45"/>
+      <c r="AS15" s="45"/>
+      <c r="AT15" s="45"/>
+      <c r="AU15" s="45"/>
+      <c r="AV15" s="45"/>
+      <c r="AW15" s="45"/>
+      <c r="AX15" s="45"/>
+      <c r="AY15" s="45"/>
+      <c r="AZ15" s="45"/>
+      <c r="BA15" s="46"/>
+      <c r="BB15" s="46"/>
+      <c r="BC15" s="46"/>
+      <c r="BD15" s="46"/>
+      <c r="BE15" s="46"/>
+      <c r="BF15" s="46"/>
       <c r="BG15" s="35"/>
     </row>
     <row r="16" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="35"/>
       <c r="B16" s="36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" s="37" t="s">
         <v>35</v>
@@ -2549,61 +2549,61 @@
         <v>1</v>
       </c>
       <c r="I16" s="41"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="46"/>
-      <c r="L16" s="46"/>
-      <c r="M16" s="46"/>
-      <c r="N16" s="46"/>
-      <c r="O16" s="46"/>
-      <c r="P16" s="46"/>
-      <c r="Q16" s="46"/>
-      <c r="R16" s="46"/>
-      <c r="S16" s="46"/>
-      <c r="T16" s="46"/>
-      <c r="U16" s="46"/>
-      <c r="V16" s="46"/>
-      <c r="W16" s="46"/>
-      <c r="X16" s="46"/>
-      <c r="Y16" s="46"/>
-      <c r="Z16" s="46"/>
-      <c r="AA16" s="46"/>
-      <c r="AB16" s="46"/>
-      <c r="AC16" s="47"/>
-      <c r="AD16" s="47"/>
-      <c r="AE16" s="47"/>
-      <c r="AF16" s="47"/>
-      <c r="AG16" s="47"/>
-      <c r="AH16" s="47"/>
-      <c r="AI16" s="47"/>
-      <c r="AJ16" s="47"/>
-      <c r="AK16" s="47"/>
-      <c r="AL16" s="46"/>
-      <c r="AM16" s="46"/>
-      <c r="AN16" s="46"/>
-      <c r="AO16" s="46"/>
-      <c r="AP16" s="46"/>
-      <c r="AQ16" s="46"/>
-      <c r="AR16" s="46"/>
-      <c r="AS16" s="46"/>
-      <c r="AT16" s="46"/>
-      <c r="AU16" s="46"/>
-      <c r="AV16" s="46"/>
-      <c r="AW16" s="46"/>
-      <c r="AX16" s="46"/>
-      <c r="AY16" s="46"/>
-      <c r="AZ16" s="46"/>
-      <c r="BA16" s="47"/>
-      <c r="BB16" s="47"/>
-      <c r="BC16" s="47"/>
-      <c r="BD16" s="47"/>
-      <c r="BE16" s="47"/>
-      <c r="BF16" s="47"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="45"/>
+      <c r="M16" s="45"/>
+      <c r="N16" s="45"/>
+      <c r="O16" s="45"/>
+      <c r="P16" s="45"/>
+      <c r="Q16" s="45"/>
+      <c r="R16" s="45"/>
+      <c r="S16" s="45"/>
+      <c r="T16" s="45"/>
+      <c r="U16" s="45"/>
+      <c r="V16" s="45"/>
+      <c r="W16" s="45"/>
+      <c r="X16" s="45"/>
+      <c r="Y16" s="45"/>
+      <c r="Z16" s="45"/>
+      <c r="AA16" s="45"/>
+      <c r="AB16" s="45"/>
+      <c r="AC16" s="46"/>
+      <c r="AD16" s="46"/>
+      <c r="AE16" s="46"/>
+      <c r="AF16" s="46"/>
+      <c r="AG16" s="46"/>
+      <c r="AH16" s="46"/>
+      <c r="AI16" s="46"/>
+      <c r="AJ16" s="46"/>
+      <c r="AK16" s="46"/>
+      <c r="AL16" s="45"/>
+      <c r="AM16" s="45"/>
+      <c r="AN16" s="45"/>
+      <c r="AO16" s="45"/>
+      <c r="AP16" s="45"/>
+      <c r="AQ16" s="45"/>
+      <c r="AR16" s="45"/>
+      <c r="AS16" s="45"/>
+      <c r="AT16" s="45"/>
+      <c r="AU16" s="45"/>
+      <c r="AV16" s="45"/>
+      <c r="AW16" s="45"/>
+      <c r="AX16" s="45"/>
+      <c r="AY16" s="45"/>
+      <c r="AZ16" s="45"/>
+      <c r="BA16" s="46"/>
+      <c r="BB16" s="46"/>
+      <c r="BC16" s="46"/>
+      <c r="BD16" s="46"/>
+      <c r="BE16" s="46"/>
+      <c r="BF16" s="46"/>
       <c r="BG16" s="35"/>
     </row>
     <row r="17" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="35"/>
       <c r="B17" s="36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="37" t="s">
         <v>37</v>
@@ -2620,68 +2620,68 @@
       <c r="G17" s="39">
         <v>1</v>
       </c>
-      <c r="H17" s="49">
+      <c r="H17" s="48">
         <v>1</v>
       </c>
       <c r="I17" s="41"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="46"/>
-      <c r="L17" s="46"/>
-      <c r="M17" s="46"/>
-      <c r="N17" s="46"/>
-      <c r="O17" s="46"/>
-      <c r="P17" s="46"/>
-      <c r="Q17" s="46"/>
-      <c r="R17" s="46"/>
-      <c r="S17" s="46"/>
-      <c r="T17" s="46"/>
-      <c r="U17" s="46"/>
-      <c r="V17" s="46"/>
-      <c r="W17" s="46"/>
-      <c r="X17" s="46"/>
-      <c r="Y17" s="46"/>
-      <c r="Z17" s="46"/>
-      <c r="AA17" s="46"/>
-      <c r="AB17" s="46"/>
-      <c r="AC17" s="47"/>
-      <c r="AD17" s="47"/>
-      <c r="AE17" s="47"/>
-      <c r="AF17" s="47"/>
-      <c r="AG17" s="47"/>
-      <c r="AH17" s="47"/>
-      <c r="AI17" s="47"/>
-      <c r="AJ17" s="47"/>
-      <c r="AK17" s="47"/>
-      <c r="AL17" s="46"/>
-      <c r="AM17" s="46"/>
-      <c r="AN17" s="46"/>
-      <c r="AO17" s="46"/>
-      <c r="AP17" s="46"/>
-      <c r="AQ17" s="46"/>
-      <c r="AR17" s="46"/>
-      <c r="AS17" s="46"/>
-      <c r="AT17" s="46"/>
-      <c r="AU17" s="46"/>
-      <c r="AV17" s="46"/>
-      <c r="AW17" s="46"/>
-      <c r="AX17" s="46"/>
-      <c r="AY17" s="46"/>
-      <c r="AZ17" s="46"/>
-      <c r="BA17" s="47"/>
-      <c r="BB17" s="47"/>
-      <c r="BC17" s="47"/>
-      <c r="BD17" s="47"/>
-      <c r="BE17" s="47"/>
-      <c r="BF17" s="47"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="45"/>
+      <c r="M17" s="45"/>
+      <c r="N17" s="45"/>
+      <c r="O17" s="45"/>
+      <c r="P17" s="45"/>
+      <c r="Q17" s="45"/>
+      <c r="R17" s="45"/>
+      <c r="S17" s="45"/>
+      <c r="T17" s="45"/>
+      <c r="U17" s="45"/>
+      <c r="V17" s="45"/>
+      <c r="W17" s="45"/>
+      <c r="X17" s="45"/>
+      <c r="Y17" s="45"/>
+      <c r="Z17" s="45"/>
+      <c r="AA17" s="45"/>
+      <c r="AB17" s="45"/>
+      <c r="AC17" s="46"/>
+      <c r="AD17" s="46"/>
+      <c r="AE17" s="46"/>
+      <c r="AF17" s="46"/>
+      <c r="AG17" s="46"/>
+      <c r="AH17" s="46"/>
+      <c r="AI17" s="46"/>
+      <c r="AJ17" s="46"/>
+      <c r="AK17" s="46"/>
+      <c r="AL17" s="45"/>
+      <c r="AM17" s="45"/>
+      <c r="AN17" s="45"/>
+      <c r="AO17" s="45"/>
+      <c r="AP17" s="45"/>
+      <c r="AQ17" s="45"/>
+      <c r="AR17" s="45"/>
+      <c r="AS17" s="45"/>
+      <c r="AT17" s="45"/>
+      <c r="AU17" s="45"/>
+      <c r="AV17" s="45"/>
+      <c r="AW17" s="45"/>
+      <c r="AX17" s="45"/>
+      <c r="AY17" s="45"/>
+      <c r="AZ17" s="45"/>
+      <c r="BA17" s="46"/>
+      <c r="BB17" s="46"/>
+      <c r="BC17" s="46"/>
+      <c r="BD17" s="46"/>
+      <c r="BE17" s="46"/>
+      <c r="BF17" s="46"/>
       <c r="BG17" s="35"/>
     </row>
     <row r="18" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="35"/>
       <c r="B18" s="36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D18" s="37" t="s">
         <v>38</v>
@@ -2701,59 +2701,59 @@
       <c r="I18" s="41"/>
       <c r="J18" s="41"/>
       <c r="K18" s="41"/>
-      <c r="L18" s="46"/>
-      <c r="M18" s="46"/>
-      <c r="N18" s="46"/>
-      <c r="O18" s="46"/>
-      <c r="P18" s="46"/>
-      <c r="Q18" s="46"/>
-      <c r="R18" s="46"/>
-      <c r="S18" s="46"/>
-      <c r="T18" s="46"/>
-      <c r="U18" s="46"/>
-      <c r="V18" s="46"/>
-      <c r="W18" s="46"/>
-      <c r="X18" s="46"/>
-      <c r="Y18" s="46"/>
-      <c r="Z18" s="46"/>
-      <c r="AA18" s="46"/>
-      <c r="AB18" s="46"/>
-      <c r="AC18" s="47"/>
-      <c r="AD18" s="47"/>
-      <c r="AE18" s="47"/>
-      <c r="AF18" s="47"/>
-      <c r="AG18" s="47"/>
-      <c r="AH18" s="47"/>
-      <c r="AI18" s="47"/>
-      <c r="AJ18" s="47"/>
-      <c r="AK18" s="47"/>
-      <c r="AL18" s="46"/>
-      <c r="AM18" s="46"/>
-      <c r="AN18" s="46"/>
-      <c r="AO18" s="46"/>
-      <c r="AP18" s="46"/>
-      <c r="AQ18" s="46"/>
-      <c r="AR18" s="46"/>
-      <c r="AS18" s="46"/>
-      <c r="AT18" s="46"/>
-      <c r="AU18" s="46"/>
-      <c r="AV18" s="46"/>
-      <c r="AW18" s="46"/>
-      <c r="AX18" s="46"/>
-      <c r="AY18" s="46"/>
-      <c r="AZ18" s="46"/>
-      <c r="BA18" s="47"/>
-      <c r="BB18" s="47"/>
-      <c r="BC18" s="47"/>
-      <c r="BD18" s="47"/>
-      <c r="BE18" s="47"/>
-      <c r="BF18" s="47"/>
+      <c r="L18" s="45"/>
+      <c r="M18" s="45"/>
+      <c r="N18" s="45"/>
+      <c r="O18" s="45"/>
+      <c r="P18" s="45"/>
+      <c r="Q18" s="45"/>
+      <c r="R18" s="45"/>
+      <c r="S18" s="45"/>
+      <c r="T18" s="45"/>
+      <c r="U18" s="45"/>
+      <c r="V18" s="45"/>
+      <c r="W18" s="45"/>
+      <c r="X18" s="45"/>
+      <c r="Y18" s="45"/>
+      <c r="Z18" s="45"/>
+      <c r="AA18" s="45"/>
+      <c r="AB18" s="45"/>
+      <c r="AC18" s="46"/>
+      <c r="AD18" s="46"/>
+      <c r="AE18" s="46"/>
+      <c r="AF18" s="46"/>
+      <c r="AG18" s="46"/>
+      <c r="AH18" s="46"/>
+      <c r="AI18" s="46"/>
+      <c r="AJ18" s="46"/>
+      <c r="AK18" s="46"/>
+      <c r="AL18" s="45"/>
+      <c r="AM18" s="45"/>
+      <c r="AN18" s="45"/>
+      <c r="AO18" s="45"/>
+      <c r="AP18" s="45"/>
+      <c r="AQ18" s="45"/>
+      <c r="AR18" s="45"/>
+      <c r="AS18" s="45"/>
+      <c r="AT18" s="45"/>
+      <c r="AU18" s="45"/>
+      <c r="AV18" s="45"/>
+      <c r="AW18" s="45"/>
+      <c r="AX18" s="45"/>
+      <c r="AY18" s="45"/>
+      <c r="AZ18" s="45"/>
+      <c r="BA18" s="46"/>
+      <c r="BB18" s="46"/>
+      <c r="BC18" s="46"/>
+      <c r="BD18" s="46"/>
+      <c r="BE18" s="46"/>
+      <c r="BF18" s="46"/>
       <c r="BG18" s="35"/>
     </row>
     <row r="19" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="35"/>
       <c r="B19" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="37" t="s">
         <v>39</v>
@@ -2774,61 +2774,61 @@
         <v>1</v>
       </c>
       <c r="I19" s="41"/>
-      <c r="J19" s="46"/>
-      <c r="K19" s="46"/>
-      <c r="L19" s="46"/>
-      <c r="M19" s="46"/>
-      <c r="N19" s="46"/>
-      <c r="O19" s="46"/>
-      <c r="P19" s="46"/>
-      <c r="Q19" s="46"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="45"/>
+      <c r="M19" s="45"/>
+      <c r="N19" s="45"/>
+      <c r="O19" s="45"/>
+      <c r="P19" s="45"/>
+      <c r="Q19" s="45"/>
       <c r="R19" s="41"/>
       <c r="S19" s="41"/>
-      <c r="T19" s="46"/>
-      <c r="U19" s="46"/>
-      <c r="V19" s="46"/>
-      <c r="W19" s="46"/>
-      <c r="X19" s="46"/>
-      <c r="Y19" s="46"/>
-      <c r="Z19" s="46"/>
-      <c r="AA19" s="46"/>
-      <c r="AB19" s="46"/>
-      <c r="AC19" s="47"/>
-      <c r="AD19" s="47"/>
-      <c r="AE19" s="47"/>
-      <c r="AF19" s="47"/>
-      <c r="AG19" s="47"/>
-      <c r="AH19" s="47"/>
-      <c r="AI19" s="47"/>
-      <c r="AJ19" s="47"/>
-      <c r="AK19" s="47"/>
-      <c r="AL19" s="46"/>
-      <c r="AM19" s="46"/>
-      <c r="AN19" s="46"/>
-      <c r="AO19" s="46"/>
-      <c r="AP19" s="46"/>
-      <c r="AQ19" s="46"/>
-      <c r="AR19" s="46"/>
-      <c r="AS19" s="46"/>
-      <c r="AT19" s="46"/>
-      <c r="AU19" s="46"/>
-      <c r="AV19" s="46"/>
-      <c r="AW19" s="46"/>
-      <c r="AX19" s="46"/>
-      <c r="AY19" s="46"/>
-      <c r="AZ19" s="46"/>
-      <c r="BA19" s="47"/>
-      <c r="BB19" s="47"/>
-      <c r="BC19" s="47"/>
-      <c r="BD19" s="47"/>
-      <c r="BE19" s="47"/>
-      <c r="BF19" s="47"/>
+      <c r="T19" s="45"/>
+      <c r="U19" s="45"/>
+      <c r="V19" s="45"/>
+      <c r="W19" s="45"/>
+      <c r="X19" s="45"/>
+      <c r="Y19" s="45"/>
+      <c r="Z19" s="45"/>
+      <c r="AA19" s="45"/>
+      <c r="AB19" s="45"/>
+      <c r="AC19" s="46"/>
+      <c r="AD19" s="46"/>
+      <c r="AE19" s="46"/>
+      <c r="AF19" s="46"/>
+      <c r="AG19" s="46"/>
+      <c r="AH19" s="46"/>
+      <c r="AI19" s="46"/>
+      <c r="AJ19" s="46"/>
+      <c r="AK19" s="46"/>
+      <c r="AL19" s="45"/>
+      <c r="AM19" s="45"/>
+      <c r="AN19" s="45"/>
+      <c r="AO19" s="45"/>
+      <c r="AP19" s="45"/>
+      <c r="AQ19" s="45"/>
+      <c r="AR19" s="45"/>
+      <c r="AS19" s="45"/>
+      <c r="AT19" s="45"/>
+      <c r="AU19" s="45"/>
+      <c r="AV19" s="45"/>
+      <c r="AW19" s="45"/>
+      <c r="AX19" s="45"/>
+      <c r="AY19" s="45"/>
+      <c r="AZ19" s="45"/>
+      <c r="BA19" s="46"/>
+      <c r="BB19" s="46"/>
+      <c r="BC19" s="46"/>
+      <c r="BD19" s="46"/>
+      <c r="BE19" s="46"/>
+      <c r="BF19" s="46"/>
       <c r="BG19" s="35"/>
     </row>
     <row r="20" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" s="35"/>
       <c r="B20" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C20" s="37" t="s">
         <v>51</v>
@@ -2848,7 +2848,7 @@
       <c r="H20" s="40">
         <v>1</v>
       </c>
-      <c r="I20" s="50"/>
+      <c r="I20" s="49"/>
       <c r="J20" s="41"/>
       <c r="K20" s="41"/>
       <c r="L20" s="41"/>
@@ -2856,48 +2856,48 @@
       <c r="N20" s="41"/>
       <c r="O20" s="41"/>
       <c r="P20" s="41"/>
-      <c r="Q20" s="51"/>
-      <c r="R20" s="51"/>
-      <c r="S20" s="51"/>
-      <c r="T20" s="51"/>
-      <c r="U20" s="51"/>
-      <c r="V20" s="51"/>
-      <c r="W20" s="51"/>
-      <c r="X20" s="51"/>
-      <c r="Y20" s="51"/>
-      <c r="Z20" s="51"/>
-      <c r="AA20" s="51"/>
-      <c r="AB20" s="51"/>
-      <c r="AC20" s="52"/>
-      <c r="AD20" s="52"/>
-      <c r="AE20" s="52"/>
-      <c r="AF20" s="52"/>
-      <c r="AG20" s="52"/>
-      <c r="AH20" s="52"/>
-      <c r="AI20" s="52"/>
-      <c r="AJ20" s="52"/>
-      <c r="AK20" s="52"/>
-      <c r="AL20" s="51"/>
-      <c r="AM20" s="51"/>
-      <c r="AN20" s="51"/>
-      <c r="AO20" s="51"/>
-      <c r="AP20" s="51"/>
-      <c r="AQ20" s="51"/>
-      <c r="AR20" s="51"/>
-      <c r="AS20" s="51"/>
-      <c r="AT20" s="51"/>
-      <c r="AU20" s="51"/>
-      <c r="AV20" s="51"/>
-      <c r="AW20" s="51"/>
-      <c r="AX20" s="51"/>
-      <c r="AY20" s="51"/>
-      <c r="AZ20" s="51"/>
-      <c r="BA20" s="52"/>
-      <c r="BB20" s="52"/>
-      <c r="BC20" s="52"/>
-      <c r="BD20" s="52"/>
-      <c r="BE20" s="52"/>
-      <c r="BF20" s="52"/>
+      <c r="Q20" s="50"/>
+      <c r="R20" s="50"/>
+      <c r="S20" s="50"/>
+      <c r="T20" s="50"/>
+      <c r="U20" s="50"/>
+      <c r="V20" s="50"/>
+      <c r="W20" s="50"/>
+      <c r="X20" s="50"/>
+      <c r="Y20" s="50"/>
+      <c r="Z20" s="50"/>
+      <c r="AA20" s="50"/>
+      <c r="AB20" s="50"/>
+      <c r="AC20" s="51"/>
+      <c r="AD20" s="51"/>
+      <c r="AE20" s="51"/>
+      <c r="AF20" s="51"/>
+      <c r="AG20" s="51"/>
+      <c r="AH20" s="51"/>
+      <c r="AI20" s="51"/>
+      <c r="AJ20" s="51"/>
+      <c r="AK20" s="51"/>
+      <c r="AL20" s="50"/>
+      <c r="AM20" s="50"/>
+      <c r="AN20" s="50"/>
+      <c r="AO20" s="50"/>
+      <c r="AP20" s="50"/>
+      <c r="AQ20" s="50"/>
+      <c r="AR20" s="50"/>
+      <c r="AS20" s="50"/>
+      <c r="AT20" s="50"/>
+      <c r="AU20" s="50"/>
+      <c r="AV20" s="50"/>
+      <c r="AW20" s="50"/>
+      <c r="AX20" s="50"/>
+      <c r="AY20" s="50"/>
+      <c r="AZ20" s="50"/>
+      <c r="BA20" s="51"/>
+      <c r="BB20" s="51"/>
+      <c r="BC20" s="51"/>
+      <c r="BD20" s="51"/>
+      <c r="BE20" s="51"/>
+      <c r="BF20" s="51"/>
       <c r="BG20" s="35"/>
     </row>
     <row r="21" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2921,58 +2921,58 @@
         <v>3</v>
       </c>
       <c r="H21" s="40">
-        <v>0</v>
-      </c>
-      <c r="I21" s="50"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="51"/>
-      <c r="L21" s="51"/>
-      <c r="M21" s="51"/>
-      <c r="N21" s="51"/>
-      <c r="O21" s="51"/>
-      <c r="P21" s="51"/>
-      <c r="Q21" s="42"/>
-      <c r="R21" s="42"/>
-      <c r="S21" s="42"/>
-      <c r="T21" s="51"/>
-      <c r="U21" s="51"/>
-      <c r="V21" s="51"/>
-      <c r="W21" s="51"/>
-      <c r="X21" s="51"/>
-      <c r="Y21" s="51"/>
-      <c r="Z21" s="51"/>
-      <c r="AA21" s="51"/>
-      <c r="AB21" s="51"/>
-      <c r="AC21" s="52"/>
-      <c r="AD21" s="52"/>
-      <c r="AE21" s="52"/>
-      <c r="AF21" s="52"/>
-      <c r="AG21" s="52"/>
-      <c r="AH21" s="52"/>
-      <c r="AI21" s="52"/>
-      <c r="AJ21" s="52"/>
-      <c r="AK21" s="52"/>
-      <c r="AL21" s="51"/>
-      <c r="AM21" s="51"/>
-      <c r="AN21" s="51"/>
-      <c r="AO21" s="51"/>
-      <c r="AP21" s="51"/>
-      <c r="AQ21" s="51"/>
-      <c r="AR21" s="51"/>
-      <c r="AS21" s="51"/>
-      <c r="AT21" s="51"/>
-      <c r="AU21" s="51"/>
-      <c r="AV21" s="51"/>
-      <c r="AW21" s="51"/>
-      <c r="AX21" s="51"/>
-      <c r="AY21" s="51"/>
-      <c r="AZ21" s="51"/>
-      <c r="BA21" s="52"/>
-      <c r="BB21" s="52"/>
-      <c r="BC21" s="52"/>
-      <c r="BD21" s="52"/>
-      <c r="BE21" s="52"/>
-      <c r="BF21" s="52"/>
+        <v>1</v>
+      </c>
+      <c r="I21" s="49"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="50"/>
+      <c r="N21" s="50"/>
+      <c r="O21" s="50"/>
+      <c r="P21" s="50"/>
+      <c r="Q21" s="41"/>
+      <c r="R21" s="41"/>
+      <c r="S21" s="41"/>
+      <c r="T21" s="50"/>
+      <c r="U21" s="50"/>
+      <c r="V21" s="50"/>
+      <c r="W21" s="50"/>
+      <c r="X21" s="50"/>
+      <c r="Y21" s="50"/>
+      <c r="Z21" s="50"/>
+      <c r="AA21" s="50"/>
+      <c r="AB21" s="50"/>
+      <c r="AC21" s="51"/>
+      <c r="AD21" s="51"/>
+      <c r="AE21" s="51"/>
+      <c r="AF21" s="51"/>
+      <c r="AG21" s="51"/>
+      <c r="AH21" s="51"/>
+      <c r="AI21" s="51"/>
+      <c r="AJ21" s="51"/>
+      <c r="AK21" s="51"/>
+      <c r="AL21" s="50"/>
+      <c r="AM21" s="50"/>
+      <c r="AN21" s="50"/>
+      <c r="AO21" s="50"/>
+      <c r="AP21" s="50"/>
+      <c r="AQ21" s="50"/>
+      <c r="AR21" s="50"/>
+      <c r="AS21" s="50"/>
+      <c r="AT21" s="50"/>
+      <c r="AU21" s="50"/>
+      <c r="AV21" s="50"/>
+      <c r="AW21" s="50"/>
+      <c r="AX21" s="50"/>
+      <c r="AY21" s="50"/>
+      <c r="AZ21" s="50"/>
+      <c r="BA21" s="51"/>
+      <c r="BB21" s="51"/>
+      <c r="BC21" s="51"/>
+      <c r="BD21" s="51"/>
+      <c r="BE21" s="51"/>
+      <c r="BF21" s="51"/>
       <c r="BG21" s="35"/>
     </row>
     <row r="22" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2998,56 +2998,56 @@
       <c r="H22" s="40">
         <v>1</v>
       </c>
-      <c r="I22" s="50"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="51"/>
-      <c r="L22" s="51"/>
-      <c r="M22" s="51"/>
-      <c r="N22" s="51"/>
-      <c r="O22" s="51"/>
-      <c r="P22" s="51"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="50"/>
+      <c r="L22" s="50"/>
+      <c r="M22" s="50"/>
+      <c r="N22" s="50"/>
+      <c r="O22" s="50"/>
+      <c r="P22" s="50"/>
       <c r="Q22" s="41"/>
       <c r="R22" s="41"/>
       <c r="S22" s="41"/>
-      <c r="T22" s="51"/>
-      <c r="U22" s="51"/>
-      <c r="V22" s="51"/>
-      <c r="W22" s="51"/>
-      <c r="X22" s="51"/>
-      <c r="Y22" s="51"/>
-      <c r="Z22" s="51"/>
-      <c r="AA22" s="51"/>
-      <c r="AB22" s="51"/>
-      <c r="AC22" s="52"/>
-      <c r="AD22" s="52"/>
-      <c r="AE22" s="52"/>
-      <c r="AF22" s="52"/>
-      <c r="AG22" s="52"/>
-      <c r="AH22" s="52"/>
-      <c r="AI22" s="52"/>
-      <c r="AJ22" s="52"/>
-      <c r="AK22" s="52"/>
-      <c r="AL22" s="51"/>
-      <c r="AM22" s="51"/>
-      <c r="AN22" s="51"/>
-      <c r="AO22" s="51"/>
-      <c r="AP22" s="51"/>
-      <c r="AQ22" s="51"/>
-      <c r="AR22" s="51"/>
-      <c r="AS22" s="51"/>
-      <c r="AT22" s="51"/>
-      <c r="AU22" s="51"/>
-      <c r="AV22" s="51"/>
-      <c r="AW22" s="51"/>
-      <c r="AX22" s="51"/>
-      <c r="AY22" s="51"/>
-      <c r="AZ22" s="51"/>
-      <c r="BA22" s="52"/>
-      <c r="BB22" s="52"/>
-      <c r="BC22" s="52"/>
-      <c r="BD22" s="52"/>
-      <c r="BE22" s="52"/>
-      <c r="BF22" s="52"/>
+      <c r="T22" s="50"/>
+      <c r="U22" s="50"/>
+      <c r="V22" s="50"/>
+      <c r="W22" s="50"/>
+      <c r="X22" s="50"/>
+      <c r="Y22" s="50"/>
+      <c r="Z22" s="50"/>
+      <c r="AA22" s="50"/>
+      <c r="AB22" s="50"/>
+      <c r="AC22" s="51"/>
+      <c r="AD22" s="51"/>
+      <c r="AE22" s="51"/>
+      <c r="AF22" s="51"/>
+      <c r="AG22" s="51"/>
+      <c r="AH22" s="51"/>
+      <c r="AI22" s="51"/>
+      <c r="AJ22" s="51"/>
+      <c r="AK22" s="51"/>
+      <c r="AL22" s="50"/>
+      <c r="AM22" s="50"/>
+      <c r="AN22" s="50"/>
+      <c r="AO22" s="50"/>
+      <c r="AP22" s="50"/>
+      <c r="AQ22" s="50"/>
+      <c r="AR22" s="50"/>
+      <c r="AS22" s="50"/>
+      <c r="AT22" s="50"/>
+      <c r="AU22" s="50"/>
+      <c r="AV22" s="50"/>
+      <c r="AW22" s="50"/>
+      <c r="AX22" s="50"/>
+      <c r="AY22" s="50"/>
+      <c r="AZ22" s="50"/>
+      <c r="BA22" s="51"/>
+      <c r="BB22" s="51"/>
+      <c r="BC22" s="51"/>
+      <c r="BD22" s="51"/>
+      <c r="BE22" s="51"/>
+      <c r="BF22" s="51"/>
       <c r="BG22" s="35"/>
     </row>
     <row r="23" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3073,62 +3073,62 @@
       <c r="H23" s="40">
         <v>1</v>
       </c>
-      <c r="I23" s="50"/>
-      <c r="J23" s="51"/>
-      <c r="K23" s="51"/>
-      <c r="L23" s="51"/>
-      <c r="M23" s="51"/>
-      <c r="N23" s="51"/>
-      <c r="O23" s="51"/>
-      <c r="P23" s="51"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="50"/>
+      <c r="O23" s="50"/>
+      <c r="P23" s="50"/>
       <c r="Q23" s="41"/>
       <c r="R23" s="41"/>
       <c r="S23" s="41"/>
-      <c r="T23" s="51"/>
-      <c r="U23" s="51"/>
-      <c r="V23" s="51"/>
-      <c r="W23" s="51"/>
-      <c r="X23" s="51"/>
-      <c r="Y23" s="51"/>
-      <c r="Z23" s="51"/>
-      <c r="AA23" s="51"/>
-      <c r="AB23" s="51"/>
-      <c r="AC23" s="52"/>
-      <c r="AD23" s="52"/>
-      <c r="AE23" s="52"/>
-      <c r="AF23" s="52"/>
-      <c r="AG23" s="52"/>
-      <c r="AH23" s="52"/>
-      <c r="AI23" s="52"/>
-      <c r="AJ23" s="52"/>
-      <c r="AK23" s="52"/>
-      <c r="AL23" s="51"/>
-      <c r="AM23" s="51"/>
-      <c r="AN23" s="51"/>
-      <c r="AO23" s="51"/>
-      <c r="AP23" s="51"/>
-      <c r="AQ23" s="51"/>
-      <c r="AR23" s="51"/>
-      <c r="AS23" s="51"/>
-      <c r="AT23" s="51"/>
-      <c r="AU23" s="51"/>
-      <c r="AV23" s="51"/>
-      <c r="AW23" s="51"/>
-      <c r="AX23" s="51"/>
-      <c r="AY23" s="51"/>
-      <c r="AZ23" s="51"/>
-      <c r="BA23" s="52"/>
-      <c r="BB23" s="52"/>
-      <c r="BC23" s="52"/>
-      <c r="BD23" s="52"/>
-      <c r="BE23" s="52"/>
-      <c r="BF23" s="52"/>
+      <c r="T23" s="50"/>
+      <c r="U23" s="50"/>
+      <c r="V23" s="50"/>
+      <c r="W23" s="50"/>
+      <c r="X23" s="50"/>
+      <c r="Y23" s="50"/>
+      <c r="Z23" s="50"/>
+      <c r="AA23" s="50"/>
+      <c r="AB23" s="50"/>
+      <c r="AC23" s="51"/>
+      <c r="AD23" s="51"/>
+      <c r="AE23" s="51"/>
+      <c r="AF23" s="51"/>
+      <c r="AG23" s="51"/>
+      <c r="AH23" s="51"/>
+      <c r="AI23" s="51"/>
+      <c r="AJ23" s="51"/>
+      <c r="AK23" s="51"/>
+      <c r="AL23" s="50"/>
+      <c r="AM23" s="50"/>
+      <c r="AN23" s="50"/>
+      <c r="AO23" s="50"/>
+      <c r="AP23" s="50"/>
+      <c r="AQ23" s="50"/>
+      <c r="AR23" s="50"/>
+      <c r="AS23" s="50"/>
+      <c r="AT23" s="50"/>
+      <c r="AU23" s="50"/>
+      <c r="AV23" s="50"/>
+      <c r="AW23" s="50"/>
+      <c r="AX23" s="50"/>
+      <c r="AY23" s="50"/>
+      <c r="AZ23" s="50"/>
+      <c r="BA23" s="51"/>
+      <c r="BB23" s="51"/>
+      <c r="BC23" s="51"/>
+      <c r="BD23" s="51"/>
+      <c r="BE23" s="51"/>
+      <c r="BF23" s="51"/>
       <c r="BG23" s="35"/>
     </row>
     <row r="24" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="35"/>
       <c r="B24" s="36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" s="37" t="s">
         <v>43</v>
@@ -3149,61 +3149,61 @@
         <v>1</v>
       </c>
       <c r="I24" s="41"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="51"/>
-      <c r="L24" s="51"/>
-      <c r="M24" s="51"/>
-      <c r="N24" s="51"/>
-      <c r="O24" s="51"/>
-      <c r="P24" s="51"/>
-      <c r="Q24" s="51"/>
-      <c r="R24" s="51"/>
-      <c r="S24" s="51"/>
-      <c r="T24" s="51"/>
-      <c r="U24" s="51"/>
-      <c r="V24" s="51"/>
-      <c r="W24" s="51"/>
-      <c r="X24" s="51"/>
-      <c r="Y24" s="51"/>
-      <c r="Z24" s="51"/>
-      <c r="AA24" s="51"/>
-      <c r="AB24" s="51"/>
-      <c r="AC24" s="52"/>
-      <c r="AD24" s="52"/>
-      <c r="AE24" s="52"/>
-      <c r="AF24" s="52"/>
-      <c r="AG24" s="52"/>
-      <c r="AH24" s="52"/>
-      <c r="AI24" s="52"/>
-      <c r="AJ24" s="52"/>
-      <c r="AK24" s="52"/>
-      <c r="AL24" s="51"/>
-      <c r="AM24" s="51"/>
-      <c r="AN24" s="51"/>
-      <c r="AO24" s="51"/>
-      <c r="AP24" s="51"/>
-      <c r="AQ24" s="51"/>
-      <c r="AR24" s="51"/>
-      <c r="AS24" s="51"/>
-      <c r="AT24" s="51"/>
-      <c r="AU24" s="51"/>
-      <c r="AV24" s="51"/>
-      <c r="AW24" s="51"/>
-      <c r="AX24" s="51"/>
-      <c r="AY24" s="51"/>
-      <c r="AZ24" s="51"/>
-      <c r="BA24" s="52"/>
-      <c r="BB24" s="52"/>
-      <c r="BC24" s="52"/>
-      <c r="BD24" s="52"/>
-      <c r="BE24" s="52"/>
-      <c r="BF24" s="52"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="50"/>
+      <c r="L24" s="50"/>
+      <c r="M24" s="50"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="50"/>
+      <c r="P24" s="50"/>
+      <c r="Q24" s="50"/>
+      <c r="R24" s="50"/>
+      <c r="S24" s="50"/>
+      <c r="T24" s="50"/>
+      <c r="U24" s="50"/>
+      <c r="V24" s="50"/>
+      <c r="W24" s="50"/>
+      <c r="X24" s="50"/>
+      <c r="Y24" s="50"/>
+      <c r="Z24" s="50"/>
+      <c r="AA24" s="50"/>
+      <c r="AB24" s="50"/>
+      <c r="AC24" s="51"/>
+      <c r="AD24" s="51"/>
+      <c r="AE24" s="51"/>
+      <c r="AF24" s="51"/>
+      <c r="AG24" s="51"/>
+      <c r="AH24" s="51"/>
+      <c r="AI24" s="51"/>
+      <c r="AJ24" s="51"/>
+      <c r="AK24" s="51"/>
+      <c r="AL24" s="50"/>
+      <c r="AM24" s="50"/>
+      <c r="AN24" s="50"/>
+      <c r="AO24" s="50"/>
+      <c r="AP24" s="50"/>
+      <c r="AQ24" s="50"/>
+      <c r="AR24" s="50"/>
+      <c r="AS24" s="50"/>
+      <c r="AT24" s="50"/>
+      <c r="AU24" s="50"/>
+      <c r="AV24" s="50"/>
+      <c r="AW24" s="50"/>
+      <c r="AX24" s="50"/>
+      <c r="AY24" s="50"/>
+      <c r="AZ24" s="50"/>
+      <c r="BA24" s="51"/>
+      <c r="BB24" s="51"/>
+      <c r="BC24" s="51"/>
+      <c r="BD24" s="51"/>
+      <c r="BE24" s="51"/>
+      <c r="BF24" s="51"/>
       <c r="BG24" s="35"/>
     </row>
     <row r="25" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="35"/>
       <c r="B25" s="36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25" s="37" t="s">
         <v>44</v>
@@ -3221,70 +3221,70 @@
         <v>2</v>
       </c>
       <c r="H25" s="40">
-        <v>0</v>
-      </c>
-      <c r="I25" s="50"/>
+        <v>1</v>
+      </c>
+      <c r="I25" s="49"/>
       <c r="J25" s="41"/>
       <c r="K25" s="41"/>
-      <c r="L25" s="51"/>
-      <c r="M25" s="51"/>
-      <c r="N25" s="51"/>
-      <c r="O25" s="51"/>
-      <c r="P25" s="51"/>
-      <c r="Q25" s="51"/>
-      <c r="R25" s="51"/>
-      <c r="S25" s="51"/>
-      <c r="T25" s="51"/>
-      <c r="U25" s="51"/>
-      <c r="V25" s="51"/>
-      <c r="W25" s="51"/>
-      <c r="X25" s="51"/>
-      <c r="Y25" s="51"/>
-      <c r="Z25" s="51"/>
-      <c r="AA25" s="51"/>
-      <c r="AB25" s="51"/>
-      <c r="AC25" s="52"/>
-      <c r="AD25" s="52"/>
-      <c r="AE25" s="52"/>
-      <c r="AF25" s="52"/>
-      <c r="AG25" s="52"/>
-      <c r="AH25" s="52"/>
-      <c r="AI25" s="52"/>
-      <c r="AJ25" s="52"/>
-      <c r="AK25" s="52"/>
-      <c r="AL25" s="51"/>
-      <c r="AM25" s="51"/>
-      <c r="AN25" s="51"/>
-      <c r="AO25" s="51"/>
-      <c r="AP25" s="51"/>
-      <c r="AQ25" s="51"/>
-      <c r="AR25" s="51"/>
-      <c r="AS25" s="51"/>
-      <c r="AT25" s="51"/>
-      <c r="AU25" s="51"/>
-      <c r="AV25" s="51"/>
-      <c r="AW25" s="51"/>
-      <c r="AX25" s="51"/>
-      <c r="AY25" s="51"/>
-      <c r="AZ25" s="51"/>
-      <c r="BA25" s="52"/>
-      <c r="BB25" s="52"/>
-      <c r="BC25" s="52"/>
-      <c r="BD25" s="52"/>
-      <c r="BE25" s="52"/>
-      <c r="BF25" s="52"/>
+      <c r="L25" s="50"/>
+      <c r="M25" s="50"/>
+      <c r="N25" s="50"/>
+      <c r="O25" s="50"/>
+      <c r="P25" s="50"/>
+      <c r="Q25" s="50"/>
+      <c r="R25" s="50"/>
+      <c r="S25" s="50"/>
+      <c r="T25" s="50"/>
+      <c r="U25" s="50"/>
+      <c r="V25" s="50"/>
+      <c r="W25" s="50"/>
+      <c r="X25" s="50"/>
+      <c r="Y25" s="50"/>
+      <c r="Z25" s="50"/>
+      <c r="AA25" s="50"/>
+      <c r="AB25" s="50"/>
+      <c r="AC25" s="51"/>
+      <c r="AD25" s="51"/>
+      <c r="AE25" s="51"/>
+      <c r="AF25" s="51"/>
+      <c r="AG25" s="51"/>
+      <c r="AH25" s="51"/>
+      <c r="AI25" s="51"/>
+      <c r="AJ25" s="51"/>
+      <c r="AK25" s="51"/>
+      <c r="AL25" s="50"/>
+      <c r="AM25" s="50"/>
+      <c r="AN25" s="50"/>
+      <c r="AO25" s="50"/>
+      <c r="AP25" s="50"/>
+      <c r="AQ25" s="50"/>
+      <c r="AR25" s="50"/>
+      <c r="AS25" s="50"/>
+      <c r="AT25" s="50"/>
+      <c r="AU25" s="50"/>
+      <c r="AV25" s="50"/>
+      <c r="AW25" s="50"/>
+      <c r="AX25" s="50"/>
+      <c r="AY25" s="50"/>
+      <c r="AZ25" s="50"/>
+      <c r="BA25" s="51"/>
+      <c r="BB25" s="51"/>
+      <c r="BC25" s="51"/>
+      <c r="BD25" s="51"/>
+      <c r="BE25" s="51"/>
+      <c r="BF25" s="51"/>
       <c r="BG25" s="35"/>
     </row>
     <row r="26" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="35"/>
       <c r="B26" s="36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C26" s="37" t="s">
         <v>45</v>
       </c>
       <c r="D26" s="37" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E26" s="38">
         <v>45732</v>
@@ -3296,70 +3296,70 @@
         <v>1</v>
       </c>
       <c r="H26" s="40">
-        <v>0</v>
-      </c>
-      <c r="I26" s="50"/>
-      <c r="J26" s="51"/>
-      <c r="K26" s="42"/>
-      <c r="L26" s="51"/>
-      <c r="M26" s="51"/>
-      <c r="N26" s="51"/>
-      <c r="O26" s="51"/>
-      <c r="P26" s="51"/>
-      <c r="Q26" s="51"/>
-      <c r="R26" s="51"/>
-      <c r="S26" s="51"/>
-      <c r="T26" s="51"/>
-      <c r="U26" s="51"/>
-      <c r="V26" s="51"/>
-      <c r="W26" s="51"/>
-      <c r="X26" s="51"/>
-      <c r="Y26" s="51"/>
-      <c r="Z26" s="51"/>
-      <c r="AA26" s="51"/>
-      <c r="AB26" s="51"/>
-      <c r="AC26" s="52"/>
-      <c r="AD26" s="52"/>
-      <c r="AE26" s="52"/>
-      <c r="AF26" s="52"/>
-      <c r="AG26" s="52"/>
-      <c r="AH26" s="52"/>
-      <c r="AI26" s="52"/>
-      <c r="AJ26" s="52"/>
-      <c r="AK26" s="52"/>
-      <c r="AL26" s="51"/>
-      <c r="AM26" s="51"/>
-      <c r="AN26" s="51"/>
-      <c r="AO26" s="51"/>
-      <c r="AP26" s="51"/>
-      <c r="AQ26" s="51"/>
-      <c r="AR26" s="51"/>
-      <c r="AS26" s="51"/>
-      <c r="AT26" s="51"/>
-      <c r="AU26" s="51"/>
-      <c r="AV26" s="51"/>
-      <c r="AW26" s="51"/>
-      <c r="AX26" s="51"/>
-      <c r="AY26" s="51"/>
-      <c r="AZ26" s="51"/>
-      <c r="BA26" s="52"/>
-      <c r="BB26" s="52"/>
-      <c r="BC26" s="52"/>
-      <c r="BD26" s="52"/>
-      <c r="BE26" s="52"/>
-      <c r="BF26" s="52"/>
+        <v>1</v>
+      </c>
+      <c r="I26" s="49"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="41"/>
+      <c r="L26" s="50"/>
+      <c r="M26" s="50"/>
+      <c r="N26" s="50"/>
+      <c r="O26" s="50"/>
+      <c r="P26" s="50"/>
+      <c r="Q26" s="50"/>
+      <c r="R26" s="50"/>
+      <c r="S26" s="50"/>
+      <c r="T26" s="50"/>
+      <c r="U26" s="50"/>
+      <c r="V26" s="50"/>
+      <c r="W26" s="50"/>
+      <c r="X26" s="50"/>
+      <c r="Y26" s="50"/>
+      <c r="Z26" s="50"/>
+      <c r="AA26" s="50"/>
+      <c r="AB26" s="50"/>
+      <c r="AC26" s="51"/>
+      <c r="AD26" s="51"/>
+      <c r="AE26" s="51"/>
+      <c r="AF26" s="51"/>
+      <c r="AG26" s="51"/>
+      <c r="AH26" s="51"/>
+      <c r="AI26" s="51"/>
+      <c r="AJ26" s="51"/>
+      <c r="AK26" s="51"/>
+      <c r="AL26" s="50"/>
+      <c r="AM26" s="50"/>
+      <c r="AN26" s="50"/>
+      <c r="AO26" s="50"/>
+      <c r="AP26" s="50"/>
+      <c r="AQ26" s="50"/>
+      <c r="AR26" s="50"/>
+      <c r="AS26" s="50"/>
+      <c r="AT26" s="50"/>
+      <c r="AU26" s="50"/>
+      <c r="AV26" s="50"/>
+      <c r="AW26" s="50"/>
+      <c r="AX26" s="50"/>
+      <c r="AY26" s="50"/>
+      <c r="AZ26" s="50"/>
+      <c r="BA26" s="51"/>
+      <c r="BB26" s="51"/>
+      <c r="BC26" s="51"/>
+      <c r="BD26" s="51"/>
+      <c r="BE26" s="51"/>
+      <c r="BF26" s="51"/>
       <c r="BG26" s="35"/>
     </row>
     <row r="27" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="35"/>
       <c r="B27" s="36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27" s="37" t="s">
         <v>46</v>
       </c>
       <c r="D27" s="37" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E27" s="38">
         <v>45732</v>
@@ -3371,67 +3371,67 @@
         <v>1</v>
       </c>
       <c r="H27" s="40">
-        <v>0</v>
-      </c>
-      <c r="I27" s="50"/>
-      <c r="J27" s="51"/>
-      <c r="K27" s="42"/>
-      <c r="L27" s="51"/>
-      <c r="M27" s="51"/>
-      <c r="N27" s="51"/>
-      <c r="O27" s="51"/>
-      <c r="P27" s="51"/>
-      <c r="Q27" s="51"/>
-      <c r="R27" s="51"/>
-      <c r="S27" s="51"/>
-      <c r="T27" s="51"/>
-      <c r="U27" s="51"/>
-      <c r="V27" s="51"/>
-      <c r="W27" s="51"/>
-      <c r="X27" s="51"/>
-      <c r="Y27" s="51"/>
-      <c r="Z27" s="51"/>
-      <c r="AA27" s="51"/>
-      <c r="AB27" s="51"/>
-      <c r="AC27" s="52"/>
-      <c r="AD27" s="52"/>
-      <c r="AE27" s="52"/>
-      <c r="AF27" s="52"/>
-      <c r="AG27" s="52"/>
-      <c r="AH27" s="52"/>
-      <c r="AI27" s="52"/>
-      <c r="AJ27" s="52"/>
-      <c r="AK27" s="52"/>
-      <c r="AL27" s="51"/>
-      <c r="AM27" s="51"/>
-      <c r="AN27" s="51"/>
-      <c r="AO27" s="51"/>
-      <c r="AP27" s="51"/>
-      <c r="AQ27" s="51"/>
-      <c r="AR27" s="51"/>
-      <c r="AS27" s="51"/>
-      <c r="AT27" s="51"/>
-      <c r="AU27" s="51"/>
-      <c r="AV27" s="51"/>
-      <c r="AW27" s="51"/>
-      <c r="AX27" s="51"/>
-      <c r="AY27" s="51"/>
-      <c r="AZ27" s="51"/>
-      <c r="BA27" s="52"/>
-      <c r="BB27" s="52"/>
-      <c r="BC27" s="52"/>
-      <c r="BD27" s="52"/>
-      <c r="BE27" s="52"/>
-      <c r="BF27" s="52"/>
+        <v>1</v>
+      </c>
+      <c r="I27" s="49"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="41"/>
+      <c r="L27" s="50"/>
+      <c r="M27" s="50"/>
+      <c r="N27" s="50"/>
+      <c r="O27" s="50"/>
+      <c r="P27" s="50"/>
+      <c r="Q27" s="50"/>
+      <c r="R27" s="50"/>
+      <c r="S27" s="50"/>
+      <c r="T27" s="50"/>
+      <c r="U27" s="50"/>
+      <c r="V27" s="50"/>
+      <c r="W27" s="50"/>
+      <c r="X27" s="50"/>
+      <c r="Y27" s="50"/>
+      <c r="Z27" s="50"/>
+      <c r="AA27" s="50"/>
+      <c r="AB27" s="50"/>
+      <c r="AC27" s="51"/>
+      <c r="AD27" s="51"/>
+      <c r="AE27" s="51"/>
+      <c r="AF27" s="51"/>
+      <c r="AG27" s="51"/>
+      <c r="AH27" s="51"/>
+      <c r="AI27" s="51"/>
+      <c r="AJ27" s="51"/>
+      <c r="AK27" s="51"/>
+      <c r="AL27" s="50"/>
+      <c r="AM27" s="50"/>
+      <c r="AN27" s="50"/>
+      <c r="AO27" s="50"/>
+      <c r="AP27" s="50"/>
+      <c r="AQ27" s="50"/>
+      <c r="AR27" s="50"/>
+      <c r="AS27" s="50"/>
+      <c r="AT27" s="50"/>
+      <c r="AU27" s="50"/>
+      <c r="AV27" s="50"/>
+      <c r="AW27" s="50"/>
+      <c r="AX27" s="50"/>
+      <c r="AY27" s="50"/>
+      <c r="AZ27" s="50"/>
+      <c r="BA27" s="51"/>
+      <c r="BB27" s="51"/>
+      <c r="BC27" s="51"/>
+      <c r="BD27" s="51"/>
+      <c r="BE27" s="51"/>
+      <c r="BF27" s="51"/>
       <c r="BG27" s="35"/>
     </row>
     <row r="28" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="35"/>
       <c r="B28" s="36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C28" s="37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D28" s="37" t="s">
         <v>38</v>
@@ -3448,13 +3448,13 @@
       <c r="H28" s="40">
         <v>1</v>
       </c>
-      <c r="I28" s="50"/>
-      <c r="J28" s="51"/>
-      <c r="K28" s="51"/>
-      <c r="L28" s="51"/>
-      <c r="M28" s="51"/>
-      <c r="N28" s="51"/>
-      <c r="O28" s="51"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="50"/>
+      <c r="N28" s="50"/>
+      <c r="O28" s="50"/>
       <c r="P28" s="41"/>
       <c r="Q28" s="41"/>
       <c r="R28" s="41"/>
@@ -3463,50 +3463,50 @@
       <c r="U28" s="41"/>
       <c r="V28" s="41"/>
       <c r="W28" s="41"/>
-      <c r="X28" s="51"/>
-      <c r="Y28" s="51"/>
-      <c r="Z28" s="51"/>
-      <c r="AA28" s="51"/>
-      <c r="AB28" s="51"/>
-      <c r="AC28" s="52"/>
-      <c r="AD28" s="52"/>
-      <c r="AE28" s="52"/>
-      <c r="AF28" s="52"/>
-      <c r="AG28" s="52"/>
-      <c r="AH28" s="52"/>
-      <c r="AI28" s="52"/>
-      <c r="AJ28" s="52"/>
-      <c r="AK28" s="52"/>
-      <c r="AL28" s="51"/>
-      <c r="AM28" s="51"/>
-      <c r="AN28" s="51"/>
-      <c r="AO28" s="51"/>
-      <c r="AP28" s="51"/>
-      <c r="AQ28" s="51"/>
-      <c r="AR28" s="51"/>
-      <c r="AS28" s="51"/>
-      <c r="AT28" s="51"/>
-      <c r="AU28" s="51"/>
-      <c r="AV28" s="51"/>
-      <c r="AW28" s="51"/>
-      <c r="AX28" s="51"/>
-      <c r="AY28" s="51"/>
-      <c r="AZ28" s="51"/>
-      <c r="BA28" s="52"/>
-      <c r="BB28" s="52"/>
-      <c r="BC28" s="52"/>
-      <c r="BD28" s="52"/>
-      <c r="BE28" s="52"/>
-      <c r="BF28" s="52"/>
+      <c r="X28" s="50"/>
+      <c r="Y28" s="50"/>
+      <c r="Z28" s="50"/>
+      <c r="AA28" s="50"/>
+      <c r="AB28" s="50"/>
+      <c r="AC28" s="51"/>
+      <c r="AD28" s="51"/>
+      <c r="AE28" s="51"/>
+      <c r="AF28" s="51"/>
+      <c r="AG28" s="51"/>
+      <c r="AH28" s="51"/>
+      <c r="AI28" s="51"/>
+      <c r="AJ28" s="51"/>
+      <c r="AK28" s="51"/>
+      <c r="AL28" s="50"/>
+      <c r="AM28" s="50"/>
+      <c r="AN28" s="50"/>
+      <c r="AO28" s="50"/>
+      <c r="AP28" s="50"/>
+      <c r="AQ28" s="50"/>
+      <c r="AR28" s="50"/>
+      <c r="AS28" s="50"/>
+      <c r="AT28" s="50"/>
+      <c r="AU28" s="50"/>
+      <c r="AV28" s="50"/>
+      <c r="AW28" s="50"/>
+      <c r="AX28" s="50"/>
+      <c r="AY28" s="50"/>
+      <c r="AZ28" s="50"/>
+      <c r="BA28" s="51"/>
+      <c r="BB28" s="51"/>
+      <c r="BC28" s="51"/>
+      <c r="BD28" s="51"/>
+      <c r="BE28" s="51"/>
+      <c r="BF28" s="51"/>
       <c r="BG28" s="35"/>
     </row>
     <row r="29" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="35"/>
       <c r="B29" s="36" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="D29" s="37" t="s">
         <v>32</v>
@@ -3521,133 +3521,133 @@
         <v>8</v>
       </c>
       <c r="H29" s="40">
-        <v>0</v>
-      </c>
-      <c r="I29" s="50"/>
-      <c r="J29" s="51"/>
-      <c r="K29" s="51"/>
-      <c r="L29" s="51"/>
-      <c r="M29" s="51"/>
-      <c r="N29" s="51"/>
-      <c r="O29" s="51"/>
-      <c r="P29" s="42"/>
-      <c r="Q29" s="42"/>
-      <c r="R29" s="42"/>
-      <c r="S29" s="42"/>
-      <c r="T29" s="42"/>
-      <c r="U29" s="42"/>
-      <c r="V29" s="42"/>
-      <c r="W29" s="42"/>
-      <c r="X29" s="51"/>
-      <c r="Y29" s="51"/>
-      <c r="Z29" s="51"/>
-      <c r="AA29" s="51"/>
-      <c r="AB29" s="51"/>
-      <c r="AC29" s="52"/>
-      <c r="AD29" s="52"/>
-      <c r="AE29" s="52"/>
-      <c r="AF29" s="52"/>
-      <c r="AG29" s="52"/>
-      <c r="AH29" s="52"/>
-      <c r="AI29" s="52"/>
-      <c r="AJ29" s="52"/>
-      <c r="AK29" s="52"/>
-      <c r="AL29" s="51"/>
-      <c r="AM29" s="51"/>
-      <c r="AN29" s="51"/>
-      <c r="AO29" s="51"/>
-      <c r="AP29" s="51"/>
-      <c r="AQ29" s="51"/>
-      <c r="AR29" s="51"/>
-      <c r="AS29" s="51"/>
-      <c r="AT29" s="51"/>
-      <c r="AU29" s="51"/>
-      <c r="AV29" s="51"/>
-      <c r="AW29" s="51"/>
-      <c r="AX29" s="51"/>
-      <c r="AY29" s="51"/>
-      <c r="AZ29" s="51"/>
-      <c r="BA29" s="52"/>
-      <c r="BB29" s="52"/>
-      <c r="BC29" s="52"/>
-      <c r="BD29" s="52"/>
-      <c r="BE29" s="52"/>
-      <c r="BF29" s="52"/>
+        <v>1</v>
+      </c>
+      <c r="I29" s="49"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="50"/>
+      <c r="L29" s="50"/>
+      <c r="M29" s="50"/>
+      <c r="N29" s="50"/>
+      <c r="O29" s="50"/>
+      <c r="P29" s="41"/>
+      <c r="Q29" s="41"/>
+      <c r="R29" s="41"/>
+      <c r="S29" s="41"/>
+      <c r="T29" s="41"/>
+      <c r="U29" s="41"/>
+      <c r="V29" s="41"/>
+      <c r="W29" s="41"/>
+      <c r="X29" s="50"/>
+      <c r="Y29" s="50"/>
+      <c r="Z29" s="50"/>
+      <c r="AA29" s="50"/>
+      <c r="AB29" s="50"/>
+      <c r="AC29" s="51"/>
+      <c r="AD29" s="51"/>
+      <c r="AE29" s="51"/>
+      <c r="AF29" s="51"/>
+      <c r="AG29" s="51"/>
+      <c r="AH29" s="51"/>
+      <c r="AI29" s="51"/>
+      <c r="AJ29" s="51"/>
+      <c r="AK29" s="51"/>
+      <c r="AL29" s="50"/>
+      <c r="AM29" s="50"/>
+      <c r="AN29" s="50"/>
+      <c r="AO29" s="50"/>
+      <c r="AP29" s="50"/>
+      <c r="AQ29" s="50"/>
+      <c r="AR29" s="50"/>
+      <c r="AS29" s="50"/>
+      <c r="AT29" s="50"/>
+      <c r="AU29" s="50"/>
+      <c r="AV29" s="50"/>
+      <c r="AW29" s="50"/>
+      <c r="AX29" s="50"/>
+      <c r="AY29" s="50"/>
+      <c r="AZ29" s="50"/>
+      <c r="BA29" s="51"/>
+      <c r="BB29" s="51"/>
+      <c r="BC29" s="51"/>
+      <c r="BD29" s="51"/>
+      <c r="BE29" s="51"/>
+      <c r="BF29" s="51"/>
       <c r="BG29" s="35"/>
     </row>
     <row r="30" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="35"/>
-      <c r="B30" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="E30" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="F30" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="G30" s="55" t="s">
-        <v>42</v>
-      </c>
-      <c r="H30" s="56">
-        <v>0</v>
-      </c>
-      <c r="I30" s="57"/>
-      <c r="J30" s="58"/>
-      <c r="K30" s="51"/>
-      <c r="L30" s="51"/>
-      <c r="M30" s="51"/>
-      <c r="N30" s="51"/>
-      <c r="O30" s="51"/>
-      <c r="P30" s="51"/>
-      <c r="Q30" s="51"/>
-      <c r="R30" s="51"/>
-      <c r="S30" s="51"/>
-      <c r="T30" s="51"/>
-      <c r="U30" s="51"/>
-      <c r="V30" s="51"/>
-      <c r="W30" s="51"/>
-      <c r="X30" s="51"/>
-      <c r="Y30" s="51"/>
-      <c r="Z30" s="51"/>
-      <c r="AA30" s="51"/>
-      <c r="AB30" s="51"/>
-      <c r="AC30" s="52"/>
-      <c r="AD30" s="52"/>
-      <c r="AE30" s="52"/>
-      <c r="AF30" s="52"/>
-      <c r="AG30" s="52"/>
-      <c r="AH30" s="52"/>
-      <c r="AI30" s="52"/>
-      <c r="AJ30" s="52"/>
-      <c r="AK30" s="52"/>
-      <c r="AL30" s="51"/>
-      <c r="AM30" s="51"/>
-      <c r="AN30" s="51"/>
-      <c r="AO30" s="51"/>
-      <c r="AP30" s="51"/>
-      <c r="AQ30" s="51"/>
-      <c r="AR30" s="51"/>
-      <c r="AS30" s="51"/>
-      <c r="AT30" s="51"/>
-      <c r="AU30" s="51"/>
-      <c r="AV30" s="51"/>
-      <c r="AW30" s="51"/>
-      <c r="AX30" s="51"/>
-      <c r="AY30" s="51"/>
-      <c r="AZ30" s="51"/>
-      <c r="BA30" s="52"/>
-      <c r="BB30" s="52"/>
-      <c r="BC30" s="52"/>
-      <c r="BD30" s="52"/>
-      <c r="BE30" s="52"/>
-      <c r="BF30" s="52"/>
+      <c r="B30" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="38">
+        <v>45737</v>
+      </c>
+      <c r="F30" s="38">
+        <v>45739</v>
+      </c>
+      <c r="G30" s="54">
+        <v>3</v>
+      </c>
+      <c r="H30" s="55">
+        <v>1</v>
+      </c>
+      <c r="I30" s="56"/>
+      <c r="J30" s="57"/>
+      <c r="K30" s="50"/>
+      <c r="L30" s="50"/>
+      <c r="M30" s="50"/>
+      <c r="N30" s="50"/>
+      <c r="O30" s="50"/>
+      <c r="P30" s="50"/>
+      <c r="Q30" s="50"/>
+      <c r="R30" s="50"/>
+      <c r="S30" s="50"/>
+      <c r="T30" s="50"/>
+      <c r="U30" s="41"/>
+      <c r="V30" s="41"/>
+      <c r="W30" s="41"/>
+      <c r="X30" s="50"/>
+      <c r="Y30" s="50"/>
+      <c r="Z30" s="50"/>
+      <c r="AA30" s="50"/>
+      <c r="AB30" s="50"/>
+      <c r="AC30" s="51"/>
+      <c r="AD30" s="51"/>
+      <c r="AE30" s="51"/>
+      <c r="AF30" s="51"/>
+      <c r="AG30" s="51"/>
+      <c r="AH30" s="51"/>
+      <c r="AI30" s="51"/>
+      <c r="AJ30" s="51"/>
+      <c r="AK30" s="51"/>
+      <c r="AL30" s="50"/>
+      <c r="AM30" s="50"/>
+      <c r="AN30" s="50"/>
+      <c r="AO30" s="50"/>
+      <c r="AP30" s="50"/>
+      <c r="AQ30" s="50"/>
+      <c r="AR30" s="50"/>
+      <c r="AS30" s="50"/>
+      <c r="AT30" s="50"/>
+      <c r="AU30" s="50"/>
+      <c r="AV30" s="50"/>
+      <c r="AW30" s="50"/>
+      <c r="AX30" s="50"/>
+      <c r="AY30" s="50"/>
+      <c r="AZ30" s="50"/>
+      <c r="BA30" s="51"/>
+      <c r="BB30" s="51"/>
+      <c r="BC30" s="51"/>
+      <c r="BD30" s="51"/>
+      <c r="BE30" s="51"/>
+      <c r="BF30" s="51"/>
       <c r="BG30" s="35"/>
     </row>
     <row r="31" spans="1:59" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -3718,7 +3718,7 @@
     <row r="32" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="35"/>
       <c r="B32" s="36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C32" s="37" t="s">
         <v>42</v>
@@ -3738,56 +3738,56 @@
       <c r="H32" s="40">
         <v>0</v>
       </c>
-      <c r="I32" s="50"/>
-      <c r="J32" s="59"/>
-      <c r="K32" s="43"/>
-      <c r="L32" s="43"/>
-      <c r="M32" s="43"/>
-      <c r="N32" s="46"/>
-      <c r="O32" s="46"/>
-      <c r="P32" s="46"/>
-      <c r="Q32" s="46"/>
-      <c r="R32" s="46"/>
-      <c r="S32" s="46"/>
-      <c r="T32" s="46"/>
-      <c r="U32" s="46"/>
-      <c r="V32" s="46"/>
-      <c r="W32" s="46"/>
-      <c r="X32" s="60"/>
-      <c r="Y32" s="60"/>
-      <c r="Z32" s="60"/>
-      <c r="AA32" s="60"/>
-      <c r="AB32" s="60"/>
-      <c r="AC32" s="61"/>
-      <c r="AD32" s="61"/>
-      <c r="AE32" s="47"/>
-      <c r="AF32" s="47"/>
-      <c r="AG32" s="47"/>
-      <c r="AH32" s="47"/>
-      <c r="AI32" s="47"/>
-      <c r="AJ32" s="47"/>
-      <c r="AK32" s="47"/>
-      <c r="AL32" s="46"/>
-      <c r="AM32" s="46"/>
-      <c r="AN32" s="46"/>
-      <c r="AO32" s="46"/>
-      <c r="AP32" s="46"/>
-      <c r="AQ32" s="46"/>
-      <c r="AR32" s="46"/>
-      <c r="AS32" s="46"/>
-      <c r="AT32" s="46"/>
-      <c r="AU32" s="46"/>
-      <c r="AV32" s="46"/>
-      <c r="AW32" s="46"/>
-      <c r="AX32" s="46"/>
-      <c r="AY32" s="46"/>
-      <c r="AZ32" s="46"/>
-      <c r="BA32" s="47"/>
-      <c r="BB32" s="47"/>
-      <c r="BC32" s="47"/>
-      <c r="BD32" s="47"/>
-      <c r="BE32" s="47"/>
-      <c r="BF32" s="47"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="58"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="42"/>
+      <c r="M32" s="42"/>
+      <c r="N32" s="45"/>
+      <c r="O32" s="45"/>
+      <c r="P32" s="45"/>
+      <c r="Q32" s="45"/>
+      <c r="R32" s="45"/>
+      <c r="S32" s="45"/>
+      <c r="T32" s="45"/>
+      <c r="U32" s="45"/>
+      <c r="V32" s="45"/>
+      <c r="W32" s="45"/>
+      <c r="X32" s="59"/>
+      <c r="Y32" s="59"/>
+      <c r="Z32" s="59"/>
+      <c r="AA32" s="59"/>
+      <c r="AB32" s="59"/>
+      <c r="AC32" s="60"/>
+      <c r="AD32" s="60"/>
+      <c r="AE32" s="46"/>
+      <c r="AF32" s="46"/>
+      <c r="AG32" s="46"/>
+      <c r="AH32" s="46"/>
+      <c r="AI32" s="46"/>
+      <c r="AJ32" s="46"/>
+      <c r="AK32" s="46"/>
+      <c r="AL32" s="45"/>
+      <c r="AM32" s="45"/>
+      <c r="AN32" s="45"/>
+      <c r="AO32" s="45"/>
+      <c r="AP32" s="45"/>
+      <c r="AQ32" s="45"/>
+      <c r="AR32" s="45"/>
+      <c r="AS32" s="45"/>
+      <c r="AT32" s="45"/>
+      <c r="AU32" s="45"/>
+      <c r="AV32" s="45"/>
+      <c r="AW32" s="45"/>
+      <c r="AX32" s="45"/>
+      <c r="AY32" s="45"/>
+      <c r="AZ32" s="45"/>
+      <c r="BA32" s="46"/>
+      <c r="BB32" s="46"/>
+      <c r="BC32" s="46"/>
+      <c r="BD32" s="46"/>
+      <c r="BE32" s="46"/>
+      <c r="BF32" s="46"/>
       <c r="BG32" s="35"/>
     </row>
     <row r="33" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3807,56 +3807,56 @@
       <c r="H33" s="40">
         <v>0</v>
       </c>
-      <c r="I33" s="62"/>
-      <c r="J33" s="45"/>
-      <c r="K33" s="46"/>
-      <c r="L33" s="46"/>
-      <c r="M33" s="46"/>
-      <c r="N33" s="46"/>
-      <c r="O33" s="46"/>
-      <c r="P33" s="46"/>
-      <c r="Q33" s="46"/>
-      <c r="R33" s="46"/>
-      <c r="S33" s="46"/>
-      <c r="T33" s="46"/>
-      <c r="U33" s="46"/>
-      <c r="V33" s="46"/>
-      <c r="W33" s="46"/>
-      <c r="X33" s="46"/>
-      <c r="Y33" s="46"/>
-      <c r="Z33" s="46"/>
-      <c r="AA33" s="46"/>
-      <c r="AB33" s="46"/>
-      <c r="AC33" s="47"/>
-      <c r="AD33" s="47"/>
-      <c r="AE33" s="47"/>
-      <c r="AF33" s="47"/>
-      <c r="AG33" s="47"/>
-      <c r="AH33" s="47"/>
-      <c r="AI33" s="47"/>
-      <c r="AJ33" s="47"/>
-      <c r="AK33" s="47"/>
-      <c r="AL33" s="46"/>
-      <c r="AM33" s="46"/>
-      <c r="AN33" s="46"/>
-      <c r="AO33" s="46"/>
-      <c r="AP33" s="46"/>
-      <c r="AQ33" s="46"/>
-      <c r="AR33" s="46"/>
-      <c r="AS33" s="46"/>
-      <c r="AT33" s="46"/>
-      <c r="AU33" s="46"/>
-      <c r="AV33" s="46"/>
-      <c r="AW33" s="46"/>
-      <c r="AX33" s="46"/>
-      <c r="AY33" s="46"/>
-      <c r="AZ33" s="46"/>
-      <c r="BA33" s="47"/>
-      <c r="BB33" s="47"/>
-      <c r="BC33" s="47"/>
-      <c r="BD33" s="47"/>
-      <c r="BE33" s="47"/>
-      <c r="BF33" s="47"/>
+      <c r="I33" s="61"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="45"/>
+      <c r="L33" s="45"/>
+      <c r="M33" s="45"/>
+      <c r="N33" s="45"/>
+      <c r="O33" s="45"/>
+      <c r="P33" s="45"/>
+      <c r="Q33" s="45"/>
+      <c r="R33" s="45"/>
+      <c r="S33" s="45"/>
+      <c r="T33" s="45"/>
+      <c r="U33" s="45"/>
+      <c r="V33" s="45"/>
+      <c r="W33" s="45"/>
+      <c r="X33" s="45"/>
+      <c r="Y33" s="45"/>
+      <c r="Z33" s="45"/>
+      <c r="AA33" s="45"/>
+      <c r="AB33" s="45"/>
+      <c r="AC33" s="46"/>
+      <c r="AD33" s="46"/>
+      <c r="AE33" s="46"/>
+      <c r="AF33" s="46"/>
+      <c r="AG33" s="46"/>
+      <c r="AH33" s="46"/>
+      <c r="AI33" s="46"/>
+      <c r="AJ33" s="46"/>
+      <c r="AK33" s="46"/>
+      <c r="AL33" s="45"/>
+      <c r="AM33" s="45"/>
+      <c r="AN33" s="45"/>
+      <c r="AO33" s="45"/>
+      <c r="AP33" s="45"/>
+      <c r="AQ33" s="45"/>
+      <c r="AR33" s="45"/>
+      <c r="AS33" s="45"/>
+      <c r="AT33" s="45"/>
+      <c r="AU33" s="45"/>
+      <c r="AV33" s="45"/>
+      <c r="AW33" s="45"/>
+      <c r="AX33" s="45"/>
+      <c r="AY33" s="45"/>
+      <c r="AZ33" s="45"/>
+      <c r="BA33" s="46"/>
+      <c r="BB33" s="46"/>
+      <c r="BC33" s="46"/>
+      <c r="BD33" s="46"/>
+      <c r="BE33" s="46"/>
+      <c r="BF33" s="46"/>
       <c r="BG33" s="35"/>
     </row>
     <row r="34" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3876,56 +3876,56 @@
       <c r="H34" s="40">
         <v>0</v>
       </c>
-      <c r="I34" s="62"/>
-      <c r="J34" s="45"/>
-      <c r="K34" s="46"/>
-      <c r="L34" s="46"/>
-      <c r="M34" s="46"/>
-      <c r="N34" s="46"/>
-      <c r="O34" s="46"/>
-      <c r="P34" s="46"/>
-      <c r="Q34" s="46"/>
-      <c r="R34" s="46"/>
-      <c r="S34" s="46"/>
-      <c r="T34" s="46"/>
-      <c r="U34" s="46"/>
-      <c r="V34" s="46"/>
-      <c r="W34" s="46"/>
-      <c r="X34" s="46"/>
-      <c r="Y34" s="46"/>
-      <c r="Z34" s="46"/>
-      <c r="AA34" s="46"/>
-      <c r="AB34" s="46"/>
-      <c r="AC34" s="47"/>
-      <c r="AD34" s="47"/>
-      <c r="AE34" s="47"/>
-      <c r="AF34" s="47"/>
-      <c r="AG34" s="47"/>
-      <c r="AH34" s="47"/>
-      <c r="AI34" s="47"/>
-      <c r="AJ34" s="47"/>
-      <c r="AK34" s="47"/>
-      <c r="AL34" s="46"/>
-      <c r="AM34" s="46"/>
-      <c r="AN34" s="46"/>
-      <c r="AO34" s="46"/>
-      <c r="AP34" s="46"/>
-      <c r="AQ34" s="46"/>
-      <c r="AR34" s="46"/>
-      <c r="AS34" s="46"/>
-      <c r="AT34" s="46"/>
-      <c r="AU34" s="46"/>
-      <c r="AV34" s="46"/>
-      <c r="AW34" s="46"/>
-      <c r="AX34" s="46"/>
-      <c r="AY34" s="46"/>
-      <c r="AZ34" s="46"/>
-      <c r="BA34" s="47"/>
-      <c r="BB34" s="47"/>
-      <c r="BC34" s="47"/>
-      <c r="BD34" s="47"/>
-      <c r="BE34" s="47"/>
-      <c r="BF34" s="47"/>
+      <c r="I34" s="61"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="45"/>
+      <c r="L34" s="45"/>
+      <c r="M34" s="45"/>
+      <c r="N34" s="45"/>
+      <c r="O34" s="45"/>
+      <c r="P34" s="45"/>
+      <c r="Q34" s="45"/>
+      <c r="R34" s="45"/>
+      <c r="S34" s="45"/>
+      <c r="T34" s="45"/>
+      <c r="U34" s="45"/>
+      <c r="V34" s="45"/>
+      <c r="W34" s="45"/>
+      <c r="X34" s="45"/>
+      <c r="Y34" s="45"/>
+      <c r="Z34" s="45"/>
+      <c r="AA34" s="45"/>
+      <c r="AB34" s="45"/>
+      <c r="AC34" s="46"/>
+      <c r="AD34" s="46"/>
+      <c r="AE34" s="46"/>
+      <c r="AF34" s="46"/>
+      <c r="AG34" s="46"/>
+      <c r="AH34" s="46"/>
+      <c r="AI34" s="46"/>
+      <c r="AJ34" s="46"/>
+      <c r="AK34" s="46"/>
+      <c r="AL34" s="45"/>
+      <c r="AM34" s="45"/>
+      <c r="AN34" s="45"/>
+      <c r="AO34" s="45"/>
+      <c r="AP34" s="45"/>
+      <c r="AQ34" s="45"/>
+      <c r="AR34" s="45"/>
+      <c r="AS34" s="45"/>
+      <c r="AT34" s="45"/>
+      <c r="AU34" s="45"/>
+      <c r="AV34" s="45"/>
+      <c r="AW34" s="45"/>
+      <c r="AX34" s="45"/>
+      <c r="AY34" s="45"/>
+      <c r="AZ34" s="45"/>
+      <c r="BA34" s="46"/>
+      <c r="BB34" s="46"/>
+      <c r="BC34" s="46"/>
+      <c r="BD34" s="46"/>
+      <c r="BE34" s="46"/>
+      <c r="BF34" s="46"/>
       <c r="BG34" s="35"/>
     </row>
     <row r="35" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3942,59 +3942,59 @@
       <c r="G35" s="39">
         <v>0</v>
       </c>
-      <c r="H35" s="49">
+      <c r="H35" s="48">
         <v>0</v>
       </c>
-      <c r="I35" s="62"/>
-      <c r="J35" s="45"/>
-      <c r="K35" s="46"/>
-      <c r="L35" s="46"/>
-      <c r="M35" s="46"/>
-      <c r="N35" s="46"/>
-      <c r="O35" s="46"/>
-      <c r="P35" s="46"/>
-      <c r="Q35" s="46"/>
-      <c r="R35" s="46"/>
-      <c r="S35" s="46"/>
-      <c r="T35" s="46"/>
-      <c r="U35" s="46"/>
-      <c r="V35" s="46"/>
-      <c r="W35" s="46"/>
-      <c r="X35" s="46"/>
-      <c r="Y35" s="46"/>
-      <c r="Z35" s="46"/>
-      <c r="AA35" s="46"/>
-      <c r="AB35" s="46"/>
-      <c r="AC35" s="47"/>
-      <c r="AD35" s="47"/>
-      <c r="AE35" s="47"/>
-      <c r="AF35" s="47"/>
-      <c r="AG35" s="47"/>
-      <c r="AH35" s="47"/>
-      <c r="AI35" s="47"/>
-      <c r="AJ35" s="47"/>
-      <c r="AK35" s="47"/>
-      <c r="AL35" s="46"/>
-      <c r="AM35" s="46"/>
-      <c r="AN35" s="46"/>
-      <c r="AO35" s="46"/>
-      <c r="AP35" s="46"/>
-      <c r="AQ35" s="46"/>
-      <c r="AR35" s="46"/>
-      <c r="AS35" s="46"/>
-      <c r="AT35" s="46"/>
-      <c r="AU35" s="46"/>
-      <c r="AV35" s="46"/>
-      <c r="AW35" s="46"/>
-      <c r="AX35" s="46"/>
-      <c r="AY35" s="46"/>
-      <c r="AZ35" s="46"/>
-      <c r="BA35" s="47"/>
-      <c r="BB35" s="47"/>
-      <c r="BC35" s="47"/>
-      <c r="BD35" s="47"/>
-      <c r="BE35" s="47"/>
-      <c r="BF35" s="47"/>
+      <c r="I35" s="61"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="45"/>
+      <c r="L35" s="45"/>
+      <c r="M35" s="45"/>
+      <c r="N35" s="45"/>
+      <c r="O35" s="45"/>
+      <c r="P35" s="45"/>
+      <c r="Q35" s="45"/>
+      <c r="R35" s="45"/>
+      <c r="S35" s="45"/>
+      <c r="T35" s="45"/>
+      <c r="U35" s="45"/>
+      <c r="V35" s="45"/>
+      <c r="W35" s="45"/>
+      <c r="X35" s="45"/>
+      <c r="Y35" s="45"/>
+      <c r="Z35" s="45"/>
+      <c r="AA35" s="45"/>
+      <c r="AB35" s="45"/>
+      <c r="AC35" s="46"/>
+      <c r="AD35" s="46"/>
+      <c r="AE35" s="46"/>
+      <c r="AF35" s="46"/>
+      <c r="AG35" s="46"/>
+      <c r="AH35" s="46"/>
+      <c r="AI35" s="46"/>
+      <c r="AJ35" s="46"/>
+      <c r="AK35" s="46"/>
+      <c r="AL35" s="45"/>
+      <c r="AM35" s="45"/>
+      <c r="AN35" s="45"/>
+      <c r="AO35" s="45"/>
+      <c r="AP35" s="45"/>
+      <c r="AQ35" s="45"/>
+      <c r="AR35" s="45"/>
+      <c r="AS35" s="45"/>
+      <c r="AT35" s="45"/>
+      <c r="AU35" s="45"/>
+      <c r="AV35" s="45"/>
+      <c r="AW35" s="45"/>
+      <c r="AX35" s="45"/>
+      <c r="AY35" s="45"/>
+      <c r="AZ35" s="45"/>
+      <c r="BA35" s="46"/>
+      <c r="BB35" s="46"/>
+      <c r="BC35" s="46"/>
+      <c r="BD35" s="46"/>
+      <c r="BE35" s="46"/>
+      <c r="BF35" s="46"/>
       <c r="BG35" s="35"/>
     </row>
     <row r="36" spans="1:59" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4079,56 +4079,56 @@
       <c r="H37" s="40">
         <v>0</v>
       </c>
-      <c r="I37" s="50"/>
-      <c r="J37" s="59"/>
-      <c r="K37" s="43"/>
-      <c r="L37" s="43"/>
-      <c r="M37" s="43"/>
-      <c r="N37" s="46"/>
-      <c r="O37" s="46"/>
-      <c r="P37" s="46"/>
-      <c r="Q37" s="46"/>
-      <c r="R37" s="46"/>
-      <c r="S37" s="46"/>
-      <c r="T37" s="46"/>
-      <c r="U37" s="46"/>
-      <c r="V37" s="46"/>
-      <c r="W37" s="46"/>
-      <c r="X37" s="46"/>
-      <c r="Y37" s="46"/>
-      <c r="Z37" s="46"/>
-      <c r="AA37" s="46"/>
-      <c r="AB37" s="46"/>
-      <c r="AC37" s="47"/>
-      <c r="AD37" s="47"/>
-      <c r="AE37" s="47"/>
-      <c r="AF37" s="47"/>
-      <c r="AG37" s="47"/>
-      <c r="AH37" s="47"/>
-      <c r="AI37" s="47"/>
-      <c r="AJ37" s="47"/>
-      <c r="AK37" s="47"/>
-      <c r="AL37" s="46"/>
-      <c r="AM37" s="46"/>
-      <c r="AN37" s="46"/>
-      <c r="AO37" s="46"/>
-      <c r="AP37" s="46"/>
-      <c r="AQ37" s="46"/>
-      <c r="AR37" s="46"/>
-      <c r="AS37" s="46"/>
-      <c r="AT37" s="46"/>
-      <c r="AU37" s="46"/>
-      <c r="AV37" s="46"/>
-      <c r="AW37" s="46"/>
-      <c r="AX37" s="46"/>
-      <c r="AY37" s="46"/>
-      <c r="AZ37" s="46"/>
-      <c r="BA37" s="47"/>
-      <c r="BB37" s="47"/>
-      <c r="BC37" s="47"/>
-      <c r="BD37" s="47"/>
-      <c r="BE37" s="47"/>
-      <c r="BF37" s="47"/>
+      <c r="I37" s="49"/>
+      <c r="J37" s="58"/>
+      <c r="K37" s="42"/>
+      <c r="L37" s="42"/>
+      <c r="M37" s="42"/>
+      <c r="N37" s="45"/>
+      <c r="O37" s="45"/>
+      <c r="P37" s="45"/>
+      <c r="Q37" s="45"/>
+      <c r="R37" s="45"/>
+      <c r="S37" s="45"/>
+      <c r="T37" s="45"/>
+      <c r="U37" s="45"/>
+      <c r="V37" s="45"/>
+      <c r="W37" s="45"/>
+      <c r="X37" s="45"/>
+      <c r="Y37" s="45"/>
+      <c r="Z37" s="45"/>
+      <c r="AA37" s="45"/>
+      <c r="AB37" s="45"/>
+      <c r="AC37" s="46"/>
+      <c r="AD37" s="46"/>
+      <c r="AE37" s="46"/>
+      <c r="AF37" s="46"/>
+      <c r="AG37" s="46"/>
+      <c r="AH37" s="46"/>
+      <c r="AI37" s="46"/>
+      <c r="AJ37" s="46"/>
+      <c r="AK37" s="46"/>
+      <c r="AL37" s="45"/>
+      <c r="AM37" s="45"/>
+      <c r="AN37" s="45"/>
+      <c r="AO37" s="45"/>
+      <c r="AP37" s="45"/>
+      <c r="AQ37" s="45"/>
+      <c r="AR37" s="45"/>
+      <c r="AS37" s="45"/>
+      <c r="AT37" s="45"/>
+      <c r="AU37" s="45"/>
+      <c r="AV37" s="45"/>
+      <c r="AW37" s="45"/>
+      <c r="AX37" s="45"/>
+      <c r="AY37" s="45"/>
+      <c r="AZ37" s="45"/>
+      <c r="BA37" s="46"/>
+      <c r="BB37" s="46"/>
+      <c r="BC37" s="46"/>
+      <c r="BD37" s="46"/>
+      <c r="BE37" s="46"/>
+      <c r="BF37" s="46"/>
       <c r="BG37" s="35"/>
     </row>
     <row r="38" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4148,56 +4148,56 @@
       <c r="H38" s="40">
         <v>0</v>
       </c>
-      <c r="I38" s="62"/>
-      <c r="J38" s="45"/>
-      <c r="K38" s="46"/>
-      <c r="L38" s="46"/>
-      <c r="M38" s="46"/>
-      <c r="N38" s="46"/>
-      <c r="O38" s="46"/>
-      <c r="P38" s="46"/>
-      <c r="Q38" s="46"/>
-      <c r="R38" s="46"/>
-      <c r="S38" s="46"/>
-      <c r="T38" s="46"/>
-      <c r="U38" s="46"/>
-      <c r="V38" s="46"/>
-      <c r="W38" s="46"/>
-      <c r="X38" s="46"/>
-      <c r="Y38" s="46"/>
-      <c r="Z38" s="46"/>
-      <c r="AA38" s="46"/>
-      <c r="AB38" s="46"/>
-      <c r="AC38" s="47"/>
-      <c r="AD38" s="47"/>
-      <c r="AE38" s="47"/>
-      <c r="AF38" s="47"/>
-      <c r="AG38" s="47"/>
-      <c r="AH38" s="47"/>
-      <c r="AI38" s="47"/>
-      <c r="AJ38" s="47"/>
-      <c r="AK38" s="47"/>
-      <c r="AL38" s="46"/>
-      <c r="AM38" s="46"/>
-      <c r="AN38" s="46"/>
-      <c r="AO38" s="46"/>
-      <c r="AP38" s="46"/>
-      <c r="AQ38" s="46"/>
-      <c r="AR38" s="46"/>
-      <c r="AS38" s="46"/>
-      <c r="AT38" s="46"/>
-      <c r="AU38" s="46"/>
-      <c r="AV38" s="46"/>
-      <c r="AW38" s="46"/>
-      <c r="AX38" s="46"/>
-      <c r="AY38" s="46"/>
-      <c r="AZ38" s="46"/>
-      <c r="BA38" s="47"/>
-      <c r="BB38" s="47"/>
-      <c r="BC38" s="47"/>
-      <c r="BD38" s="47"/>
-      <c r="BE38" s="47"/>
-      <c r="BF38" s="47"/>
+      <c r="I38" s="61"/>
+      <c r="J38" s="44"/>
+      <c r="K38" s="45"/>
+      <c r="L38" s="45"/>
+      <c r="M38" s="45"/>
+      <c r="N38" s="45"/>
+      <c r="O38" s="45"/>
+      <c r="P38" s="45"/>
+      <c r="Q38" s="45"/>
+      <c r="R38" s="45"/>
+      <c r="S38" s="45"/>
+      <c r="T38" s="45"/>
+      <c r="U38" s="45"/>
+      <c r="V38" s="45"/>
+      <c r="W38" s="45"/>
+      <c r="X38" s="45"/>
+      <c r="Y38" s="45"/>
+      <c r="Z38" s="45"/>
+      <c r="AA38" s="45"/>
+      <c r="AB38" s="45"/>
+      <c r="AC38" s="46"/>
+      <c r="AD38" s="46"/>
+      <c r="AE38" s="46"/>
+      <c r="AF38" s="46"/>
+      <c r="AG38" s="46"/>
+      <c r="AH38" s="46"/>
+      <c r="AI38" s="46"/>
+      <c r="AJ38" s="46"/>
+      <c r="AK38" s="46"/>
+      <c r="AL38" s="45"/>
+      <c r="AM38" s="45"/>
+      <c r="AN38" s="45"/>
+      <c r="AO38" s="45"/>
+      <c r="AP38" s="45"/>
+      <c r="AQ38" s="45"/>
+      <c r="AR38" s="45"/>
+      <c r="AS38" s="45"/>
+      <c r="AT38" s="45"/>
+      <c r="AU38" s="45"/>
+      <c r="AV38" s="45"/>
+      <c r="AW38" s="45"/>
+      <c r="AX38" s="45"/>
+      <c r="AY38" s="45"/>
+      <c r="AZ38" s="45"/>
+      <c r="BA38" s="46"/>
+      <c r="BB38" s="46"/>
+      <c r="BC38" s="46"/>
+      <c r="BD38" s="46"/>
+      <c r="BE38" s="46"/>
+      <c r="BF38" s="46"/>
       <c r="BG38" s="35"/>
     </row>
     <row r="39" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4217,56 +4217,56 @@
       <c r="H39" s="40">
         <v>0</v>
       </c>
-      <c r="I39" s="62"/>
-      <c r="J39" s="45"/>
-      <c r="K39" s="46"/>
-      <c r="L39" s="46"/>
-      <c r="M39" s="46"/>
-      <c r="N39" s="46"/>
-      <c r="O39" s="46"/>
-      <c r="P39" s="46"/>
-      <c r="Q39" s="46"/>
-      <c r="R39" s="46"/>
-      <c r="S39" s="46"/>
-      <c r="T39" s="46"/>
-      <c r="U39" s="46"/>
-      <c r="V39" s="46"/>
-      <c r="W39" s="46"/>
-      <c r="X39" s="46"/>
-      <c r="Y39" s="46"/>
-      <c r="Z39" s="46"/>
-      <c r="AA39" s="46"/>
-      <c r="AB39" s="46"/>
-      <c r="AC39" s="47"/>
-      <c r="AD39" s="47"/>
-      <c r="AE39" s="47"/>
-      <c r="AF39" s="47"/>
-      <c r="AG39" s="47"/>
-      <c r="AH39" s="47"/>
-      <c r="AI39" s="47"/>
-      <c r="AJ39" s="47"/>
-      <c r="AK39" s="47"/>
-      <c r="AL39" s="46"/>
-      <c r="AM39" s="46"/>
-      <c r="AN39" s="46"/>
-      <c r="AO39" s="46"/>
-      <c r="AP39" s="46"/>
-      <c r="AQ39" s="46"/>
-      <c r="AR39" s="46"/>
-      <c r="AS39" s="46"/>
-      <c r="AT39" s="46"/>
-      <c r="AU39" s="46"/>
-      <c r="AV39" s="46"/>
-      <c r="AW39" s="46"/>
-      <c r="AX39" s="46"/>
-      <c r="AY39" s="46"/>
-      <c r="AZ39" s="46"/>
-      <c r="BA39" s="47"/>
-      <c r="BB39" s="47"/>
-      <c r="BC39" s="47"/>
-      <c r="BD39" s="47"/>
-      <c r="BE39" s="47"/>
-      <c r="BF39" s="47"/>
+      <c r="I39" s="61"/>
+      <c r="J39" s="44"/>
+      <c r="K39" s="45"/>
+      <c r="L39" s="45"/>
+      <c r="M39" s="45"/>
+      <c r="N39" s="45"/>
+      <c r="O39" s="45"/>
+      <c r="P39" s="45"/>
+      <c r="Q39" s="45"/>
+      <c r="R39" s="45"/>
+      <c r="S39" s="45"/>
+      <c r="T39" s="45"/>
+      <c r="U39" s="45"/>
+      <c r="V39" s="45"/>
+      <c r="W39" s="45"/>
+      <c r="X39" s="45"/>
+      <c r="Y39" s="45"/>
+      <c r="Z39" s="45"/>
+      <c r="AA39" s="45"/>
+      <c r="AB39" s="45"/>
+      <c r="AC39" s="46"/>
+      <c r="AD39" s="46"/>
+      <c r="AE39" s="46"/>
+      <c r="AF39" s="46"/>
+      <c r="AG39" s="46"/>
+      <c r="AH39" s="46"/>
+      <c r="AI39" s="46"/>
+      <c r="AJ39" s="46"/>
+      <c r="AK39" s="46"/>
+      <c r="AL39" s="45"/>
+      <c r="AM39" s="45"/>
+      <c r="AN39" s="45"/>
+      <c r="AO39" s="45"/>
+      <c r="AP39" s="45"/>
+      <c r="AQ39" s="45"/>
+      <c r="AR39" s="45"/>
+      <c r="AS39" s="45"/>
+      <c r="AT39" s="45"/>
+      <c r="AU39" s="45"/>
+      <c r="AV39" s="45"/>
+      <c r="AW39" s="45"/>
+      <c r="AX39" s="45"/>
+      <c r="AY39" s="45"/>
+      <c r="AZ39" s="45"/>
+      <c r="BA39" s="46"/>
+      <c r="BB39" s="46"/>
+      <c r="BC39" s="46"/>
+      <c r="BD39" s="46"/>
+      <c r="BE39" s="46"/>
+      <c r="BF39" s="46"/>
       <c r="BG39" s="35"/>
     </row>
     <row r="40" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4283,59 +4283,59 @@
       <c r="G40" s="39">
         <v>0</v>
       </c>
-      <c r="H40" s="49">
+      <c r="H40" s="48">
         <v>0</v>
       </c>
-      <c r="I40" s="62"/>
-      <c r="J40" s="45"/>
-      <c r="K40" s="46"/>
-      <c r="L40" s="46"/>
-      <c r="M40" s="46"/>
-      <c r="N40" s="46"/>
-      <c r="O40" s="46"/>
-      <c r="P40" s="46"/>
-      <c r="Q40" s="46"/>
-      <c r="R40" s="46"/>
-      <c r="S40" s="46"/>
-      <c r="T40" s="46"/>
-      <c r="U40" s="46"/>
-      <c r="V40" s="46"/>
-      <c r="W40" s="46"/>
-      <c r="X40" s="46"/>
-      <c r="Y40" s="46"/>
-      <c r="Z40" s="46"/>
-      <c r="AA40" s="46"/>
-      <c r="AB40" s="46"/>
-      <c r="AC40" s="47"/>
-      <c r="AD40" s="47"/>
-      <c r="AE40" s="47"/>
-      <c r="AF40" s="47"/>
-      <c r="AG40" s="47"/>
-      <c r="AH40" s="47"/>
-      <c r="AI40" s="47"/>
-      <c r="AJ40" s="47"/>
-      <c r="AK40" s="47"/>
-      <c r="AL40" s="46"/>
-      <c r="AM40" s="46"/>
-      <c r="AN40" s="46"/>
-      <c r="AO40" s="46"/>
-      <c r="AP40" s="46"/>
-      <c r="AQ40" s="46"/>
-      <c r="AR40" s="46"/>
-      <c r="AS40" s="46"/>
-      <c r="AT40" s="46"/>
-      <c r="AU40" s="46"/>
-      <c r="AV40" s="46"/>
-      <c r="AW40" s="46"/>
-      <c r="AX40" s="46"/>
-      <c r="AY40" s="46"/>
-      <c r="AZ40" s="46"/>
-      <c r="BA40" s="47"/>
-      <c r="BB40" s="47"/>
-      <c r="BC40" s="47"/>
-      <c r="BD40" s="47"/>
-      <c r="BE40" s="47"/>
-      <c r="BF40" s="47"/>
+      <c r="I40" s="61"/>
+      <c r="J40" s="44"/>
+      <c r="K40" s="45"/>
+      <c r="L40" s="45"/>
+      <c r="M40" s="45"/>
+      <c r="N40" s="45"/>
+      <c r="O40" s="45"/>
+      <c r="P40" s="45"/>
+      <c r="Q40" s="45"/>
+      <c r="R40" s="45"/>
+      <c r="S40" s="45"/>
+      <c r="T40" s="45"/>
+      <c r="U40" s="45"/>
+      <c r="V40" s="45"/>
+      <c r="W40" s="45"/>
+      <c r="X40" s="45"/>
+      <c r="Y40" s="45"/>
+      <c r="Z40" s="45"/>
+      <c r="AA40" s="45"/>
+      <c r="AB40" s="45"/>
+      <c r="AC40" s="46"/>
+      <c r="AD40" s="46"/>
+      <c r="AE40" s="46"/>
+      <c r="AF40" s="46"/>
+      <c r="AG40" s="46"/>
+      <c r="AH40" s="46"/>
+      <c r="AI40" s="46"/>
+      <c r="AJ40" s="46"/>
+      <c r="AK40" s="46"/>
+      <c r="AL40" s="45"/>
+      <c r="AM40" s="45"/>
+      <c r="AN40" s="45"/>
+      <c r="AO40" s="45"/>
+      <c r="AP40" s="45"/>
+      <c r="AQ40" s="45"/>
+      <c r="AR40" s="45"/>
+      <c r="AS40" s="45"/>
+      <c r="AT40" s="45"/>
+      <c r="AU40" s="45"/>
+      <c r="AV40" s="45"/>
+      <c r="AW40" s="45"/>
+      <c r="AX40" s="45"/>
+      <c r="AY40" s="45"/>
+      <c r="AZ40" s="45"/>
+      <c r="BA40" s="46"/>
+      <c r="BB40" s="46"/>
+      <c r="BC40" s="46"/>
+      <c r="BD40" s="46"/>
+      <c r="BE40" s="46"/>
+      <c r="BF40" s="46"/>
       <c r="BG40" s="35"/>
     </row>
     <row r="41" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4355,56 +4355,56 @@
       <c r="H41" s="40">
         <v>0</v>
       </c>
-      <c r="I41" s="62"/>
-      <c r="J41" s="45"/>
-      <c r="K41" s="46"/>
-      <c r="L41" s="46"/>
-      <c r="M41" s="46"/>
-      <c r="N41" s="46"/>
-      <c r="O41" s="46"/>
-      <c r="P41" s="46"/>
-      <c r="Q41" s="46"/>
-      <c r="R41" s="46"/>
-      <c r="S41" s="46"/>
-      <c r="T41" s="46"/>
-      <c r="U41" s="46"/>
-      <c r="V41" s="46"/>
-      <c r="W41" s="46"/>
-      <c r="X41" s="46"/>
-      <c r="Y41" s="46"/>
-      <c r="Z41" s="46"/>
-      <c r="AA41" s="46"/>
-      <c r="AB41" s="46"/>
-      <c r="AC41" s="47"/>
-      <c r="AD41" s="47"/>
-      <c r="AE41" s="47"/>
-      <c r="AF41" s="47"/>
-      <c r="AG41" s="47"/>
-      <c r="AH41" s="47"/>
-      <c r="AI41" s="47"/>
-      <c r="AJ41" s="47"/>
-      <c r="AK41" s="47"/>
-      <c r="AL41" s="46"/>
-      <c r="AM41" s="46"/>
-      <c r="AN41" s="46"/>
-      <c r="AO41" s="46"/>
-      <c r="AP41" s="46"/>
-      <c r="AQ41" s="46"/>
-      <c r="AR41" s="46"/>
-      <c r="AS41" s="46"/>
-      <c r="AT41" s="46"/>
-      <c r="AU41" s="46"/>
-      <c r="AV41" s="46"/>
-      <c r="AW41" s="46"/>
-      <c r="AX41" s="46"/>
-      <c r="AY41" s="46"/>
-      <c r="AZ41" s="46"/>
-      <c r="BA41" s="47"/>
-      <c r="BB41" s="47"/>
-      <c r="BC41" s="47"/>
-      <c r="BD41" s="47"/>
-      <c r="BE41" s="47"/>
-      <c r="BF41" s="47"/>
+      <c r="I41" s="61"/>
+      <c r="J41" s="44"/>
+      <c r="K41" s="45"/>
+      <c r="L41" s="45"/>
+      <c r="M41" s="45"/>
+      <c r="N41" s="45"/>
+      <c r="O41" s="45"/>
+      <c r="P41" s="45"/>
+      <c r="Q41" s="45"/>
+      <c r="R41" s="45"/>
+      <c r="S41" s="45"/>
+      <c r="T41" s="45"/>
+      <c r="U41" s="45"/>
+      <c r="V41" s="45"/>
+      <c r="W41" s="45"/>
+      <c r="X41" s="45"/>
+      <c r="Y41" s="45"/>
+      <c r="Z41" s="45"/>
+      <c r="AA41" s="45"/>
+      <c r="AB41" s="45"/>
+      <c r="AC41" s="46"/>
+      <c r="AD41" s="46"/>
+      <c r="AE41" s="46"/>
+      <c r="AF41" s="46"/>
+      <c r="AG41" s="46"/>
+      <c r="AH41" s="46"/>
+      <c r="AI41" s="46"/>
+      <c r="AJ41" s="46"/>
+      <c r="AK41" s="46"/>
+      <c r="AL41" s="45"/>
+      <c r="AM41" s="45"/>
+      <c r="AN41" s="45"/>
+      <c r="AO41" s="45"/>
+      <c r="AP41" s="45"/>
+      <c r="AQ41" s="45"/>
+      <c r="AR41" s="45"/>
+      <c r="AS41" s="45"/>
+      <c r="AT41" s="45"/>
+      <c r="AU41" s="45"/>
+      <c r="AV41" s="45"/>
+      <c r="AW41" s="45"/>
+      <c r="AX41" s="45"/>
+      <c r="AY41" s="45"/>
+      <c r="AZ41" s="45"/>
+      <c r="BA41" s="46"/>
+      <c r="BB41" s="46"/>
+      <c r="BC41" s="46"/>
+      <c r="BD41" s="46"/>
+      <c r="BE41" s="46"/>
+      <c r="BF41" s="46"/>
       <c r="BG41" s="35"/>
     </row>
     <row r="42" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4424,56 +4424,56 @@
       <c r="H42" s="40">
         <v>0</v>
       </c>
-      <c r="I42" s="62"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="46"/>
-      <c r="L42" s="46"/>
-      <c r="M42" s="46"/>
-      <c r="N42" s="46"/>
-      <c r="O42" s="46"/>
-      <c r="P42" s="46"/>
-      <c r="Q42" s="46"/>
-      <c r="R42" s="46"/>
-      <c r="S42" s="46"/>
-      <c r="T42" s="46"/>
-      <c r="U42" s="46"/>
-      <c r="V42" s="46"/>
-      <c r="W42" s="46"/>
-      <c r="X42" s="46"/>
-      <c r="Y42" s="46"/>
-      <c r="Z42" s="46"/>
-      <c r="AA42" s="46"/>
-      <c r="AB42" s="46"/>
-      <c r="AC42" s="47"/>
-      <c r="AD42" s="47"/>
-      <c r="AE42" s="47"/>
-      <c r="AF42" s="47"/>
-      <c r="AG42" s="47"/>
-      <c r="AH42" s="47"/>
-      <c r="AI42" s="47"/>
-      <c r="AJ42" s="47"/>
-      <c r="AK42" s="47"/>
-      <c r="AL42" s="46"/>
-      <c r="AM42" s="46"/>
-      <c r="AN42" s="46"/>
-      <c r="AO42" s="46"/>
-      <c r="AP42" s="46"/>
-      <c r="AQ42" s="46"/>
-      <c r="AR42" s="46"/>
-      <c r="AS42" s="46"/>
-      <c r="AT42" s="46"/>
-      <c r="AU42" s="46"/>
-      <c r="AV42" s="46"/>
-      <c r="AW42" s="46"/>
-      <c r="AX42" s="46"/>
-      <c r="AY42" s="46"/>
-      <c r="AZ42" s="46"/>
-      <c r="BA42" s="47"/>
-      <c r="BB42" s="47"/>
-      <c r="BC42" s="47"/>
-      <c r="BD42" s="47"/>
-      <c r="BE42" s="47"/>
-      <c r="BF42" s="47"/>
+      <c r="I42" s="61"/>
+      <c r="J42" s="44"/>
+      <c r="K42" s="45"/>
+      <c r="L42" s="45"/>
+      <c r="M42" s="45"/>
+      <c r="N42" s="45"/>
+      <c r="O42" s="45"/>
+      <c r="P42" s="45"/>
+      <c r="Q42" s="45"/>
+      <c r="R42" s="45"/>
+      <c r="S42" s="45"/>
+      <c r="T42" s="45"/>
+      <c r="U42" s="45"/>
+      <c r="V42" s="45"/>
+      <c r="W42" s="45"/>
+      <c r="X42" s="45"/>
+      <c r="Y42" s="45"/>
+      <c r="Z42" s="45"/>
+      <c r="AA42" s="45"/>
+      <c r="AB42" s="45"/>
+      <c r="AC42" s="46"/>
+      <c r="AD42" s="46"/>
+      <c r="AE42" s="46"/>
+      <c r="AF42" s="46"/>
+      <c r="AG42" s="46"/>
+      <c r="AH42" s="46"/>
+      <c r="AI42" s="46"/>
+      <c r="AJ42" s="46"/>
+      <c r="AK42" s="46"/>
+      <c r="AL42" s="45"/>
+      <c r="AM42" s="45"/>
+      <c r="AN42" s="45"/>
+      <c r="AO42" s="45"/>
+      <c r="AP42" s="45"/>
+      <c r="AQ42" s="45"/>
+      <c r="AR42" s="45"/>
+      <c r="AS42" s="45"/>
+      <c r="AT42" s="45"/>
+      <c r="AU42" s="45"/>
+      <c r="AV42" s="45"/>
+      <c r="AW42" s="45"/>
+      <c r="AX42" s="45"/>
+      <c r="AY42" s="45"/>
+      <c r="AZ42" s="45"/>
+      <c r="BA42" s="46"/>
+      <c r="BB42" s="46"/>
+      <c r="BC42" s="46"/>
+      <c r="BD42" s="46"/>
+      <c r="BE42" s="46"/>
+      <c r="BF42" s="46"/>
       <c r="BG42" s="35"/>
     </row>
     <row r="43" spans="1:59" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4544,10 +4544,10 @@
     <row r="44" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A44" s="35"/>
       <c r="B44" s="36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C44" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D44" s="37" t="s">
         <v>47</v>
@@ -4579,41 +4579,41 @@
       <c r="U44" s="41"/>
       <c r="V44" s="41"/>
       <c r="W44" s="41"/>
-      <c r="X44" s="63"/>
-      <c r="Y44" s="63"/>
-      <c r="Z44" s="63"/>
-      <c r="AA44" s="63"/>
-      <c r="AB44" s="63"/>
-      <c r="AC44" s="64"/>
-      <c r="AD44" s="64"/>
-      <c r="AE44" s="64"/>
-      <c r="AF44" s="64"/>
-      <c r="AG44" s="64"/>
-      <c r="AH44" s="64"/>
-      <c r="AI44" s="64"/>
-      <c r="AJ44" s="64"/>
-      <c r="AK44" s="64"/>
-      <c r="AL44" s="63"/>
-      <c r="AM44" s="63"/>
-      <c r="AN44" s="63"/>
-      <c r="AO44" s="63"/>
-      <c r="AP44" s="63"/>
-      <c r="AQ44" s="63"/>
-      <c r="AR44" s="63"/>
-      <c r="AS44" s="63"/>
-      <c r="AT44" s="63"/>
-      <c r="AU44" s="63"/>
-      <c r="AV44" s="63"/>
-      <c r="AW44" s="63"/>
-      <c r="AX44" s="63"/>
-      <c r="AY44" s="63"/>
-      <c r="AZ44" s="63"/>
-      <c r="BA44" s="64"/>
-      <c r="BB44" s="64"/>
-      <c r="BC44" s="64"/>
-      <c r="BD44" s="64"/>
-      <c r="BE44" s="64"/>
-      <c r="BF44" s="64"/>
+      <c r="X44" s="62"/>
+      <c r="Y44" s="62"/>
+      <c r="Z44" s="62"/>
+      <c r="AA44" s="62"/>
+      <c r="AB44" s="62"/>
+      <c r="AC44" s="63"/>
+      <c r="AD44" s="63"/>
+      <c r="AE44" s="63"/>
+      <c r="AF44" s="63"/>
+      <c r="AG44" s="63"/>
+      <c r="AH44" s="63"/>
+      <c r="AI44" s="63"/>
+      <c r="AJ44" s="63"/>
+      <c r="AK44" s="63"/>
+      <c r="AL44" s="62"/>
+      <c r="AM44" s="62"/>
+      <c r="AN44" s="62"/>
+      <c r="AO44" s="62"/>
+      <c r="AP44" s="62"/>
+      <c r="AQ44" s="62"/>
+      <c r="AR44" s="62"/>
+      <c r="AS44" s="62"/>
+      <c r="AT44" s="62"/>
+      <c r="AU44" s="62"/>
+      <c r="AV44" s="62"/>
+      <c r="AW44" s="62"/>
+      <c r="AX44" s="62"/>
+      <c r="AY44" s="62"/>
+      <c r="AZ44" s="62"/>
+      <c r="BA44" s="63"/>
+      <c r="BB44" s="63"/>
+      <c r="BC44" s="63"/>
+      <c r="BD44" s="63"/>
+      <c r="BE44" s="63"/>
+      <c r="BF44" s="63"/>
       <c r="BG44" s="35"/>
     </row>
     <row r="45" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4633,56 +4633,56 @@
       <c r="H45" s="40">
         <v>0</v>
       </c>
-      <c r="I45" s="62"/>
-      <c r="J45" s="45"/>
-      <c r="K45" s="46"/>
-      <c r="L45" s="46"/>
-      <c r="M45" s="46"/>
-      <c r="N45" s="46"/>
-      <c r="O45" s="46"/>
-      <c r="P45" s="46"/>
-      <c r="Q45" s="46"/>
-      <c r="R45" s="46"/>
-      <c r="S45" s="46"/>
-      <c r="T45" s="46"/>
-      <c r="U45" s="46"/>
-      <c r="V45" s="46"/>
-      <c r="W45" s="46"/>
-      <c r="X45" s="46"/>
-      <c r="Y45" s="46"/>
-      <c r="Z45" s="46"/>
-      <c r="AA45" s="46"/>
-      <c r="AB45" s="46"/>
-      <c r="AC45" s="47"/>
-      <c r="AD45" s="47"/>
-      <c r="AE45" s="47"/>
-      <c r="AF45" s="47"/>
-      <c r="AG45" s="47"/>
-      <c r="AH45" s="47"/>
-      <c r="AI45" s="47"/>
-      <c r="AJ45" s="47"/>
-      <c r="AK45" s="47"/>
-      <c r="AL45" s="46"/>
-      <c r="AM45" s="46"/>
-      <c r="AN45" s="46"/>
-      <c r="AO45" s="46"/>
-      <c r="AP45" s="46"/>
-      <c r="AQ45" s="46"/>
-      <c r="AR45" s="46"/>
-      <c r="AS45" s="46"/>
-      <c r="AT45" s="46"/>
-      <c r="AU45" s="46"/>
-      <c r="AV45" s="46"/>
-      <c r="AW45" s="46"/>
-      <c r="AX45" s="46"/>
-      <c r="AY45" s="46"/>
-      <c r="AZ45" s="46"/>
-      <c r="BA45" s="47"/>
-      <c r="BB45" s="47"/>
-      <c r="BC45" s="47"/>
-      <c r="BD45" s="47"/>
-      <c r="BE45" s="47"/>
-      <c r="BF45" s="47"/>
+      <c r="I45" s="61"/>
+      <c r="J45" s="44"/>
+      <c r="K45" s="45"/>
+      <c r="L45" s="45"/>
+      <c r="M45" s="45"/>
+      <c r="N45" s="45"/>
+      <c r="O45" s="45"/>
+      <c r="P45" s="45"/>
+      <c r="Q45" s="45"/>
+      <c r="R45" s="45"/>
+      <c r="S45" s="45"/>
+      <c r="T45" s="45"/>
+      <c r="U45" s="45"/>
+      <c r="V45" s="45"/>
+      <c r="W45" s="45"/>
+      <c r="X45" s="45"/>
+      <c r="Y45" s="45"/>
+      <c r="Z45" s="45"/>
+      <c r="AA45" s="45"/>
+      <c r="AB45" s="45"/>
+      <c r="AC45" s="46"/>
+      <c r="AD45" s="46"/>
+      <c r="AE45" s="46"/>
+      <c r="AF45" s="46"/>
+      <c r="AG45" s="46"/>
+      <c r="AH45" s="46"/>
+      <c r="AI45" s="46"/>
+      <c r="AJ45" s="46"/>
+      <c r="AK45" s="46"/>
+      <c r="AL45" s="45"/>
+      <c r="AM45" s="45"/>
+      <c r="AN45" s="45"/>
+      <c r="AO45" s="45"/>
+      <c r="AP45" s="45"/>
+      <c r="AQ45" s="45"/>
+      <c r="AR45" s="45"/>
+      <c r="AS45" s="45"/>
+      <c r="AT45" s="45"/>
+      <c r="AU45" s="45"/>
+      <c r="AV45" s="45"/>
+      <c r="AW45" s="45"/>
+      <c r="AX45" s="45"/>
+      <c r="AY45" s="45"/>
+      <c r="AZ45" s="45"/>
+      <c r="BA45" s="46"/>
+      <c r="BB45" s="46"/>
+      <c r="BC45" s="46"/>
+      <c r="BD45" s="46"/>
+      <c r="BE45" s="46"/>
+      <c r="BF45" s="46"/>
       <c r="BG45" s="35"/>
     </row>
     <row r="46" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4702,56 +4702,56 @@
       <c r="H46" s="40">
         <v>0</v>
       </c>
-      <c r="I46" s="62"/>
-      <c r="J46" s="45"/>
-      <c r="K46" s="46"/>
-      <c r="L46" s="46"/>
-      <c r="M46" s="46"/>
-      <c r="N46" s="46"/>
-      <c r="O46" s="46"/>
-      <c r="P46" s="46"/>
-      <c r="Q46" s="46"/>
-      <c r="R46" s="46"/>
-      <c r="S46" s="46"/>
-      <c r="T46" s="46"/>
-      <c r="U46" s="46"/>
-      <c r="V46" s="46"/>
-      <c r="W46" s="46"/>
-      <c r="X46" s="46"/>
-      <c r="Y46" s="46"/>
-      <c r="Z46" s="46"/>
-      <c r="AA46" s="46"/>
-      <c r="AB46" s="46"/>
-      <c r="AC46" s="47"/>
-      <c r="AD46" s="47"/>
-      <c r="AE46" s="47"/>
-      <c r="AF46" s="47"/>
-      <c r="AG46" s="47"/>
-      <c r="AH46" s="47"/>
-      <c r="AI46" s="47"/>
-      <c r="AJ46" s="47"/>
-      <c r="AK46" s="47"/>
-      <c r="AL46" s="46"/>
-      <c r="AM46" s="46"/>
-      <c r="AN46" s="46"/>
-      <c r="AO46" s="46"/>
-      <c r="AP46" s="46"/>
-      <c r="AQ46" s="46"/>
-      <c r="AR46" s="46"/>
-      <c r="AS46" s="46"/>
-      <c r="AT46" s="46"/>
-      <c r="AU46" s="46"/>
-      <c r="AV46" s="46"/>
-      <c r="AW46" s="46"/>
-      <c r="AX46" s="46"/>
-      <c r="AY46" s="46"/>
-      <c r="AZ46" s="46"/>
-      <c r="BA46" s="47"/>
-      <c r="BB46" s="47"/>
-      <c r="BC46" s="47"/>
-      <c r="BD46" s="47"/>
-      <c r="BE46" s="47"/>
-      <c r="BF46" s="47"/>
+      <c r="I46" s="61"/>
+      <c r="J46" s="44"/>
+      <c r="K46" s="45"/>
+      <c r="L46" s="45"/>
+      <c r="M46" s="45"/>
+      <c r="N46" s="45"/>
+      <c r="O46" s="45"/>
+      <c r="P46" s="45"/>
+      <c r="Q46" s="45"/>
+      <c r="R46" s="45"/>
+      <c r="S46" s="45"/>
+      <c r="T46" s="45"/>
+      <c r="U46" s="45"/>
+      <c r="V46" s="45"/>
+      <c r="W46" s="45"/>
+      <c r="X46" s="45"/>
+      <c r="Y46" s="45"/>
+      <c r="Z46" s="45"/>
+      <c r="AA46" s="45"/>
+      <c r="AB46" s="45"/>
+      <c r="AC46" s="46"/>
+      <c r="AD46" s="46"/>
+      <c r="AE46" s="46"/>
+      <c r="AF46" s="46"/>
+      <c r="AG46" s="46"/>
+      <c r="AH46" s="46"/>
+      <c r="AI46" s="46"/>
+      <c r="AJ46" s="46"/>
+      <c r="AK46" s="46"/>
+      <c r="AL46" s="45"/>
+      <c r="AM46" s="45"/>
+      <c r="AN46" s="45"/>
+      <c r="AO46" s="45"/>
+      <c r="AP46" s="45"/>
+      <c r="AQ46" s="45"/>
+      <c r="AR46" s="45"/>
+      <c r="AS46" s="45"/>
+      <c r="AT46" s="45"/>
+      <c r="AU46" s="45"/>
+      <c r="AV46" s="45"/>
+      <c r="AW46" s="45"/>
+      <c r="AX46" s="45"/>
+      <c r="AY46" s="45"/>
+      <c r="AZ46" s="45"/>
+      <c r="BA46" s="46"/>
+      <c r="BB46" s="46"/>
+      <c r="BC46" s="46"/>
+      <c r="BD46" s="46"/>
+      <c r="BE46" s="46"/>
+      <c r="BF46" s="46"/>
       <c r="BG46" s="35"/>
     </row>
     <row r="47" spans="1:59" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4768,59 +4768,59 @@
       <c r="G47" s="39">
         <v>0</v>
       </c>
-      <c r="H47" s="49">
+      <c r="H47" s="48">
         <v>0</v>
       </c>
-      <c r="I47" s="62"/>
-      <c r="J47" s="45"/>
-      <c r="K47" s="46"/>
-      <c r="L47" s="46"/>
-      <c r="M47" s="46"/>
-      <c r="N47" s="46"/>
-      <c r="O47" s="46"/>
-      <c r="P47" s="46"/>
-      <c r="Q47" s="46"/>
-      <c r="R47" s="46"/>
-      <c r="S47" s="46"/>
-      <c r="T47" s="46"/>
-      <c r="U47" s="46"/>
-      <c r="V47" s="46"/>
-      <c r="W47" s="46"/>
-      <c r="X47" s="46"/>
-      <c r="Y47" s="46"/>
-      <c r="Z47" s="46"/>
-      <c r="AA47" s="46"/>
-      <c r="AB47" s="46"/>
-      <c r="AC47" s="47"/>
-      <c r="AD47" s="47"/>
-      <c r="AE47" s="47"/>
-      <c r="AF47" s="47"/>
-      <c r="AG47" s="47"/>
-      <c r="AH47" s="47"/>
-      <c r="AI47" s="47"/>
-      <c r="AJ47" s="47"/>
-      <c r="AK47" s="47"/>
-      <c r="AL47" s="46"/>
-      <c r="AM47" s="46"/>
-      <c r="AN47" s="46"/>
-      <c r="AO47" s="46"/>
-      <c r="AP47" s="46"/>
-      <c r="AQ47" s="46"/>
-      <c r="AR47" s="46"/>
-      <c r="AS47" s="46"/>
-      <c r="AT47" s="46"/>
-      <c r="AU47" s="46"/>
-      <c r="AV47" s="46"/>
-      <c r="AW47" s="46"/>
-      <c r="AX47" s="46"/>
-      <c r="AY47" s="46"/>
-      <c r="AZ47" s="46"/>
-      <c r="BA47" s="47"/>
-      <c r="BB47" s="47"/>
-      <c r="BC47" s="47"/>
-      <c r="BD47" s="47"/>
-      <c r="BE47" s="47"/>
-      <c r="BF47" s="47"/>
+      <c r="I47" s="61"/>
+      <c r="J47" s="44"/>
+      <c r="K47" s="45"/>
+      <c r="L47" s="45"/>
+      <c r="M47" s="45"/>
+      <c r="N47" s="45"/>
+      <c r="O47" s="45"/>
+      <c r="P47" s="45"/>
+      <c r="Q47" s="45"/>
+      <c r="R47" s="45"/>
+      <c r="S47" s="45"/>
+      <c r="T47" s="45"/>
+      <c r="U47" s="45"/>
+      <c r="V47" s="45"/>
+      <c r="W47" s="45"/>
+      <c r="X47" s="45"/>
+      <c r="Y47" s="45"/>
+      <c r="Z47" s="45"/>
+      <c r="AA47" s="45"/>
+      <c r="AB47" s="45"/>
+      <c r="AC47" s="46"/>
+      <c r="AD47" s="46"/>
+      <c r="AE47" s="46"/>
+      <c r="AF47" s="46"/>
+      <c r="AG47" s="46"/>
+      <c r="AH47" s="46"/>
+      <c r="AI47" s="46"/>
+      <c r="AJ47" s="46"/>
+      <c r="AK47" s="46"/>
+      <c r="AL47" s="45"/>
+      <c r="AM47" s="45"/>
+      <c r="AN47" s="45"/>
+      <c r="AO47" s="45"/>
+      <c r="AP47" s="45"/>
+      <c r="AQ47" s="45"/>
+      <c r="AR47" s="45"/>
+      <c r="AS47" s="45"/>
+      <c r="AT47" s="45"/>
+      <c r="AU47" s="45"/>
+      <c r="AV47" s="45"/>
+      <c r="AW47" s="45"/>
+      <c r="AX47" s="45"/>
+      <c r="AY47" s="45"/>
+      <c r="AZ47" s="45"/>
+      <c r="BA47" s="46"/>
+      <c r="BB47" s="46"/>
+      <c r="BC47" s="46"/>
+      <c r="BD47" s="46"/>
+      <c r="BE47" s="46"/>
+      <c r="BF47" s="46"/>
       <c r="BG47" s="35"/>
     </row>
     <row r="48" spans="1:59" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4828,10 +4828,10 @@
       <c r="B48" s="14"/>
       <c r="C48" s="14"/>
       <c r="D48" s="14"/>
-      <c r="E48" s="65"/>
-      <c r="F48" s="65"/>
-      <c r="G48" s="66"/>
-      <c r="H48" s="66"/>
+      <c r="E48" s="64"/>
+      <c r="F48" s="64"/>
+      <c r="G48" s="65"/>
+      <c r="H48" s="65"/>
       <c r="I48" s="14"/>
       <c r="J48" s="14"/>
       <c r="K48" s="14"/>
@@ -4889,10 +4889,10 @@
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
       <c r="D49" s="14"/>
-      <c r="E49" s="65"/>
-      <c r="F49" s="65"/>
-      <c r="G49" s="66"/>
-      <c r="H49" s="66"/>
+      <c r="E49" s="64"/>
+      <c r="F49" s="64"/>
+      <c r="G49" s="65"/>
+      <c r="H49" s="65"/>
       <c r="I49" s="14"/>
       <c r="J49" s="14"/>
       <c r="K49" s="14"/>
@@ -4950,10 +4950,10 @@
       <c r="B50" s="14"/>
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
-      <c r="E50" s="65"/>
-      <c r="F50" s="65"/>
-      <c r="G50" s="66"/>
-      <c r="H50" s="66"/>
+      <c r="E50" s="64"/>
+      <c r="F50" s="64"/>
+      <c r="G50" s="65"/>
+      <c r="H50" s="65"/>
       <c r="I50" s="14"/>
       <c r="J50" s="14"/>
       <c r="K50" s="14"/>
@@ -5008,6 +5008,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="I5:O5"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="H8:H11"/>
+    <mergeCell ref="X8:AK8"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="F8:F11"/>
+    <mergeCell ref="G8:G11"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="B1:AE2"/>
@@ -5024,15 +5033,6 @@
     <mergeCell ref="D5:G5"/>
     <mergeCell ref="P5:AA5"/>
     <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="H8:H11"/>
-    <mergeCell ref="X8:AK8"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="F8:F11"/>
-    <mergeCell ref="G8:G11"/>
-    <mergeCell ref="I5:O5"/>
   </mergeCells>
   <conditionalFormatting sqref="H32:H47 H13:H30">
     <cfRule type="colorScale" priority="1">

</xml_diff>